<commit_message>
[FIX]: se corrigio funcionalidades del mapa
</commit_message>
<xml_diff>
--- a/data/scraped/trabajos.xlsx
+++ b/data/scraped/trabajos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,120 +410,141 @@
         <v>empresa</v>
       </c>
       <c r="C1" t="str">
+        <v>ubicacion</v>
+      </c>
+      <c r="D1" t="str">
         <v>salario</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>descripcion</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>url</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>403 Forbidden</v>
+        <v>Desarrollador/a FullStack</v>
       </c>
       <c r="B2" t="str">
-        <v>No disponible</v>
+        <v>Holcim Apasco</v>
       </c>
       <c r="C2" t="str">
-        <v>No especificado</v>
+        <v>San Pedro Tlaquepaque, Jalisco</v>
       </c>
       <c r="D2" t="str">
-        <v>No disponible</v>
+        <v>$ 20,000.00</v>
       </c>
       <c r="E2" t="str">
+        <v>¿QUIÉN ES HOLCIM?Somos el líder mundial en soluciones innovadoras y sostenibles para la construcción mediante cuatro segmentos de negocio: cemento, concreto/hormigón premezclado, agregados, soluciones y productos.Nuestro objetivo es impulsar la construcción circular para construir más con menos. Gracias a nuestro enfoque en la reducción de emisiones de CO2, cuidado al medio ambiente, apoyo a las comunidades y desarrollo de nuestra gente, hemos logrado que nuestros 70.000 colaboradores y colaboradoras en todo el mundo sienten una gran pasión por construir progreso para las personas y el planeta, creando mejores soluciones y experiencias para sus clientes, comunidades y equipos.¡TRABAJA CON NOSOTROS!Tendrás la oportunidad de compartir la pasión que tenemos por nuestro planeta, aportar perspectivas innovadoras, dentro de un entorno dinámico y retador, que promueve la diversidad e inclusión.Porque solo si trabajamos juntos en una cultura en la que todos prosperamos, podremos construir el mundo en el que todos queremos vivir.TE ESTAMOS BUSCANDO: Desarrollador/a FullStack!Serás responsable de diseñar, desarrollar y mantener aplicaciones web completas (frontend y backend), asegurando interfaces atractivas, usabilidad, seguridad y alto rendimiento.Tus principales retos serán:Crear interfaces de usuario modernas, responsivas y funcionales.Desarrollar APIs robustas e integraciones con servicios externos.Implementar y administrar bases de datos relacionales y no relacionales.Asegurar la autenticación y seguridad de las aplicaciones.Integrar plataformas de pago y otros servicios de terceros.Colaborar con equipos multidisciplinarios en entornos ágiles.Lugar de trabajo: Carretera a Tlaquepaque Jalisco, San Martin de las flores.Requisitos indispensables:Licenciatura o ingeniería en sistemas, desarrollo de software o afín.Experiencia comprobable en desarrollo Full Stack.Dominio de HTML, CSS, JavaScript y frameworks como React, Angular o VuejsConocimientos en backend con Nodejs, Python o Java.Manejo de bases de datos relacionales (SQL Server, PostgreSQL) y no relacionales (MongoDB, Firebase).Experiencia con integración de APIs REST y GraphQL.Uso de servicios en la nube (AWS, GCP) y control de versiones con Git/GitHub.Inglés B2.Requisitos deseados:Experiencia en entornos de retail, e commerce o mayoristas (B2B/B2C).Familiaridad con plataformas de pago.Conocimientos en backend con Nodejs, Python o Java.¡NO TE PIERDAS LA OPORTUNIDAD DE SER PARTE DE NUESTRO EQUIPO!¡CONSTRUYE PROGRESO CON NOSOTROS!</v>
+      </c>
+      <c r="F2" t="str">
         <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrolladora-fullstack-en-san-pedro-tlaquepaque-7B5D20BFE204246961373E686DCF3405#lc=ListOffers-Score3-0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>403 Forbidden</v>
+        <v>Programador/a - Temporal</v>
       </c>
       <c r="B3" t="str">
-        <v>No disponible</v>
+        <v>Caja Morelia Valladolid</v>
       </c>
       <c r="C3" t="str">
-        <v>No especificado</v>
+        <v>Morelia, Michoacán</v>
       </c>
       <c r="D3" t="str">
-        <v>No disponible</v>
+        <v>$ 7,209</v>
       </c>
       <c r="E3" t="str">
+        <v>Empresa Mexicana dedicada al servicio Financiero con 59 años de historia y presencia nacional, Caja Morelia Valladolid solicita personal.PROGRAMADOR TEMPORALOFECEMOS:-Sueldo base.-Prestaciones superiores a las de Ley.-Vales de despensa 8% del sueldo bruto mensual.-Fondo de ahorro del 13% del sueldo bruto mensual.-Seguro de vida.-Prima vacacional 100%.-30 días de aguinaldo desde el primer año.-Uniformes.-Opciones a becas.- Y mucho más...REQUISITOS:•Licenciatura o ingeniería Titulado en Informática, Sistemas Computacionales, TIC’s a fines.•Dominio de bases de datos SQL SERVER•Dominio de .NET C# o JAVA•Dominio Programación web (Html5, Maquetado CSS, Javascript, ECMAScript 2015+, VueJS2)•Dominio API Rest y SOAP (Net Core, nodeJS)•Dominio Programación móvil (Android, IOS, híbrido o nativo)•Manejo de Control de Versiones GIT.•Manejo de Plataforma JIRA &amp; Confluence•Deseable Delphi 6Horario de trabajo: Lunes a Viernes de 8:30 am a 5 pm y Sábados de 8:30 am a 2 pmInteresados postularse por este medio</v>
+      </c>
+      <c r="F3" t="str">
         <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-programadora-temporal-en-morelia-DA3519AF994F093961373E686DCF3405#lc=ListOffers-Score0-1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>403 Forbidden</v>
+        <v>Work From Home Shopify Engineer / Ref. 0176</v>
       </c>
       <c r="B4" t="str">
-        <v>No disponible</v>
+        <v>BairesDev LLC</v>
       </c>
       <c r="C4" t="str">
-        <v>No especificado</v>
+        <v>Aguascalientes, Aguascalientes</v>
       </c>
       <c r="D4" t="str">
-        <v>No disponible</v>
+        <v>$ 3,700</v>
       </c>
       <c r="E4" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Shopify Engineer at BairesDevWe are looking for a Shopify Engineer to join our Development team and help the client take its eCommerce platform to the next level. The Shopify Engineer will be responsible for designing, developing, and maintaining the clients Shopify website and integrations with other systems. This is an excellent opportunity for those professionals looking to develop in one of the fastest-growing companies in the industry!What You Will Do:- Collaborate with the eCommerce team to understand business requirements and translate them into technical solutions.- Design and implement custom Shopify themes and templates.- Build and maintain custom Shopify apps and plugins.- Integrate Shopify with other systems such as CRM, ERP, and payment gateways.- Ensure website performance and security are optimized.- Troubleshoot and resolve website issues.Heres what we are looking for:- 3+ years of experience with Shopify Liquid.- 2+ years of experience with a JS Framework (React, NextJS, VueJS, etc).- Proven track record in Shopify App development.- Shopify headless architecture experience (stores/apps) is desirable, but not mandatory.- Upper English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F4" t="str">
         <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-shopify-engineer-ref-0176-en-aguascalientes-2F8573081BEEE1A961373E686DCF3405#lc=ListOffers-Score0-2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>403 Forbidden</v>
+        <v>Trabajo Desde Casa Ingeniero Vue.js / Ref. 0255</v>
       </c>
       <c r="B5" t="str">
-        <v>No disponible</v>
+        <v>BairesDev LLC</v>
       </c>
       <c r="C5" t="str">
-        <v>No especificado</v>
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
       </c>
       <c r="D5" t="str">
-        <v>No disponible</v>
+        <v>$ 3,700</v>
       </c>
       <c r="E5" t="str">
+        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Ingeniero Vue.js en BairesDevBuscamos Ingenieros de Vue.js para unirse a nuestro equipo de Desarrollo y participar en diferentes proyectos conformados por equipos multiculturales distribuidos por todo el mundo. Buscamos personas proactivas, jugadores de equipo apasionados por la programación en este lenguaje y orientados a brindar la mejor experiencia al usuario final.Principales responsabilidades:- Desarrollar aplicaciones de interfaz utilizando Vue.js y el ecosistema circundante.- Traducir con precisión las necesidades de los usuarios y las empresas en un código de interfaz funcional.- Desarrollar y probar IU para escritorio y sitios web receptivos.- Implementar pruebas automatizadas integradas en los flujos de trabajo de desarrollo y mantenimiento.- Crear códigos y bibliotecas reutilizables para uso futuro.- Estar actualizado con todos los desarrollos recientes en el espacio JavaScript y Vue.js.- Estar centrado en las actualizaciones de seguridad y los problemas encontrados con Vue.js y todas las dependencias del proyecto.- Realizar actualizaciones y mejoras necesarias para mantenerse al día con las mejores prácticas modernas de seguridad y desarrollo.- Contribuir con ideas e innovaciones, siempre que vea una oportunidad de mejora.- Trabajar en colaboración con nuestros equipos multidisciplinares.¿Qué Buscamos?:- 5+ años de experiencia en desarrollo de software.- 3+ años de experiencia con el desarrollo de Vue.Js.- Fuertes habilidades con el lenguaje JavaScript y frameworks (React, Angular, Ember, etc.).- Experta o avanzada experiencia en tecnologías front-end, arquitecturas de seguridad y experiencia de usuario.- Avanzado en el desarrollo y prueba de aplicaciones web basadas en web, basadas en web móvil y totalmente receptivas utilizando marcos de JavaScript como Jest, Mocha, Chai, Jasmine, etc.- Experiencia en integraciones de servicios (servicios web, sistemas CMS / Commerce, API de terceros, etc.).- Experiencia tanto en el consumo como en el diseño de API RESTful.- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) seja mais fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
+      </c>
+      <c r="F5" t="str">
         <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-ingeniero-vuejs-ref-0255-en-miguel-hidalgo-410F255D92AE8E8661373E686DCF3405#lc=ListOffers-Score0-3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>403 Forbidden</v>
+        <v>Trabajo Desde Casa Desarrollador de Vue.js / Ref. 0255</v>
       </c>
       <c r="B6" t="str">
-        <v>No disponible</v>
+        <v>BairesDev LLC</v>
       </c>
       <c r="C6" t="str">
-        <v>No especificado</v>
+        <v>Benito Juárez, Quintana Roo</v>
       </c>
       <c r="D6" t="str">
-        <v>No disponible</v>
+        <v>$ 3,700</v>
       </c>
       <c r="E6" t="str">
+        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Desarrollador de Vue.js en BairesDevBuscamos Desarrollador de Vue.js para unirse a nuestro equipo de Desarrollo y participar en diferentes proyectos conformados por equipos multiculturales distribuidos por todo el mundo. Buscamos personas proactivas, jugadores de equipo apasionados por la programación en este lenguaje y orientados a brindar la mejor experiencia al usuario final.Actividades principales:- Desarrollar aplicaciones de interfaz utilizando Vue.js y el ecosistema circundante.- Traducir con precisión las necesidades de los usuarios y las empresas en un código de interfaz funcional.- Desarrollar y probar IU para escritorio y sitios web receptivos.- Implementar pruebas automatizadas integradas en los flujos de trabajo de desarrollo y mantenimiento.- Crear códigos y bibliotecas reutilizables para uso futuro.- Estar actualizado con todos los desarrollos recientes en el espacio JavaScript y Vue.js.- Estar centrado en las actualizaciones de seguridad y los problemas encontrados con Vue.js y todas las dependencias del proyecto.- Realizar actualizaciones y mejoras necesarias para mantenerse al día con las mejores prácticas modernas de seguridad y desarrollo.- Contribuir con ideas e innovaciones, siempre que vea una oportunidad de mejora.- Trabajar en colaboración con nuestros equipos multidisciplinares.¿Qué Buscamos?:- 5+ años de experiencia en desarrollo de software.- 3+ años de experiencia con el desarrollo de Vue.Js.- Fuertes habilidades con el lenguaje JavaScript y frameworks (React, Angular, Ember, etc.).- Experta o avanzada experiencia en tecnologías front-end, arquitecturas de seguridad y experiencia de usuario.- Avanzado en el desarrollo y prueba de aplicaciones web basadas en web, basadas en web móvil y totalmente receptivas utilizando marcos de JavaScript como Jest, Mocha, Chai, Jasmine, etc.- Experiencia en integraciones de servicios (servicios web, sistemas CMS / Commerce, API de terceros, etc.).- Experiencia tanto en el consumo como en el diseño de API RESTful.- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) seja mais fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
+      </c>
+      <c r="F6" t="str">
         <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-desarrollador-de-vuejs-ref-0255-en-benito-juarez-7A14BBB695EF0B0C61373E686DCF3405#lc=ListOffers-Score0-4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>403 Forbidden</v>
+        <v>Programador/a - Temporal</v>
       </c>
       <c r="B7" t="str">
-        <v>No disponible</v>
+        <v>Caja Morelia Valladolid</v>
       </c>
       <c r="C7" t="str">
-        <v>No especificado</v>
+        <v>Morelia, Michoacán</v>
       </c>
       <c r="D7" t="str">
-        <v>No disponible</v>
+        <v>$ 7,209</v>
       </c>
       <c r="E7" t="str">
+        <v>Empresa Mexicana dedicada al servicio Financiero con 59 años de historia y presencia nacional, Caja Morelia Valladolid solicita personal.PROGRAMADOR TEMPORALOFECEMOS:-Sueldo base.-Prestaciones superiores a las de Ley.-Vales de despensa 8% del sueldo bruto mensual.-Fondo de ahorro del 13% del sueldo bruto mensual.-Seguro de vida.-Prima vacacional 100%.-30 días de aguinaldo desde el primer año.-Uniformes.-Opciones a becas.- Y mucho más...REQUISITOS:•Licenciatura o ingeniería Titulado en Informática, Sistemas Computacionales, TIC’s a fines.•Dominio de bases de datos SQL SERVER•Dominio de .NET C# o JAVA•Dominio Programación web (Html5, Maquetado CSS, Javascript, ECMAScript 2015+, VueJS2)•Dominio API Rest y SOAP (Net Core, nodeJS)•Dominio Programación móvil (Android, IOS, híbrido o nativo)•Manejo de Control de Versiones GIT.•Manejo de Plataforma JIRA &amp; Confluence•Deseable Delphi 6Horario de trabajo: Lunes a Viernes de 8:30 am a 5 pm y Sábados de 8:30 am a 2 pmInteresados postularse por este medio</v>
+      </c>
+      <c r="F7" t="str">
         <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-programadora-temporal-en-morelia-4B58ECD317F4993161373E686DCF3405#lc=ListOffers-Score0-5</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[UPDATE] modificacion en datos de empleo dentro del mapa
</commit_message>
<xml_diff>
--- a/data/scraped/trabajos.xlsx
+++ b/data/scraped/trabajos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,127 +424,327 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Desarrollador/a FullStack</v>
+        <v>Barrendero/A - Turno Nocturno o Vespertino</v>
       </c>
       <c r="B2" t="str">
-        <v>Holcim Apasco</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C2" t="str">
-        <v>San Pedro Tlaquepaque, Jalisco</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D2" t="str">
-        <v>$ 20,000.00</v>
+        <v>$ 5,437</v>
       </c>
       <c r="E2" t="str">
-        <v>¿QUIÉN ES HOLCIM?Somos el líder mundial en soluciones innovadoras y sostenibles para la construcción mediante cuatro segmentos de negocio: cemento, concreto/hormigón premezclado, agregados, soluciones y productos.Nuestro objetivo es impulsar la construcción circular para construir más con menos. Gracias a nuestro enfoque en la reducción de emisiones de CO2, cuidado al medio ambiente, apoyo a las comunidades y desarrollo de nuestra gente, hemos logrado que nuestros 70.000 colaboradores y colaboradoras en todo el mundo sienten una gran pasión por construir progreso para las personas y el planeta, creando mejores soluciones y experiencias para sus clientes, comunidades y equipos.¡TRABAJA CON NOSOTROS!Tendrás la oportunidad de compartir la pasión que tenemos por nuestro planeta, aportar perspectivas innovadoras, dentro de un entorno dinámico y retador, que promueve la diversidad e inclusión.Porque solo si trabajamos juntos en una cultura en la que todos prosperamos, podremos construir el mundo en el que todos queremos vivir.TE ESTAMOS BUSCANDO: Desarrollador/a FullStack!Serás responsable de diseñar, desarrollar y mantener aplicaciones web completas (frontend y backend), asegurando interfaces atractivas, usabilidad, seguridad y alto rendimiento.Tus principales retos serán:Crear interfaces de usuario modernas, responsivas y funcionales.Desarrollar APIs robustas e integraciones con servicios externos.Implementar y administrar bases de datos relacionales y no relacionales.Asegurar la autenticación y seguridad de las aplicaciones.Integrar plataformas de pago y otros servicios de terceros.Colaborar con equipos multidisciplinarios en entornos ágiles.Lugar de trabajo: Carretera a Tlaquepaque Jalisco, San Martin de las flores.Requisitos indispensables:Licenciatura o ingeniería en sistemas, desarrollo de software o afín.Experiencia comprobable en desarrollo Full Stack.Dominio de HTML, CSS, JavaScript y frameworks como React, Angular o VuejsConocimientos en backend con Nodejs, Python o Java.Manejo de bases de datos relacionales (SQL Server, PostgreSQL) y no relacionales (MongoDB, Firebase).Experiencia con integración de APIs REST y GraphQL.Uso de servicios en la nube (AWS, GCP) y control de versiones con Git/GitHub.Inglés B2.Requisitos deseados:Experiencia en entornos de retail, e commerce o mayoristas (B2B/B2C).Familiaridad con plataformas de pago.Conocimientos en backend con Nodejs, Python o Java.¡NO TE PIERDAS LA OPORTUNIDAD DE SER PARTE DE NUESTRO EQUIPO!¡CONSTRUYE PROGRESO CON NOSOTROS!</v>
+        <v>Buscamos tu talento como Barrendero/a para turno Nocturno o Vespertino:Zona de trabajo: Central de abastos IztapalapaBarrenderos Nocturno (Horario 5 pm a 5 am)Barrenderos Vespertino (Horario de 10 am a 7:00 pm)Lunes a domingo descanso entre semana*Contratacion inmediata*Contar con documentacion (Acta de nacimiento, Comprobante de clabe interbancaria es decir cuenta de banco, nss, curp, ine, constancia de situacion fiscal y comprobante de domicilo)Agenda hoy mismo comunicate al 5 5 796 9 59 09</v>
       </c>
       <c r="F2" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrolladora-fullstack-en-san-pedro-tlaquepaque-7B5D20BFE204246961373E686DCF3405#lc=ListOffers-Score3-0</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderoa-turno-nocturno-o-vespertino-en-iztapalapa-8EFACEA56D1028F261373E686DCF3405#lc=ListOffers-Score4-0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Programador/a - Temporal</v>
+        <v>Barrendero Central de Abastos - Iztapalapa</v>
       </c>
       <c r="B3" t="str">
-        <v>Caja Morelia Valladolid</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C3" t="str">
-        <v>Morelia, Michoacán</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D3" t="str">
-        <v>$ 7,209</v>
+        <v>$ 10,000.00</v>
       </c>
       <c r="E3" t="str">
-        <v>Empresa Mexicana dedicada al servicio Financiero con 59 años de historia y presencia nacional, Caja Morelia Valladolid solicita personal.PROGRAMADOR TEMPORALOFECEMOS:-Sueldo base.-Prestaciones superiores a las de Ley.-Vales de despensa 8% del sueldo bruto mensual.-Fondo de ahorro del 13% del sueldo bruto mensual.-Seguro de vida.-Prima vacacional 100%.-30 días de aguinaldo desde el primer año.-Uniformes.-Opciones a becas.- Y mucho más...REQUISITOS:•Licenciatura o ingeniería Titulado en Informática, Sistemas Computacionales, TIC’s a fines.•Dominio de bases de datos SQL SERVER•Dominio de .NET C# o JAVA•Dominio Programación web (Html5, Maquetado CSS, Javascript, ECMAScript 2015+, VueJS2)•Dominio API Rest y SOAP (Net Core, nodeJS)•Dominio Programación móvil (Android, IOS, híbrido o nativo)•Manejo de Control de Versiones GIT.•Manejo de Plataforma JIRA &amp; Confluence•Deseable Delphi 6Horario de trabajo: Lunes a Viernes de 8:30 am a 5 pm y Sábados de 8:30 am a 2 pmInteresados postularse por este medio</v>
+        <v>Importante mercado está en busca de tu talentoSOLICITA BARRENDERO MATUTINO O NOCTURNOOFRECEMOS:Sueldo de $8,0000 a $10,000 neto mensualUniforme gratuitoPrestaciones de leyREQUISITOS:Experiencia no necesariaPrimaria concluidaDocumentos completos en copiaLunes a Domingo de 5pm a 5am o 10am a 7pm, 1 descanso rolado a la semanaZona de trabajo: Central de abastos Iztapalapa, CDMX5511 4122 82Si estas interesada/o postúlate con tu CV actualizado</v>
       </c>
       <c r="F3" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-programadora-temporal-en-morelia-DA3519AF994F093961373E686DCF3405#lc=ListOffers-Score0-1</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-central-de-abastos-iztapalapa-en-iztapalapa-D4CB1C1EE38BEE9A61373E686DCF3405#lc=ListOffers-Score4-1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Work From Home Shopify Engineer / Ref. 0176</v>
+        <v>Barrendero con o sin experiencia / Nocturno y Vespertino - Zona Central de abastos Iztapalapa</v>
       </c>
       <c r="B4" t="str">
-        <v>BairesDev LLC</v>
+        <v>Importante empresa del sector</v>
       </c>
       <c r="C4" t="str">
-        <v>Aguascalientes, Aguascalientes</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D4" t="str">
-        <v>$ 3,700</v>
+        <v>$9,000</v>
       </c>
       <c r="E4" t="str">
-        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Shopify Engineer at BairesDevWe are looking for a Shopify Engineer to join our Development team and help the client take its eCommerce platform to the next level. The Shopify Engineer will be responsible for designing, developing, and maintaining the clients Shopify website and integrations with other systems. This is an excellent opportunity for those professionals looking to develop in one of the fastest-growing companies in the industry!What You Will Do:- Collaborate with the eCommerce team to understand business requirements and translate them into technical solutions.- Design and implement custom Shopify themes and templates.- Build and maintain custom Shopify apps and plugins.- Integrate Shopify with other systems such as CRM, ERP, and payment gateways.- Ensure website performance and security are optimized.- Troubleshoot and resolve website issues.Heres what we are looking for:- 3+ years of experience with Shopify Liquid.- 2+ years of experience with a JS Framework (React, NextJS, VueJS, etc).- Proven track record in Shopify App development.- Shopify headless architecture experience (stores/apps) is desirable, but not mandatory.- Upper English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+        <v>Se busca barrendero para turnos nocturnos y vespertinos.Buscamos a una persona responsable, con experiencia en limpieza y mantenimiento de espacios comunes.El trabajo requiere desplazamientos cortos y uso de herramientas básicas de limpieza.Se valorará experiencia previa en limpieza, aunque no es imprescindible.Se ofrece contrato temporal con posibilidad de renovación.Se requiere disponibilidad para trabajar en horarios nocturnos y vespertinos.Se busca un perfil con actitud positiva y compromiso con el trabajo bien hecho.Se requiere puntualidad y capacidad para trabajar en equipo.Se ofrece ambiente de trabajo agradable y posibilidad de formación continua.Si tienes interés en mantener espacios limpios y cuidando los detalles, esta oportunidad puede ser para ti.Envía tu currículum con tus datos y experiencia previa en limpieza.Buscas un trabajo estable y con oportunidades de crecimiento profesional.Únete a nuestro equipo y contribuye a mantener nuestros entornos limpios y ordenados.</v>
       </c>
       <c r="F4" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-shopify-engineer-ref-0176-en-aguascalientes-2F8573081BEEE1A961373E686DCF3405#lc=ListOffers-Score0-2</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-con-o-sin-experiencia-nocturno-y-vespertino-zona-central-de-abastos-iztapalapa-en-iztapalapa-9BB6F3E7844AC9D961373E686DCF3405#lc=ListOffers-Score4-2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Trabajo Desde Casa Ingeniero Vue.js / Ref. 0255</v>
+        <v>EG Barrendero Vespertino Central de Abastos</v>
       </c>
       <c r="B5" t="str">
-        <v>BairesDev LLC</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C5" t="str">
-        <v>Miguel Hidalgo, Ciudad de México DF</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D5" t="str">
-        <v>$ 3,700</v>
+        <v>$ 8,000.00</v>
       </c>
       <c r="E5" t="str">
-        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Ingeniero Vue.js en BairesDevBuscamos Ingenieros de Vue.js para unirse a nuestro equipo de Desarrollo y participar en diferentes proyectos conformados por equipos multiculturales distribuidos por todo el mundo. Buscamos personas proactivas, jugadores de equipo apasionados por la programación en este lenguaje y orientados a brindar la mejor experiencia al usuario final.Principales responsabilidades:- Desarrollar aplicaciones de interfaz utilizando Vue.js y el ecosistema circundante.- Traducir con precisión las necesidades de los usuarios y las empresas en un código de interfaz funcional.- Desarrollar y probar IU para escritorio y sitios web receptivos.- Implementar pruebas automatizadas integradas en los flujos de trabajo de desarrollo y mantenimiento.- Crear códigos y bibliotecas reutilizables para uso futuro.- Estar actualizado con todos los desarrollos recientes en el espacio JavaScript y Vue.js.- Estar centrado en las actualizaciones de seguridad y los problemas encontrados con Vue.js y todas las dependencias del proyecto.- Realizar actualizaciones y mejoras necesarias para mantenerse al día con las mejores prácticas modernas de seguridad y desarrollo.- Contribuir con ideas e innovaciones, siempre que vea una oportunidad de mejora.- Trabajar en colaboración con nuestros equipos multidisciplinares.¿Qué Buscamos?:- 5+ años de experiencia en desarrollo de software.- 3+ años de experiencia con el desarrollo de Vue.Js.- Fuertes habilidades con el lenguaje JavaScript y frameworks (React, Angular, Ember, etc.).- Experta o avanzada experiencia en tecnologías front-end, arquitecturas de seguridad y experiencia de usuario.- Avanzado en el desarrollo y prueba de aplicaciones web basadas en web, basadas en web móvil y totalmente receptivas utilizando marcos de JavaScript como Jest, Mocha, Chai, Jasmine, etc.- Experiencia en integraciones de servicios (servicios web, sistemas CMS / Commerce, API de terceros, etc.).- Experiencia tanto en el consumo como en el diseño de API RESTful.- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) seja mais fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO VESPERTINOOFRECEMOS:• Sueldo de hasta $8,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
       </c>
       <c r="F5" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-ingeniero-vuejs-ref-0255-en-miguel-hidalgo-410F255D92AE8E8661373E686DCF3405#lc=ListOffers-Score0-3</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-vespertino-central-de-abastos-en-iztapalapa-B6999002976CCE4B61373E686DCF3405#lc=ListOffers-Score4-3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Trabajo Desde Casa Desarrollador de Vue.js / Ref. 0255</v>
+        <v>EG Barrendero Nocturno Central de Abastos</v>
       </c>
       <c r="B6" t="str">
-        <v>BairesDev LLC</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C6" t="str">
-        <v>Benito Juárez, Quintana Roo</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D6" t="str">
-        <v>$ 3,700</v>
+        <v>$ 10,000.00</v>
       </c>
       <c r="E6" t="str">
-        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Desarrollador de Vue.js en BairesDevBuscamos Desarrollador de Vue.js para unirse a nuestro equipo de Desarrollo y participar en diferentes proyectos conformados por equipos multiculturales distribuidos por todo el mundo. Buscamos personas proactivas, jugadores de equipo apasionados por la programación en este lenguaje y orientados a brindar la mejor experiencia al usuario final.Actividades principales:- Desarrollar aplicaciones de interfaz utilizando Vue.js y el ecosistema circundante.- Traducir con precisión las necesidades de los usuarios y las empresas en un código de interfaz funcional.- Desarrollar y probar IU para escritorio y sitios web receptivos.- Implementar pruebas automatizadas integradas en los flujos de trabajo de desarrollo y mantenimiento.- Crear códigos y bibliotecas reutilizables para uso futuro.- Estar actualizado con todos los desarrollos recientes en el espacio JavaScript y Vue.js.- Estar centrado en las actualizaciones de seguridad y los problemas encontrados con Vue.js y todas las dependencias del proyecto.- Realizar actualizaciones y mejoras necesarias para mantenerse al día con las mejores prácticas modernas de seguridad y desarrollo.- Contribuir con ideas e innovaciones, siempre que vea una oportunidad de mejora.- Trabajar en colaboración con nuestros equipos multidisciplinares.¿Qué Buscamos?:- 5+ años de experiencia en desarrollo de software.- 3+ años de experiencia con el desarrollo de Vue.Js.- Fuertes habilidades con el lenguaje JavaScript y frameworks (React, Angular, Ember, etc.).- Experta o avanzada experiencia en tecnologías front-end, arquitecturas de seguridad y experiencia de usuario.- Avanzado en el desarrollo y prueba de aplicaciones web basadas en web, basadas en web móvil y totalmente receptivas utilizando marcos de JavaScript como Jest, Mocha, Chai, Jasmine, etc.- Experiencia en integraciones de servicios (servicios web, sistemas CMS / Commerce, API de terceros, etc.).- Experiencia tanto en el consumo como en el diseño de API RESTful.- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) seja mais fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO NOCTURNOOFRECEMOS:• Sueldo de hasta $10,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
       </c>
       <c r="F6" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-desarrollador-de-vuejs-ref-0255-en-benito-juarez-7A14BBB695EF0B0C61373E686DCF3405#lc=ListOffers-Score0-4</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-nocturno-central-de-abastos-en-iztapalapa-BFADA104A2B4F0B661373E686DCF3405#lc=ListOffers-Score4-4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Programador/a - Temporal</v>
+        <v>Barrenderos matutino y nocturno con o sin experiencia</v>
       </c>
       <c r="B7" t="str">
-        <v>Caja Morelia Valladolid</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C7" t="str">
-        <v>Morelia, Michoacán</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D7" t="str">
-        <v>$ 7,209</v>
+        <v>$ 8,000.00</v>
       </c>
       <c r="E7" t="str">
-        <v>Empresa Mexicana dedicada al servicio Financiero con 59 años de historia y presencia nacional, Caja Morelia Valladolid solicita personal.PROGRAMADOR TEMPORALOFECEMOS:-Sueldo base.-Prestaciones superiores a las de Ley.-Vales de despensa 8% del sueldo bruto mensual.-Fondo de ahorro del 13% del sueldo bruto mensual.-Seguro de vida.-Prima vacacional 100%.-30 días de aguinaldo desde el primer año.-Uniformes.-Opciones a becas.- Y mucho más...REQUISITOS:•Licenciatura o ingeniería Titulado en Informática, Sistemas Computacionales, TIC’s a fines.•Dominio de bases de datos SQL SERVER•Dominio de .NET C# o JAVA•Dominio Programación web (Html5, Maquetado CSS, Javascript, ECMAScript 2015+, VueJS2)•Dominio API Rest y SOAP (Net Core, nodeJS)•Dominio Programación móvil (Android, IOS, híbrido o nativo)•Manejo de Control de Versiones GIT.•Manejo de Plataforma JIRA &amp; Confluence•Deseable Delphi 6Horario de trabajo: Lunes a Viernes de 8:30 am a 5 pm y Sábados de 8:30 am a 2 pmInteresados postularse por este medio</v>
+        <v>Unete al mejor equipo de trabajo como BARRENDER@TURNOS DISPONIBLESmatutino: 9:00 am - 6:00 pmnocturno: 6pm - 6 amLunes a Sábado a Domingo descanso rolado entre semanaSalario: $2,000 semanales ( $2,500 NOCTURNO)+ prestaciones+uniformesSexo indistintoNo necesitas experienciaContratación inmediataZona de trabajo: Central de Abastos CDMX ( IZTAPALAPA)</v>
       </c>
       <c r="F7" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-programadora-temporal-en-morelia-4B58ECD317F4993161373E686DCF3405#lc=ListOffers-Score0-5</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderos-matutino-y-nocturno-con-o-sin-experiencia-en-iztapalapa-11A7D3B0A60709DB61373E686DCF3405#lc=ListOffers-Score4-5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>EG Barrendero Nocturno Central de Abastos</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D8" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO NOCTURNOOFRECEMOS:• Sueldo de hasta $10,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F8" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-nocturno-central-de-abastos-en-iztapalapa-C9417E1A9ACBCE5A61373E686DCF3405#lc=ListOffers-Score4-6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>EG Barrendero Vespertino Central de Abastos</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D9" t="str">
+        <v>$ 8,000.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO VESPERTINOOFRECEMOS:• Sueldo de hasta $8,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F9" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-vespertino-central-de-abastos-en-iztapalapa-41FCE64536945C4661373E686DCF3405#lc=ListOffers-Score4-7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Barrendero - Central de abastos cdmx (iztapalapa)</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D10" t="str">
+        <v>$ 5,437</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Se solicita para Central de Abastos:Contratación inmediata- Barrenderos NocturnoHorario 5 pm a 5 amSueldo: 10 mil pesos mensuales- Barrenderos VespertinoHorario de 10 am a 7:00 pmSueldo: 8000 pesos mensualesBarrido de patios de la centralDocumentos: Acta, ine, curp, nss, constancia sat, comprobante domicilio, estado de cuenta bancario</v>
+      </c>
+      <c r="F10" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-central-de-abastos-cdmx-iztapalapa-en-iztapalapa-001D869701974DF161373E686DCF3405#lc=ListOffers-Score4-8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Barrendero con turno fijo en la tarde - En Central de Abastos Iztapalapa</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D11" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Importante empresa dedicada al sector limpieza solicita Barrendero.Requisitos:- Mayor de 18 años- Experiencia no necesariaOfrecemos:- $8,000 mensuales netos (Pago semanal)- Prestaciones de ley- Trabajo de Lunes a Domingo con 1 descanso en la semana- Horario de 10:00 am a 7:00 pmZona de trabajo: Central de Abastos Iztapalapa.Actividades : acompañamiento de camionesLevantar basura de cajones de tolvaLevantar basura que cae de los camiones al momento de la cargaLevantar basura al paso del recorridoInteresados que cuenten con documentos (Acta de nacimiento, Cuenta de Banco, Comprobante de domicilio, INE, CURP, IMSS, RFC) postularse por éste medio, y un ejecutivo te contactará por whatsapp.</v>
+      </c>
+      <c r="F11" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-con-turno-fijo-en-la-tarde-en-central-de-abastos-iztapalapa-en-iztapalapa-33BD941F42C610F461373E686DCF3405#lc=ListOffers-Score4-9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Barrendero Nocturno - En Central de Abastos Iztapalapa</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D12" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Importante empresa dedicada al sector limpieza solicita Barrendero para el turno Nocturno.Requisitos:- Mayor de 18 años- Experiencia no necesariaOfrecemos:- $10,000 mensuales netos (Pago semanal)- Prestaciones de ley- Trabajo de Lunes a Domingo con 1 descanso en la semana- Horario de 5:00 pm a 5:00 amZona de trabajo: Central de Abastos Iztapalapa.Actividades : acompañamiento de camionesLevantar basura de cajones de tolvaLevantar basura que cae de los camiones al momento de la cargaLevantar basura al paso del recorridoInteresados que cuenten con documentos (Acta de nacimiento, Cuenta de Banco, Comprobante de domicilio, INE, CURP, IMSS, RFC) postularse por éste medio, y un ejecutivo te contactará por whatsapp.</v>
+      </c>
+      <c r="F12" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-nocturno-en-central-de-abastos-iztapalapa-en-iztapalapa-0F3EFD8ABAA464EE61373E686DCF3405#lc=ListOffers-Score4-10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Barrenderos / $2,000 a la semana Central de Abastos CDMX</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D13" t="str">
+        <v>$2,000</v>
+      </c>
+      <c r="E13" t="str">
+        <v>SOLICITAMOS POR EXPANSION: BARRENDEROSZONA: IZTAPALAPA (CENTRAL DE ABASTOS)SUELDO $2,000 semanales libresPagos semanalesContarás con Prestaciones de LeyHorario: 9:00 am a 6:00 pmLunes a Domingo, 1 día de descanso entre semana</v>
+      </c>
+      <c r="F13" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderos-2000-a-la-semana-central-de-abastos-cdmx-en-iztapalapa-75FC0F398FF27B2C61373E686DCF3405#lc=ListOffers-Score4-11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Auxiliar limpieza - Central de Abastos</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D14" t="str">
+        <v>$ 8,000.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Estamos en búsqueda de tu talento como:TENEMOS DISPONIBLES 2 VACANTES DE AUXILIAR DE LIMPIEZA:BARRENDEROTurno: Nocturno (De 6:00PM a 6:00AM)Sueldo: $10,000 mensualesBARRENDEROTurno: Vespertino (De 10:00AM a 7:00AM)Sueldo: $8,000 mensuales¡NO NECESITAS EXPERIENCIA! - INGRESO INMEDIATOSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F14" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-limpieza-central-de-abastos-en-iztapalapa-37C5E76C32BA148461373E686DCF3405#lc=ListOffers-Score3-12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Auxiliar de Limpieza sin Experiencia para Iztapalapa Turno Nocturno - $10,000 mensual Contratación el mismo dia</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D15" t="str">
+        <v>$10,000</v>
+      </c>
+      <c r="E15" t="str">
+        <v>"Importante marca de Limpieza está en busca de tu talento"Solicita Axiliar de limpieza (Barrendero) sin ExperienciaRequisitos:Tener disponibilidad de HorarioBuena ActitudLunes a Domingo con descanso entre semanaEdad: entre 18 a 55 añosNo contar con Infonavit de preferenciaSin tatuajes o perforaciones de preferenciaZona de trabajo: IztapalapaOFRECEMOS:Sueldo base Neto semana $2500 semanalNocturno 5pm a 5am $2500 semanalesPago SemanalVacante FijaSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F15" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-de-limpieza-sin-experiencia-para-iztapalapa-turno-nocturno-10000-mensual-contratacion-el-mismo-dia-en-iztapalapa-F37FE05104C1EFD961373E686DCF3405#lc=ListOffers-Score3-13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Auxiliar de Limpieza sin Experiencia para Iztapalapa Turno Intermedio - $8000 mensual Contratación el mismo dia</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D16" t="str">
+        <v>$8000</v>
+      </c>
+      <c r="E16" t="str">
+        <v>"Importante marca de Limpieza está en busca de tu talento"Solicita Axiliar de limpieza (Barrendero) sin ExperienciaRequisitos:Tener disponibilidad de HorarioBuena ActitudLunes a Domingo con descanso entre semana 10 am a 7pmEdad: entre 18 a 55 añosNo contar con Infonavit de preferenciaSin tatuajes o perforaciones de preferenciaZona de trabajo: IztapalapaOFRECEMOS:Sueldo base Neto semanal $2000 semanalIntermedio 10am a 7pm $2000 semanalesPago SemanalVacante FijaSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F16" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-de-limpieza-sin-experiencia-para-iztapalapa-turno-intermedio-8000-mensual-contratacion-el-mismo-dia-en-iztapalapa-21DBF84AE98E8B6161373E686DCF3405#lc=ListOffers-Score3-14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Auxiliares de limpieza contratación inmediata - Iztapalapa Central de abastos</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D17" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Importante empresa de residuos está en busca de tu talentoSolicitamos personal de limpieza (diversas áreas)BarrenderosAuxiliares de limpieza de pasillosLavadores de camionesZONA IZTAPALAPAOFRECEMOS:Sueldo semanal (dependiendo de la posición)Horario dependiendo de la operaciónPagos semanalesRequisitos:Disponibilidad de horarioExperiencia no necesaria o mínimaZona de trabajoCENTRAL DE ABASTOS IZTAPALAPASi estas interesada/o postúlate con tu CV actualizado o marca al 5580109495</v>
+      </c>
+      <c r="F17" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliares-de-limpieza-contratacion-inmediata-iztapalapa-central-de-abastos-en-iztapalapa-65BB4A5C627E4E3761373E686DCF3405#lc=ListOffers-Score3-15</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[FIX]: Se corrigio el error de que no cambiaba de página
</commit_message>
<xml_diff>
--- a/data/scraped/trabajos.xlsx
+++ b/data/scraped/trabajos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,127 +424,327 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Desarrollador/a FullStack</v>
+        <v>Barrendero/A - Turno Nocturno o Vespertino</v>
       </c>
       <c r="B2" t="str">
-        <v>Holcim Apasco</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C2" t="str">
-        <v>San Pedro Tlaquepaque, Jalisco</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D2" t="str">
-        <v>$ 20,000.00</v>
+        <v>$ 5,437</v>
       </c>
       <c r="E2" t="str">
-        <v>¿QUIÉN ES HOLCIM?Somos el líder mundial en soluciones innovadoras y sostenibles para la construcción mediante cuatro segmentos de negocio: cemento, concreto/hormigón premezclado, agregados, soluciones y productos.Nuestro objetivo es impulsar la construcción circular para construir más con menos. Gracias a nuestro enfoque en la reducción de emisiones de CO2, cuidado al medio ambiente, apoyo a las comunidades y desarrollo de nuestra gente, hemos logrado que nuestros 70.000 colaboradores y colaboradoras en todo el mundo sienten una gran pasión por construir progreso para las personas y el planeta, creando mejores soluciones y experiencias para sus clientes, comunidades y equipos.¡TRABAJA CON NOSOTROS!Tendrás la oportunidad de compartir la pasión que tenemos por nuestro planeta, aportar perspectivas innovadoras, dentro de un entorno dinámico y retador, que promueve la diversidad e inclusión.Porque solo si trabajamos juntos en una cultura en la que todos prosperamos, podremos construir el mundo en el que todos queremos vivir.TE ESTAMOS BUSCANDO: Desarrollador/a FullStack!Serás responsable de diseñar, desarrollar y mantener aplicaciones web completas (frontend y backend), asegurando interfaces atractivas, usabilidad, seguridad y alto rendimiento.Tus principales retos serán:Crear interfaces de usuario modernas, responsivas y funcionales.Desarrollar APIs robustas e integraciones con servicios externos.Implementar y administrar bases de datos relacionales y no relacionales.Asegurar la autenticación y seguridad de las aplicaciones.Integrar plataformas de pago y otros servicios de terceros.Colaborar con equipos multidisciplinarios en entornos ágiles.Lugar de trabajo: Carretera a Tlaquepaque Jalisco, San Martin de las flores.Requisitos indispensables:Licenciatura o ingeniería en sistemas, desarrollo de software o afín.Experiencia comprobable en desarrollo Full Stack.Dominio de HTML, CSS, JavaScript y frameworks como React, Angular o VuejsConocimientos en backend con Nodejs, Python o Java.Manejo de bases de datos relacionales (SQL Server, PostgreSQL) y no relacionales (MongoDB, Firebase).Experiencia con integración de APIs REST y GraphQL.Uso de servicios en la nube (AWS, GCP) y control de versiones con Git/GitHub.Inglés B2.Requisitos deseados:Experiencia en entornos de retail, e commerce o mayoristas (B2B/B2C).Familiaridad con plataformas de pago.Conocimientos en backend con Nodejs, Python o Java.¡NO TE PIERDAS LA OPORTUNIDAD DE SER PARTE DE NUESTRO EQUIPO!¡CONSTRUYE PROGRESO CON NOSOTROS!</v>
+        <v>Buscamos tu talento como Barrendero/a para turno Nocturno o Vespertino:Zona de trabajo: Central de abastos IztapalapaBarrenderos Nocturno (Horario 5 pm a 5 am)Barrenderos Vespertino (Horario de 10 am a 7:00 pm)Lunes a domingo descanso entre semana*Contratacion inmediata*Contar con documentacion (Acta de nacimiento, Comprobante de clabe interbancaria es decir cuenta de banco, nss, curp, ine, constancia de situacion fiscal y comprobante de domicilo)Agenda hoy mismo comunicate al 5 5 796 9 59 09</v>
       </c>
       <c r="F2" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrolladora-fullstack-en-san-pedro-tlaquepaque-7B5D20BFE204246961373E686DCF3405#lc=ListOffers-Score3-0</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderoa-turno-nocturno-o-vespertino-en-iztapalapa-8EFACEA56D1028F261373E686DCF3405#lc=ListOffers-Score4-0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Programador/a - Temporal</v>
+        <v>Barrendero Central de Abastos - Iztapalapa</v>
       </c>
       <c r="B3" t="str">
-        <v>Caja Morelia Valladolid</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C3" t="str">
-        <v>Morelia, Michoacán</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D3" t="str">
-        <v>$ 7,209</v>
+        <v>$ 10,000.00</v>
       </c>
       <c r="E3" t="str">
-        <v>Empresa Mexicana dedicada al servicio Financiero con 59 años de historia y presencia nacional, Caja Morelia Valladolid solicita personal.PROGRAMADOR TEMPORALOFECEMOS:-Sueldo base.-Prestaciones superiores a las de Ley.-Vales de despensa 8% del sueldo bruto mensual.-Fondo de ahorro del 13% del sueldo bruto mensual.-Seguro de vida.-Prima vacacional 100%.-30 días de aguinaldo desde el primer año.-Uniformes.-Opciones a becas.- Y mucho más...REQUISITOS:•Licenciatura o ingeniería Titulado en Informática, Sistemas Computacionales, TIC’s a fines.•Dominio de bases de datos SQL SERVER•Dominio de .NET C# o JAVA•Dominio Programación web (Html5, Maquetado CSS, Javascript, ECMAScript 2015+, VueJS2)•Dominio API Rest y SOAP (Net Core, nodeJS)•Dominio Programación móvil (Android, IOS, híbrido o nativo)•Manejo de Control de Versiones GIT.•Manejo de Plataforma JIRA &amp; Confluence•Deseable Delphi 6Horario de trabajo: Lunes a Viernes de 8:30 am a 5 pm y Sábados de 8:30 am a 2 pmInteresados postularse por este medio</v>
+        <v>Importante mercado está en busca de tu talentoSOLICITA BARRENDERO MATUTINO O NOCTURNOOFRECEMOS:Sueldo de $8,0000 a $10,000 neto mensualUniforme gratuitoPrestaciones de leyREQUISITOS:Experiencia no necesariaPrimaria concluidaDocumentos completos en copiaLunes a Domingo de 5pm a 5am o 10am a 7pm, 1 descanso rolado a la semanaZona de trabajo: Central de abastos Iztapalapa, CDMX5511 4122 82Si estas interesada/o postúlate con tu CV actualizado</v>
       </c>
       <c r="F3" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-programadora-temporal-en-morelia-DA3519AF994F093961373E686DCF3405#lc=ListOffers-Score0-1</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-central-de-abastos-iztapalapa-en-iztapalapa-D4CB1C1EE38BEE9A61373E686DCF3405#lc=ListOffers-Score4-1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Work From Home Shopify Engineer / Ref. 0176</v>
+        <v>Barrendero con o sin experiencia / Nocturno y Vespertino - Zona Central de abastos Iztapalapa</v>
       </c>
       <c r="B4" t="str">
-        <v>BairesDev LLC</v>
+        <v>Importante empresa del sector</v>
       </c>
       <c r="C4" t="str">
-        <v>Aguascalientes, Aguascalientes</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D4" t="str">
-        <v>$ 3,700</v>
+        <v>$9,000</v>
       </c>
       <c r="E4" t="str">
-        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Shopify Engineer at BairesDevWe are looking for a Shopify Engineer to join our Development team and help the client take its eCommerce platform to the next level. The Shopify Engineer will be responsible for designing, developing, and maintaining the clients Shopify website and integrations with other systems. This is an excellent opportunity for those professionals looking to develop in one of the fastest-growing companies in the industry!What You Will Do:- Collaborate with the eCommerce team to understand business requirements and translate them into technical solutions.- Design and implement custom Shopify themes and templates.- Build and maintain custom Shopify apps and plugins.- Integrate Shopify with other systems such as CRM, ERP, and payment gateways.- Ensure website performance and security are optimized.- Troubleshoot and resolve website issues.Heres what we are looking for:- 3+ years of experience with Shopify Liquid.- 2+ years of experience with a JS Framework (React, NextJS, VueJS, etc).- Proven track record in Shopify App development.- Shopify headless architecture experience (stores/apps) is desirable, but not mandatory.- Upper English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+        <v>Se busca barrendero para turnos nocturnos y vespertinos.Buscamos a una persona responsable, con experiencia en limpieza y mantenimiento de espacios comunes.El trabajo requiere desplazamientos cortos y uso de herramientas básicas de limpieza.Se valorará experiencia previa en limpieza, aunque no es imprescindible.Se ofrece contrato temporal con posibilidad de renovación.Se requiere disponibilidad para trabajar en horarios nocturnos y vespertinos.Se busca un perfil con actitud positiva y compromiso con el trabajo bien hecho.Se requiere puntualidad y capacidad para trabajar en equipo.Se ofrece ambiente de trabajo agradable y posibilidad de formación continua.Si tienes interés en mantener espacios limpios y cuidando los detalles, esta oportunidad puede ser para ti.Envía tu currículum con tus datos y experiencia previa en limpieza.Buscas un trabajo estable y con oportunidades de crecimiento profesional.Únete a nuestro equipo y contribuye a mantener nuestros entornos limpios y ordenados.</v>
       </c>
       <c r="F4" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-shopify-engineer-ref-0176-en-aguascalientes-2F8573081BEEE1A961373E686DCF3405#lc=ListOffers-Score0-2</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-con-o-sin-experiencia-nocturno-y-vespertino-zona-central-de-abastos-iztapalapa-en-iztapalapa-9BB6F3E7844AC9D961373E686DCF3405#lc=ListOffers-Score4-2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Trabajo Desde Casa Ingeniero Vue.js / Ref. 0255</v>
+        <v>EG Barrendero Vespertino Central de Abastos</v>
       </c>
       <c r="B5" t="str">
-        <v>BairesDev LLC</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C5" t="str">
-        <v>Miguel Hidalgo, Ciudad de México DF</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D5" t="str">
-        <v>$ 3,700</v>
+        <v>$ 8,000.00</v>
       </c>
       <c r="E5" t="str">
-        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Ingeniero Vue.js en BairesDevBuscamos Ingenieros de Vue.js para unirse a nuestro equipo de Desarrollo y participar en diferentes proyectos conformados por equipos multiculturales distribuidos por todo el mundo. Buscamos personas proactivas, jugadores de equipo apasionados por la programación en este lenguaje y orientados a brindar la mejor experiencia al usuario final.Principales responsabilidades:- Desarrollar aplicaciones de interfaz utilizando Vue.js y el ecosistema circundante.- Traducir con precisión las necesidades de los usuarios y las empresas en un código de interfaz funcional.- Desarrollar y probar IU para escritorio y sitios web receptivos.- Implementar pruebas automatizadas integradas en los flujos de trabajo de desarrollo y mantenimiento.- Crear códigos y bibliotecas reutilizables para uso futuro.- Estar actualizado con todos los desarrollos recientes en el espacio JavaScript y Vue.js.- Estar centrado en las actualizaciones de seguridad y los problemas encontrados con Vue.js y todas las dependencias del proyecto.- Realizar actualizaciones y mejoras necesarias para mantenerse al día con las mejores prácticas modernas de seguridad y desarrollo.- Contribuir con ideas e innovaciones, siempre que vea una oportunidad de mejora.- Trabajar en colaboración con nuestros equipos multidisciplinares.¿Qué Buscamos?:- 5+ años de experiencia en desarrollo de software.- 3+ años de experiencia con el desarrollo de Vue.Js.- Fuertes habilidades con el lenguaje JavaScript y frameworks (React, Angular, Ember, etc.).- Experta o avanzada experiencia en tecnologías front-end, arquitecturas de seguridad y experiencia de usuario.- Avanzado en el desarrollo y prueba de aplicaciones web basadas en web, basadas en web móvil y totalmente receptivas utilizando marcos de JavaScript como Jest, Mocha, Chai, Jasmine, etc.- Experiencia en integraciones de servicios (servicios web, sistemas CMS / Commerce, API de terceros, etc.).- Experiencia tanto en el consumo como en el diseño de API RESTful.- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) seja mais fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO VESPERTINOOFRECEMOS:• Sueldo de hasta $8,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
       </c>
       <c r="F5" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-ingeniero-vuejs-ref-0255-en-miguel-hidalgo-410F255D92AE8E8661373E686DCF3405#lc=ListOffers-Score0-3</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-vespertino-central-de-abastos-en-iztapalapa-B6999002976CCE4B61373E686DCF3405#lc=ListOffers-Score4-3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Trabajo Desde Casa Desarrollador de Vue.js / Ref. 0255</v>
+        <v>EG Barrendero Nocturno Central de Abastos</v>
       </c>
       <c r="B6" t="str">
-        <v>BairesDev LLC</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C6" t="str">
-        <v>Benito Juárez, Quintana Roo</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D6" t="str">
-        <v>$ 3,700</v>
+        <v>$ 10,000.00</v>
       </c>
       <c r="E6" t="str">
-        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Desarrollador de Vue.js en BairesDevBuscamos Desarrollador de Vue.js para unirse a nuestro equipo de Desarrollo y participar en diferentes proyectos conformados por equipos multiculturales distribuidos por todo el mundo. Buscamos personas proactivas, jugadores de equipo apasionados por la programación en este lenguaje y orientados a brindar la mejor experiencia al usuario final.Actividades principales:- Desarrollar aplicaciones de interfaz utilizando Vue.js y el ecosistema circundante.- Traducir con precisión las necesidades de los usuarios y las empresas en un código de interfaz funcional.- Desarrollar y probar IU para escritorio y sitios web receptivos.- Implementar pruebas automatizadas integradas en los flujos de trabajo de desarrollo y mantenimiento.- Crear códigos y bibliotecas reutilizables para uso futuro.- Estar actualizado con todos los desarrollos recientes en el espacio JavaScript y Vue.js.- Estar centrado en las actualizaciones de seguridad y los problemas encontrados con Vue.js y todas las dependencias del proyecto.- Realizar actualizaciones y mejoras necesarias para mantenerse al día con las mejores prácticas modernas de seguridad y desarrollo.- Contribuir con ideas e innovaciones, siempre que vea una oportunidad de mejora.- Trabajar en colaboración con nuestros equipos multidisciplinares.¿Qué Buscamos?:- 5+ años de experiencia en desarrollo de software.- 3+ años de experiencia con el desarrollo de Vue.Js.- Fuertes habilidades con el lenguaje JavaScript y frameworks (React, Angular, Ember, etc.).- Experta o avanzada experiencia en tecnologías front-end, arquitecturas de seguridad y experiencia de usuario.- Avanzado en el desarrollo y prueba de aplicaciones web basadas en web, basadas en web móvil y totalmente receptivas utilizando marcos de JavaScript como Jest, Mocha, Chai, Jasmine, etc.- Experiencia en integraciones de servicios (servicios web, sistemas CMS / Commerce, API de terceros, etc.).- Experiencia tanto en el consumo como en el diseño de API RESTful.- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) seja mais fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO NOCTURNOOFRECEMOS:• Sueldo de hasta $10,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
       </c>
       <c r="F6" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-desarrollador-de-vuejs-ref-0255-en-benito-juarez-7A14BBB695EF0B0C61373E686DCF3405#lc=ListOffers-Score0-4</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-nocturno-central-de-abastos-en-iztapalapa-BFADA104A2B4F0B661373E686DCF3405#lc=ListOffers-Score4-4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Programador/a - Temporal</v>
+        <v>Barrenderos matutino y nocturno con o sin experiencia</v>
       </c>
       <c r="B7" t="str">
-        <v>Caja Morelia Valladolid</v>
+        <v>Idea Market Solutions</v>
       </c>
       <c r="C7" t="str">
-        <v>Morelia, Michoacán</v>
+        <v>Iztapalapa, Ciudad de México DF</v>
       </c>
       <c r="D7" t="str">
-        <v>$ 7,209</v>
+        <v>$ 8,000.00</v>
       </c>
       <c r="E7" t="str">
-        <v>Empresa Mexicana dedicada al servicio Financiero con 59 años de historia y presencia nacional, Caja Morelia Valladolid solicita personal.PROGRAMADOR TEMPORALOFECEMOS:-Sueldo base.-Prestaciones superiores a las de Ley.-Vales de despensa 8% del sueldo bruto mensual.-Fondo de ahorro del 13% del sueldo bruto mensual.-Seguro de vida.-Prima vacacional 100%.-30 días de aguinaldo desde el primer año.-Uniformes.-Opciones a becas.- Y mucho más...REQUISITOS:•Licenciatura o ingeniería Titulado en Informática, Sistemas Computacionales, TIC’s a fines.•Dominio de bases de datos SQL SERVER•Dominio de .NET C# o JAVA•Dominio Programación web (Html5, Maquetado CSS, Javascript, ECMAScript 2015+, VueJS2)•Dominio API Rest y SOAP (Net Core, nodeJS)•Dominio Programación móvil (Android, IOS, híbrido o nativo)•Manejo de Control de Versiones GIT.•Manejo de Plataforma JIRA &amp; Confluence•Deseable Delphi 6Horario de trabajo: Lunes a Viernes de 8:30 am a 5 pm y Sábados de 8:30 am a 2 pmInteresados postularse por este medio</v>
+        <v>Unete al mejor equipo de trabajo como BARRENDER@TURNOS DISPONIBLESmatutino: 9:00 am - 6:00 pmnocturno: 6pm - 6 amLunes a Sábado a Domingo descanso rolado entre semanaSalario: $2,000 semanales ( $2,500 NOCTURNO)+ prestaciones+uniformesSexo indistintoNo necesitas experienciaContratación inmediataZona de trabajo: Central de Abastos CDMX ( IZTAPALAPA)</v>
       </c>
       <c r="F7" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-programadora-temporal-en-morelia-4B58ECD317F4993161373E686DCF3405#lc=ListOffers-Score0-5</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderos-matutino-y-nocturno-con-o-sin-experiencia-en-iztapalapa-11A7D3B0A60709DB61373E686DCF3405#lc=ListOffers-Score4-5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>EG Barrendero Nocturno Central de Abastos</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D8" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO NOCTURNOOFRECEMOS:• Sueldo de hasta $10,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F8" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-nocturno-central-de-abastos-en-iztapalapa-C9417E1A9ACBCE5A61373E686DCF3405#lc=ListOffers-Score4-6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>EG Barrendero Vespertino Central de Abastos</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D9" t="str">
+        <v>$ 8,000.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO VESPERTINOOFRECEMOS:• Sueldo de hasta $8,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F9" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-vespertino-central-de-abastos-en-iztapalapa-41FCE64536945C4661373E686DCF3405#lc=ListOffers-Score4-7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Barrendero - Central de abastos cdmx (iztapalapa)</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D10" t="str">
+        <v>$ 5,437</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Se solicita para Central de Abastos:Contratación inmediata- Barrenderos NocturnoHorario 5 pm a 5 amSueldo: 10 mil pesos mensuales- Barrenderos VespertinoHorario de 10 am a 7:00 pmSueldo: 8000 pesos mensualesBarrido de patios de la centralDocumentos: Acta, ine, curp, nss, constancia sat, comprobante domicilio, estado de cuenta bancario</v>
+      </c>
+      <c r="F10" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-central-de-abastos-cdmx-iztapalapa-en-iztapalapa-001D869701974DF161373E686DCF3405#lc=ListOffers-Score4-8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Barrendero con turno fijo en la tarde - En Central de Abastos Iztapalapa</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D11" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Importante empresa dedicada al sector limpieza solicita Barrendero.Requisitos:- Mayor de 18 años- Experiencia no necesariaOfrecemos:- $8,000 mensuales netos (Pago semanal)- Prestaciones de ley- Trabajo de Lunes a Domingo con 1 descanso en la semana- Horario de 10:00 am a 7:00 pmZona de trabajo: Central de Abastos Iztapalapa.Actividades : acompañamiento de camionesLevantar basura de cajones de tolvaLevantar basura que cae de los camiones al momento de la cargaLevantar basura al paso del recorridoInteresados que cuenten con documentos (Acta de nacimiento, Cuenta de Banco, Comprobante de domicilio, INE, CURP, IMSS, RFC) postularse por éste medio, y un ejecutivo te contactará por whatsapp.</v>
+      </c>
+      <c r="F11" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-con-turno-fijo-en-la-tarde-en-central-de-abastos-iztapalapa-en-iztapalapa-33BD941F42C610F461373E686DCF3405#lc=ListOffers-Score4-9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Barrendero Nocturno - En Central de Abastos Iztapalapa</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D12" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Importante empresa dedicada al sector limpieza solicita Barrendero para el turno Nocturno.Requisitos:- Mayor de 18 años- Experiencia no necesariaOfrecemos:- $10,000 mensuales netos (Pago semanal)- Prestaciones de ley- Trabajo de Lunes a Domingo con 1 descanso en la semana- Horario de 5:00 pm a 5:00 amZona de trabajo: Central de Abastos Iztapalapa.Actividades : acompañamiento de camionesLevantar basura de cajones de tolvaLevantar basura que cae de los camiones al momento de la cargaLevantar basura al paso del recorridoInteresados que cuenten con documentos (Acta de nacimiento, Cuenta de Banco, Comprobante de domicilio, INE, CURP, IMSS, RFC) postularse por éste medio, y un ejecutivo te contactará por whatsapp.</v>
+      </c>
+      <c r="F12" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-nocturno-en-central-de-abastos-iztapalapa-en-iztapalapa-0F3EFD8ABAA464EE61373E686DCF3405#lc=ListOffers-Score4-10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Barrenderos / $2,000 a la semana Central de Abastos CDMX</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D13" t="str">
+        <v>$2,000</v>
+      </c>
+      <c r="E13" t="str">
+        <v>SOLICITAMOS POR EXPANSION: BARRENDEROSZONA: IZTAPALAPA (CENTRAL DE ABASTOS)SUELDO $2,000 semanales libresPagos semanalesContarás con Prestaciones de LeyHorario: 9:00 am a 6:00 pmLunes a Domingo, 1 día de descanso entre semana</v>
+      </c>
+      <c r="F13" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderos-2000-a-la-semana-central-de-abastos-cdmx-en-iztapalapa-75FC0F398FF27B2C61373E686DCF3405#lc=ListOffers-Score4-11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Auxiliar limpieza - Central de Abastos</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D14" t="str">
+        <v>$ 8,000.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Estamos en búsqueda de tu talento como:TENEMOS DISPONIBLES 2 VACANTES DE AUXILIAR DE LIMPIEZA:BARRENDEROTurno: Nocturno (De 6:00PM a 6:00AM)Sueldo: $10,000 mensualesBARRENDEROTurno: Vespertino (De 10:00AM a 7:00AM)Sueldo: $8,000 mensuales¡NO NECESITAS EXPERIENCIA! - INGRESO INMEDIATOSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F14" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-limpieza-central-de-abastos-en-iztapalapa-37C5E76C32BA148461373E686DCF3405#lc=ListOffers-Score3-12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Auxiliar de Limpieza sin Experiencia para Iztapalapa Turno Nocturno - $10,000 mensual Contratación el mismo dia</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D15" t="str">
+        <v>$10,000</v>
+      </c>
+      <c r="E15" t="str">
+        <v>"Importante marca de Limpieza está en busca de tu talento"Solicita Axiliar de limpieza (Barrendero) sin ExperienciaRequisitos:Tener disponibilidad de HorarioBuena ActitudLunes a Domingo con descanso entre semanaEdad: entre 18 a 55 añosNo contar con Infonavit de preferenciaSin tatuajes o perforaciones de preferenciaZona de trabajo: IztapalapaOFRECEMOS:Sueldo base Neto semana $2500 semanalNocturno 5pm a 5am $2500 semanalesPago SemanalVacante FijaSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F15" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-de-limpieza-sin-experiencia-para-iztapalapa-turno-nocturno-10000-mensual-contratacion-el-mismo-dia-en-iztapalapa-F37FE05104C1EFD961373E686DCF3405#lc=ListOffers-Score3-13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Auxiliar de Limpieza sin Experiencia para Iztapalapa Turno Intermedio - $8000 mensual Contratación el mismo dia</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D16" t="str">
+        <v>$8000</v>
+      </c>
+      <c r="E16" t="str">
+        <v>"Importante marca de Limpieza está en busca de tu talento"Solicita Axiliar de limpieza (Barrendero) sin ExperienciaRequisitos:Tener disponibilidad de HorarioBuena ActitudLunes a Domingo con descanso entre semana 10 am a 7pmEdad: entre 18 a 55 añosNo contar con Infonavit de preferenciaSin tatuajes o perforaciones de preferenciaZona de trabajo: IztapalapaOFRECEMOS:Sueldo base Neto semanal $2000 semanalIntermedio 10am a 7pm $2000 semanalesPago SemanalVacante FijaSi estas interesada/o postúlate con tu CV actualizado</v>
+      </c>
+      <c r="F16" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-de-limpieza-sin-experiencia-para-iztapalapa-turno-intermedio-8000-mensual-contratacion-el-mismo-dia-en-iztapalapa-21DBF84AE98E8B6161373E686DCF3405#lc=ListOffers-Score3-14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Auxiliares de limpieza contratación inmediata - Iztapalapa Central de abastos</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Idea Market Solutions</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Iztapalapa, Ciudad de México DF</v>
+      </c>
+      <c r="D17" t="str">
+        <v>$ 10,000.00</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Importante empresa de residuos está en busca de tu talentoSolicitamos personal de limpieza (diversas áreas)BarrenderosAuxiliares de limpieza de pasillosLavadores de camionesZONA IZTAPALAPAOFRECEMOS:Sueldo semanal (dependiendo de la posición)Horario dependiendo de la operaciónPagos semanalesRequisitos:Disponibilidad de horarioExperiencia no necesaria o mínimaZona de trabajoCENTRAL DE ABASTOS IZTAPALAPASi estas interesada/o postúlate con tu CV actualizado o marca al 5580109495</v>
+      </c>
+      <c r="F17" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliares-de-limpieza-contratacion-inmediata-iztapalapa-central-de-abastos-en-iztapalapa-65BB4A5C627E4E3761373E686DCF3405#lc=ListOffers-Score3-15</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ADD]: se agrego funcionalidad para que no aparezca el chrome a la hora de ejecutar scrapping
</commit_message>
<xml_diff>
--- a/data/scraped/trabajos.xlsx
+++ b/data/scraped/trabajos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,327 +424,1627 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Barrendero/A - Turno Nocturno o Vespertino</v>
+        <v>Trabajo Desde Casa Desarrollador Next.js / Ref. 0697</v>
       </c>
       <c r="B2" t="str">
-        <v>Idea Market Solutions</v>
+        <v>BairesDev LLC</v>
       </c>
       <c r="C2" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Puebla, Puebla</v>
       </c>
       <c r="D2" t="str">
-        <v>$ 5,437</v>
+        <v>$ 3,700</v>
       </c>
       <c r="E2" t="str">
-        <v>Buscamos tu talento como Barrendero/a para turno Nocturno o Vespertino:Zona de trabajo: Central de abastos IztapalapaBarrenderos Nocturno (Horario 5 pm a 5 am)Barrenderos Vespertino (Horario de 10 am a 7:00 pm)Lunes a domingo descanso entre semana*Contratacion inmediata*Contar con documentacion (Acta de nacimiento, Comprobante de clabe interbancaria es decir cuenta de banco, nss, curp, ine, constancia de situacion fiscal y comprobante de domicilo)Agenda hoy mismo comunicate al 5 5 796 9 59 09</v>
+        <v>En BairesDev® llevamos 15 años liderando proyectos de tecnología para clientes como Google, Rolls-Royce y las startups más innovadoras de Silicon Valley. Actualmente, contamos con un equipo de 4000 profesionales conformado por el top 1% de la industria trabajando de forma remota desde más de 50 países.Al postularte a esta vacante, estarás dando el primer paso en un proceso que va más allá de lo convencional: Buscaremos conocer en profundidad tus habilidades, intereses y expectativas con el objetivo de realizar una búsqueda personalizada y encontrar el rol ideal para ti en BairesDev.Desarrollador Next.js en BairesDevEstamos buscando un desarrollador de Next.js para trabajar en una agencia de comercio y experiencia del cliente global de servicio completo. Esta es una excelente oportunidad para ser uno de los miembros clave de nuestro equipo de Ingeniería y posicionarse para oportunidades únicas de crecimiento profesional.Principales responsabilidades:- Desarrollar software y aplicaciones web de calidad.- Analizar y mantener las aplicaciones de software existentes.- Diseñar código altamente escalable y comprobable.- Descubrir y corregir errores de programación.¿Qué Buscamos?:- 3+ años de experiencia en Next.js.- 3+ años de experiencia profesional en el desarrollo de aplicaciones web listas para producción- Propiedad de la obra de principio a fin.- Competencia en el desarrollo de aplicaciones web y comprensión de los marcos JavaScript y React.- Experiencia con sistemas de bases de datos relacionales (por ejemplo, PostgreSQL, MySQL).- Nivel de inglés avanzado.Qué ofrecemos para que tu trabajo (y tu vida) sea más fácil:- Trabajo 100% remoto: trabaja desde tu casa o donde quieras.- Compensación en USD o en tu moneda local, como prefieras, muy por encima de la media del mercado.- Hardware y software.- Horarios flexibles- Licencias por mater/paternidad, vacaciones y días festivos nacionales pagos.- Ambiente laboral multicultural e innovador, perfecto para hacer amigos, colaborar y aprender de las personas más talentosas del mundo.- Oportunidades de crecimiento y desarrollo profesional a través de mentorías y entrenamientos.¡Únete a nuestro equipo global!</v>
       </c>
       <c r="F2" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderoa-turno-nocturno-o-vespertino-en-iztapalapa-8EFACEA56D1028F261373E686DCF3405#lc=ListOffers-Score4-0</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-trabajo-desde-casa-desarrollador-nextjs-ref-0697-en-puebla-92B7C9A73131DB0E61373E686DCF3405#lc=ListOffers-Score4-0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Barrendero Central de Abastos - Iztapalapa</v>
+        <v>Work From Home Next.js Developer / Ref. 0697</v>
       </c>
       <c r="B3" t="str">
-        <v>Idea Market Solutions</v>
+        <v>BairesDev LLC</v>
       </c>
       <c r="C3" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Mérida, Yucatán</v>
       </c>
       <c r="D3" t="str">
-        <v>$ 10,000.00</v>
+        <v>$ 3,700</v>
       </c>
       <c r="E3" t="str">
-        <v>Importante mercado está en busca de tu talentoSOLICITA BARRENDERO MATUTINO O NOCTURNOOFRECEMOS:Sueldo de $8,0000 a $10,000 neto mensualUniforme gratuitoPrestaciones de leyREQUISITOS:Experiencia no necesariaPrimaria concluidaDocumentos completos en copiaLunes a Domingo de 5pm a 5am o 10am a 7pm, 1 descanso rolado a la semanaZona de trabajo: Central de abastos Iztapalapa, CDMX5511 4122 82Si estas interesada/o postúlate con tu CV actualizado</v>
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Next.js Developer at BairesDevWe are looking for a Next.js developer to work in a full-service global customer experience and commerce agency. This is an excellent opportunity to be one of the key members of our Engineering team and position yourself for unique career growth opportunities.What You Will Do:- Develop quality software and web applications.- Analyze and maintain existing software applications.- Design highly scalable, testable code.- Discover and fix programming bugs.Heres what we are looking for:- 3+ years of Next.js experience.- 3+ years of professional experience developing production ready web applications.- Ownership of work from beginning to end.- Proficiency developing web applications and understanding of JavaScript and React frameworks.- Experience with relational database systems (e.g. PostgreSQL, MySQL).- Advanced English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
       </c>
       <c r="F3" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-central-de-abastos-iztapalapa-en-iztapalapa-D4CB1C1EE38BEE9A61373E686DCF3405#lc=ListOffers-Score4-1</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-nextjs-developer-ref-0697-en-merida-E2FEE67F615966CC61373E686DCF3405#lc=ListOffers-Score4-1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Barrendero con o sin experiencia / Nocturno y Vespertino - Zona Central de abastos Iztapalapa</v>
+        <v>Coordinador Contable administrativo - fiscal</v>
       </c>
       <c r="B4" t="str">
         <v>Importante empresa del sector</v>
       </c>
       <c r="C4" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>San Pedro Tlaquepaque, Jalisco</v>
       </c>
       <c r="D4" t="str">
-        <v>$9,000</v>
+        <v>$ 23,900.00</v>
       </c>
       <c r="E4" t="str">
-        <v>Se busca barrendero para turnos nocturnos y vespertinos.Buscamos a una persona responsable, con experiencia en limpieza y mantenimiento de espacios comunes.El trabajo requiere desplazamientos cortos y uso de herramientas básicas de limpieza.Se valorará experiencia previa en limpieza, aunque no es imprescindible.Se ofrece contrato temporal con posibilidad de renovación.Se requiere disponibilidad para trabajar en horarios nocturnos y vespertinos.Se busca un perfil con actitud positiva y compromiso con el trabajo bien hecho.Se requiere puntualidad y capacidad para trabajar en equipo.Se ofrece ambiente de trabajo agradable y posibilidad de formación continua.Si tienes interés en mantener espacios limpios y cuidando los detalles, esta oportunidad puede ser para ti.Envía tu currículum con tus datos y experiencia previa en limpieza.Buscas un trabajo estable y con oportunidades de crecimiento profesional.Únete a nuestro equipo y contribuye a mantener nuestros entornos limpios y ordenados.</v>
+        <v>COORDINADOR CONTABLE-ADMINISTRATIVOPROPOSITO: Asegurar el cumplimiento de las funciones del área contable, supervisando los registros de provisión, egreso, venta e ingreso en sistema contable CONTPAQi conforme a las Normas de Información Financiera y/o Principios contables; además de la correcta aplicación y pago a los colabores; garantizar operaciones de facturación, cortes e inventarios en CEDIS y Retail; el registro correcto de las operaciones mencionadas permitirá generar Información Financiera veraz y oportuna para la toma de decisiones, así como la determinación y entero de obligaciones fiscales.Sexo IndistintoLicenciatura en Contaduría (deseable fiscal-administracion)Experiencia mínima 3 años en puesto similarConocimientos técnicos:*Contables-Financieros*-Conocer normativa contable NIF (Normas de Información Financiera y/o Principios contables)-Registros contables.-Administración y control de los recursos, ej. Flujo Efectivo, Inversión, Cuentas por cobrar.-Interpretación de Información Financiera.-Conocer y entender razones financieras del negocio.-Elaboración de Informes.*Fiscal*-Conocer legislación fiscal.-Saber elaborar y presentar declaraciones de cualquier tipo, en Régimen General de Ley.*Deseable conocer sistema de facturación y control de Inventario de sistemas Sizes &amp; Colors -Next.Principales Actividades-Asegurar y hacer cumplir cada uno de los procesos del departamento Administrativo:-Pago correcto y oportuno de Nómina y otras prestaciones a colaboradores.-Emisión de Facturación a clientes.-Pago correcto a Proveedores.-Registro contable correcto y en tiempo de provisión de gastos, provisión de compras, egresos, ingresos, ventas.-Antigüedad de saldos de clientes veraz y oportuno.-Registro oportuno de los depósitos de clientes de CEDIS y Tiendas.-Elaborar y presentar estados financieros a dirección general y gerencia de zona.-Elaborar y determinar papel de trabajo de costos de operación de CEDIS y Tiendas.-Determinar, presentar y enterar obligaciones fiscales, seguridad social.Ofrecemos:Sueldo competitivoPago semanalVales de despensaBono de puntualidadBono de asistenciaPrestaciones de leyCrecimiento laboralContratación directa por la empresa</v>
       </c>
       <c r="F4" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-con-o-sin-experiencia-nocturno-y-vespertino-zona-central-de-abastos-iztapalapa-en-iztapalapa-9BB6F3E7844AC9D961373E686DCF3405#lc=ListOffers-Score4-2</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-coordinador-contable-administrativo-fiscal-en-san-pedro-tlaquepaque-4F9175A0910F7E3161373E686DCF3405#lc=ListOffers-Score3-2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>EG Barrendero Vespertino Central de Abastos</v>
+        <v>Specialty Chef – Indian Cuisine - Moon Palace</v>
       </c>
       <c r="B5" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Palace Resorts</v>
       </c>
       <c r="C5" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Benito Juárez, Quintana Roo</v>
       </c>
       <c r="D5" t="str">
-        <v>$ 8,000.00</v>
+        <v>$ 13,095</v>
       </c>
       <c r="E5" t="str">
-        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO VESPERTINOOFRECEMOS:• Sueldo de hasta $8,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>Are you an expert in cooking, with a focus on Indian cuisine?Moon Palace Cancun is looking for its next Specialty Chef in Indian Cuisine!Join a hotel chain known for innovation, excellence, and world-class hospitality:What are we looking for?• Intermediate English• Culinary studies• Knowledge of Food and Beverage Hygiene Standards, General Kitchen Standards, Culinary Specialties, and Cost Control• Experience in preparing Indian specialty dishesWhat do we offer?• Lead in one of the most exclusive resorts in the Caribbean• Top-tier work environment• Real opportunities for professional growth• Ongoing training and access to cutting-edge technologies• Superior benefits and unique perksCancun, Mexico | Moon Palace CancunApply today and discover what it means to be part of the next level in hospitality!</v>
       </c>
       <c r="F5" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-vespertino-central-de-abastos-en-iztapalapa-B6999002976CCE4B61373E686DCF3405#lc=ListOffers-Score4-3</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-specialty-chef-indian-cuisine-moon-palace-en-benito-juarez-FF00836AD5746FB561373E686DCF3405#lc=ListOffers-Score3-3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>EG Barrendero Nocturno Central de Abastos</v>
+        <v>Tech Leader</v>
       </c>
       <c r="B6" t="str">
-        <v>Idea Market Solutions</v>
+        <v>AVASA</v>
       </c>
       <c r="C6" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Mérida, Yucatán</v>
       </c>
       <c r="D6" t="str">
-        <v>$ 10,000.00</v>
+        <v>$ 45,000.00</v>
       </c>
       <c r="E6" t="str">
-        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO NOCTURNOOFRECEMOS:• Sueldo de hasta $10,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>Buscamos sumarte a nuestro equipo de trabajo, para desarrollarte como:TEACH LEADEROfrecemos:-Atractivo sueldo acorde a aptitudes-Prestaciones de ley (inmediatas)-Beneficios internos-Oportunidades de desarrollo y crecimientoFunciones:-Conocimiento y capacidad para liderar equipos de trabajo-Acostumbrado a trabajar por objetivos-Diseño y desarrollo de aplicaciones web (Next.js)-Implementar y mantener APis y servicios backend en Node,js-Code reviews-Colaborar con el product ownerImportante-Experiencia mínima 5 años-Disponibilidad para trabajar presencialmente</v>
       </c>
       <c r="F6" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-nocturno-central-de-abastos-en-iztapalapa-BFADA104A2B4F0B661373E686DCF3405#lc=ListOffers-Score4-4</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-tech-leader-en-merida-E3AAC97D5DD966BA61373E686DCF3405#lc=ListOffers-Score3-4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Barrenderos matutino y nocturno con o sin experiencia</v>
+        <v>New Bilingual Technical Support Campaign</v>
       </c>
       <c r="B7" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Telvista</v>
       </c>
       <c r="C7" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Tijuana, Baja California</v>
       </c>
       <c r="D7" t="str">
-        <v>$ 8,000.00</v>
+        <v>$ 16,000.00</v>
       </c>
       <c r="E7" t="str">
-        <v>Unete al mejor equipo de trabajo como BARRENDER@TURNOS DISPONIBLESmatutino: 9:00 am - 6:00 pmnocturno: 6pm - 6 amLunes a Sábado a Domingo descanso rolado entre semanaSalario: $2,000 semanales ( $2,500 NOCTURNO)+ prestaciones+uniformesSexo indistintoNo necesitas experienciaContratación inmediataZona de trabajo: Central de Abastos CDMX ( IZTAPALAPA)</v>
+        <v>We are excited to have you as part of are new campaign in TELvista!We are looking for talented who want to be part of our growing team of technical support.TELvista offers an excellent work environment, benefits by law and access to exclusive programs:You can choose your schedule!!!Base salary $4,000 pesos A WEEKAttendance &amp; productivity BONUS.REQUIREMENTS:Advance Conversational EnglishPC skillsIf youre ready to take the next step in your career, we can have an Interview today and join one of the best companies to work for.</v>
       </c>
       <c r="F7" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderos-matutino-y-nocturno-con-o-sin-experiencia-en-iztapalapa-11A7D3B0A60709DB61373E686DCF3405#lc=ListOffers-Score4-5</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-new-bilingual-technical-support-campaign-en-tijuana-1AC9CD048BB25A1861373E686DCF3405#lc=ListOffers-Score3-5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>EG Barrendero Nocturno Central de Abastos</v>
+        <v>Soporte de mesa de ayuda</v>
       </c>
       <c r="B8" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Promologistics</v>
       </c>
       <c r="C8" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
       </c>
       <c r="D8" t="str">
-        <v>$ 10,000.00</v>
+        <v>$ 11,000.00</v>
       </c>
       <c r="E8" t="str">
-        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO NOCTURNOOFRECEMOS:• Sueldo de hasta $10,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>Te estamos buscandoTu misión será ofrecer un servicio de atención al cliente de alta calidad, gestionando y resolviendo problemas técnicos y operativos de manera eficiente.Objetivo de la Posición:Otorgar soporte a la operación del ERP y servicios de Next Cloud.Responsabilidades Principales:1. Atención al cliente final mediante llamada telefónica, portal de tickets, correo electrónico.2. Seguimiento y persecución de tickets.3. Escalamiento de tickets a con el resto de áreas de Next Cloud.Indicadores de Desempeño.Cumplimiento de SLA de atencion de tickets y NPSCierre de tickets efectivamente validados por el cliente.Encuesta de satisfaccion por ticket cerradoConocimientos y experiencia:Indispensable:- Mínimo 1 años como ejecutivo de soporte de mesa de ayuda en ERP.- Paquetería de Microsoft Office- Trato directo con cliente, facilidad de palabra.- Excelente redaccion y ortografiaImportante:- Soporte de plataformas tecnológicas.- Curva de aprendizaje corta.- Conocimiento de sistemas de gestión de tareas y atención a clientesOfrecemos:$11,000 pesos netos mensualesEsquema Hibrido 80% HO y 20 Oficina.Prestaciones de LeyEl trabajo ofrece una oportunidad para formar parte de un equipo dinámico y comprometido con la excelencia en servicio al cliente.Ofrecemos un entorno de trabajo flexibleSi tienes un enfoque orientado al servicio y una capacidad para trabajar en equipo, esta posición podría ser ideal para ti.Únete a nosotros y contribuye al éxito de nuestro equipo de soporte.</v>
       </c>
       <c r="F8" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-nocturno-central-de-abastos-en-iztapalapa-C9417E1A9ACBCE5A61373E686DCF3405#lc=ListOffers-Score4-6</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-soporte-de-mesa-de-ayuda-en-miguel-hidalgo-8B96CEAEA5E648BD61373E686DCF3405#lc=ListOffers-Score3-6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>EG Barrendero Vespertino Central de Abastos</v>
+        <v>Full Stack Python Engineer</v>
       </c>
       <c r="B9" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Pearl Talent</v>
       </c>
       <c r="C9" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Colombia</v>
       </c>
       <c r="D9" t="str">
-        <v>$ 8,000.00</v>
+        <v>$5</v>
       </c>
       <c r="E9" t="str">
-        <v>Importante empresa de MANTENIMIENTO está en busca de tu talentoSolicita: BARRENDERO VESPERTINOOFRECEMOS:• Sueldo de hasta $8,000• Prestaciones de ley• PAGO SEMANALREQUISITOS:• SIN EXPERIENCIA• Escolaridad mínima• L a D• Horario fijoZONA DE TRABAJO: CENTRAL DE ABASTOS, IZTAPALAPA, CDMXSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>DescriptionWork Arrangement: Fully remote, overlapping EST working hours.Job Type: Full-timeSalary Range: based on experience, with performance-based bonuses.Work Schedule: 40 hours per week, with core hours between 9 AM – 5 PM EST (flexible based on sprint deadlines).Locations: Remote, open to candidates globally.About Pearl TalentPearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Hear why we exist, what we believe in, and who we’re building for:Why Work with Us?We’re not just another recruiting firm—we focus on placing candidates with exceptional US and EU founders who prioritize the long-term success of their team members. We also provide retention bonuses at 3, 6, 9, and 12 months, as well as community-driven benefits like an annual retreat.Role OverviewAs a Full Stack Python Engineer, you’ll take ownership of our Integrations Platform - the infrastructure that powers external system connectivity and real-time, AI-driven workflows. This role blends deep backend expertise with strong frontend skills, as you’ll be building both robust API integrations and intuitive UI components for our visual workflow builder. You’ll work across the full product lifecycle, translating complex business needs into scalable software that directly impacts customers. Ideal for engineers who thrive at the intersection of product and code, and who want to help define the future of intelligent, configurable SaaS.Key ResponsibilitiesBack-End Development:Own the integrations platform that connects external systems to real-time, AI-driven workflows.Design and scale FastAPI services that support dynamic, customer-configurable workflows.Build reusable, intelligent backend nodes using Python, FastAPI, and LangGraph to automate key business logic.Interface with both modern APIs and legacy enterprise systems (e.g., SOAP/XML).Optimize PostgreSQL queries and ensure high system reliability with Redis-backed caching.Front-End Development:Develop and maintain the visual workflow builder using React and TypeScript (Next.js).Translate complex backend logic into clear, intuitive UI components used directly by customers.Work closely with product and design to ensure frontend UX aligns with customer needs.AI &amp; Infrastructure Integration:Implement AI-powered automation nodes using OpenAI, LangChain, and Google Cloud AI services.Maintain clean, containerized deployment workflows using Docker and Google Cloud Platform.Cross-functional Collaboration:Partner with product stakeholders to shape features from concept to production.Translate real-world customer pain points into scalable software solutions.Contribute to product strategy with a strong understanding of usability and business impact.RequirementsMust-Have:5+ years of professional full-stack engineering experienceSolid experience with Python (FastAPI), PostgreSQL, and modern backend architectureFrontend proficiency in React, TypeScript, and component-based designExperience delivering customer-facing features - not just internal toolsStrong product thinking - you care about the "why" behind the codeComfortable working with both RESTful and legacy APIs (e.g., SOAP/XML)Strong communication skills and remote collaboration habitsNice-to-Have:Experience with workflow automation tools or visual buildersFamiliarity with logistics platforms or enterprise system integrationsBackground in AI/ML tools (LangChain, LangGraph, OpenAI APIs)Hands-on with Docker and deployment on Google CloudWhat You’ll Love About This RoleYou’ll be building software that feels like magic to our users - combining powerful backend workflows, sleek UI, and AI to automate the world's most complex industries. This is your chance to take ownership of critical systems and help shape a platform poised to redefine how vertical SaaS gets built.BenefitsCompensation PackageCompetitive Salary: Based on experience and skillsRemote Work: Fully remote—work from anywhereGenerous PTO: Ample paid time off to rest and rechargeDirect Mentorship: Grow through guidance from international industry expertsLearning &amp; Development: Ongoing access to resources for professional growthGlobal Networking: Work and connect with professionals around the worldWork-Life Balance: Flexible hours that support a healthy work-life balanceOur Recruitment ProcessApplicationScreeningTop-grading InterviewSkills Assessment: Technical Assessment + Internal AssessmentClient InterviewJob OfferClient OnboardingReady to Join Us?If this role aligns with your skills and career goals, we’d love to hear from you. Apply now to take the next step in your journey with Pearl.</v>
       </c>
       <c r="F9" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-eg-barrendero-vespertino-central-de-abastos-en-iztapalapa-41FCE64536945C4661373E686DCF3405#lc=ListOffers-Score4-7</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-full-stack-python-engineer-en-colombia-CD530EDE89DB0E5461373E686DCF3405#lc=ListOffers-Score3-7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Barrendero - Central de abastos cdmx (iztapalapa)</v>
+        <v>Sales Team Lead</v>
       </c>
       <c r="B10" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Pearl Talent</v>
       </c>
       <c r="C10" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Chihuahua, Chihuahua</v>
       </c>
       <c r="D10" t="str">
-        <v>$ 5,437</v>
+        <v>$5</v>
       </c>
       <c r="E10" t="str">
-        <v>Se solicita para Central de Abastos:Contratación inmediata- Barrenderos NocturnoHorario 5 pm a 5 amSueldo: 10 mil pesos mensuales- Barrenderos VespertinoHorario de 10 am a 7:00 pmSueldo: 8000 pesos mensualesBarrido de patios de la centralDocumentos: Acta, ine, curp, nss, constancia sat, comprobante domicilio, estado de cuenta bancario</v>
+        <v>DescriptionJob Type: Full-time (40 hours/week)Salary Range: based on experience, with performance-based bonuses.Work Schedule: Monday to Friday, ideally 9:00 AM – 6:00 PM ESTLocations: Remote — candidates must be in EST or have 4+ hours overlapAbout Pearl TalentPearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Hear why we exist, what we believe in, and who we’re building for:Why Work with Us?We’re not just another recruiting firm—we focus on placing candidates with exceptional US and EU founders who prioritize the long-term success of their team members. We also provide retention bonuses at 3, 6, 9, and 12 months, as well as community-driven benefits like an annual retreat.Role OverviewWe’re seeking two high-performing Sales Enablement Team Managers, based in Latin America, to establish and scale both our inbound and outbound sales operations. These roles are instrumental in building the operational infrastructure, setting KPIs, and leading future teams of individual contributors to drive revenue growth and customer success.As a key leader, you will initially collaborate directly with senior leadership and actively participate in calls to refine processes, develop SOPs, and set the foundation for scalable sales functions. Once established, you will transition to managing a team, ensuring performance, coaching, and continual optimization of our sales strategies.Key ResponsibilitiesPersonally conduct inbound/outbound calls during the initial ramp period to assess and improve sales processes.Develop, document, and implement detailed onboarding plans, SOPs, FAQs, and sales playbooks to support scalable team operations.Define and monitor sales KPIs, ensuring team accountability and performance optimization.Build and manage a high-performing team of sales individual contributors, providing coaching, call reviews, and performance feedback.Act as a strategic partner to leadership, providing regular reports and insights on sales metrics, pipeline progress, and revenue outcomes.Optimize inbound and outbound sales processes through data-driven experimentation and best practices.Lead team training initiatives, including negotiation tactics, objection handling, upselling, and cross-selling techniques.Foster clarity of roles, expectations, and performance standards within the team.Collaborate on the implementation of sales tools and systems to improve efficiency and tracking.Serve as the internal advocate for customer insights, surfacing feedback to inform product and operational strategies.RequirementsMust-Have:Bilingual in Spanish and English.Proven leadership experience managing sales teams, with a track record of driving revenue growth.Strong sales acumen with advanced negotiation and objection handling skills.Experience developing sales processes, defining KPIs, and coaching sales representatives.Data-driven approach to performance management and sales optimization.Excellent written and verbal English communication skills.Highly organized, self-motivated, and adaptable to fast-paced, remote environments.Nice-to-Have:Background in telecom, SaaS, or relationship-driven tech businesses.Experience building remote, distributed sales teams.Familiarity with CRM systems such as HubSpot or Salesforce.Exposure to VoIP tools like OpenPhone.Passion for human-centric products and services.Tools &amp; Communication Channels:CRM: HubSpot, SalesforceDialers: OpenPhoneMessaging: Slack, ZoomDocumentation: Notion, Google DocsScheduling: Calendly, Google CalendarBenefitsCompensation PackageCompetitive Salary: Based on experience and skillsRemote Work: Fully remote—work from anywhereGenerous PTO: Ample paid time off to rest and rechargeHealth Coverage: HMO coverage after 3 months for full-time employeesDirect Mentorship: Grow through guidance from international industry expertsLearning &amp; Development: Ongoing access to resources for professional growthGlobal Networking: Work and connect with professionals around the worldWork-Life Balance: Flexible hours that support a healthy work-life balanceOur Recruitment ProcessApplicationScreeningTop-grading InterviewSkills AssessmentClient InterviewJob OfferClient OnboardingReady to Join Us?If this role aligns with your skills and career goals, we’d love to hear from you. Apply now to take the next step in your journey with Pearl.</v>
       </c>
       <c r="F10" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-central-de-abastos-cdmx-iztapalapa-en-iztapalapa-001D869701974DF161373E686DCF3405#lc=ListOffers-Score4-8</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-sales-team-lead-en-chihuahua-F67F7246DC04C0EC61373E686DCF3405#lc=ListOffers-Score3-8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Barrendero con turno fijo en la tarde - En Central de Abastos Iztapalapa</v>
+        <v>Account Manager / Customer Success Representative</v>
       </c>
       <c r="B11" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Pearl Talent</v>
       </c>
       <c r="C11" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Chihuahua, Chihuahua</v>
       </c>
       <c r="D11" t="str">
-        <v>$ 10,000.00</v>
+        <v>$5</v>
       </c>
       <c r="E11" t="str">
-        <v>Importante empresa dedicada al sector limpieza solicita Barrendero.Requisitos:- Mayor de 18 años- Experiencia no necesariaOfrecemos:- $8,000 mensuales netos (Pago semanal)- Prestaciones de ley- Trabajo de Lunes a Domingo con 1 descanso en la semana- Horario de 10:00 am a 7:00 pmZona de trabajo: Central de Abastos Iztapalapa.Actividades : acompañamiento de camionesLevantar basura de cajones de tolvaLevantar basura que cae de los camiones al momento de la cargaLevantar basura al paso del recorridoInteresados que cuenten con documentos (Acta de nacimiento, Cuenta de Banco, Comprobante de domicilio, INE, CURP, IMSS, RFC) postularse por éste medio, y un ejecutivo te contactará por whatsapp.</v>
+        <v>DescriptionJob Type: Full-time (40 hours/week)Salary Range: based on experience, with performance-based bonuses.Work Schedule: Monday to Friday, ideally 9:00 AM – 6:00 PM ESTLocations: Remote — candidates must be in EST or have 4+ hours overlapAbout Pearl TalentPearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Hear why we exist, what we believe in, and who we’re building for:Why Work with Us?We’re not just another recruiting firm—we focus on placing candidates with exceptional US and EU founders who prioritize the long-term success of their team members. We also provide retention bonuses at 3, 6, 9, and 12 months, as well as community-driven benefits like an annual retreat.About the CompanyThe company is a fast-growing, design-driven startup at the intersection of social commerce and mobile tech. Backed by strong early traction, they empower creators to express their personal style through a visually rich, community-first experience. The team moves fast, values clean design and code, and gives every collaborator a visible impact on product direction.Role OverviewWe’re seeking a Latin America-based high-performing Account Manager / Customer Success Representative to scale the vendor experience and build white-glove relationships with clients. This role is instrumental in owning post-sale success, ensuring long-term client happiness, and identifying growth and referral opportunities across an expanding network of clients and connectors.You will be the key custodian of the client experience—building trust, capturing feedback, anticipating issues, and driving value for every vendor you support.Key ResponsibilitiesOwn and manage post-sale relationships with 20–30 vendor accountsBuild detailed onboarding plans, SOPs, and CRM documentation (HubSpot, Notion, etc.)Conduct structured onboarding and re-onboarding processes that feel personalized and eliteCapture and maintain detailed vendor insights—understanding their needs, tone, and preferencesAct as the internal voice of the vendor, surfacing feedback and performance blockers to product and connector teamsRun regular check-ins, collect NPS, initiate feedback loops, and subtly request referralsEnsure vendors receive immediate value through prompt matching with active connectorsTrack all account data, performance metrics, and interaction notes in HubSpot and internal dashboardsAssist with referral generation or upsell motions as appropriateSupport events and community initiatives (e.g., founder dinners, intro strategy planning)Collaborate with Connector Success teammates to align vendors with ideal connector profilesRequirementsMust-Have:Flawless written and verbal EnglishFamiliarity with HubSpotStrong multitasking skills—capable of managing 20–30 relationships concurrentlyExtreme attention to detail, particularly with CRM data, call notes, and context trackingPolished, warm, and professionally presentable for a client-facing roleHighly organized, self-managing, and emotionally intelligentNice-to-Have:Background in B2B customer success, partnerships, or account managementExperience supporting startups, SaaS platforms, or relationship-driven tech businessesExposure to the startup community, founder ecosystem, or high-end networking circlesFamiliarity with OpenPhone or similar VoIP toolsPassion for human-centric products or servicesExperience working in remote, asynchronous, fast-moving environmentsTools &amp; Communication Channels:CRM: HubSpot, SalesforceDialers: OpenPhoneMessaging: Slack, ZoomDocumentation: Notion, Google DocsScheduling: Calendly, Google CalendarBenefitsCompensation PackageCompetitive Salary: Based on experience and skillsRemote Work: Fully remote—work from anywhereGenerous PTO: Ample paid time off to rest and rechargeHealth Coverage: HMO coverage after 3 months for full-time employeesDirect Mentorship: Grow through guidance from international industry expertsLearning &amp; Development: Ongoing access to resources for professional growthGlobal Networking: Work and connect with professionals around the worldWork-Life Balance: Flexible hours that support a healthy work-life balanceOur Recruitment ProcessApplicationScreeningTop-grading InterviewSkills AssessmentClient InterviewJob OfferClient OnboardingReady to Join Us?If this role aligns with your skills and career goals, we’d love to hear from you. Apply now to take the next step in your journey with Pearl.</v>
       </c>
       <c r="F11" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-con-turno-fijo-en-la-tarde-en-central-de-abastos-iztapalapa-en-iztapalapa-33BD941F42C610F461373E686DCF3405#lc=ListOffers-Score4-9</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-account-manager-customer-success-representative-en-chihuahua-4E60B347562C819161373E686DCF3405#lc=ListOffers-Score3-9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Barrendero Nocturno - En Central de Abastos Iztapalapa</v>
+        <v>Developer Front End</v>
       </c>
       <c r="B12" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Importante empresa del sector</v>
       </c>
       <c r="C12" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
       </c>
       <c r="D12" t="str">
-        <v>$ 10,000.00</v>
+        <v>$ 25,000.00</v>
       </c>
       <c r="E12" t="str">
-        <v>Importante empresa dedicada al sector limpieza solicita Barrendero para el turno Nocturno.Requisitos:- Mayor de 18 años- Experiencia no necesariaOfrecemos:- $10,000 mensuales netos (Pago semanal)- Prestaciones de ley- Trabajo de Lunes a Domingo con 1 descanso en la semana- Horario de 5:00 pm a 5:00 amZona de trabajo: Central de Abastos Iztapalapa.Actividades : acompañamiento de camionesLevantar basura de cajones de tolvaLevantar basura que cae de los camiones al momento de la cargaLevantar basura al paso del recorridoInteresados que cuenten con documentos (Acta de nacimiento, Cuenta de Banco, Comprobante de domicilio, INE, CURP, IMSS, RFC) postularse por éste medio, y un ejecutivo te contactará por whatsapp.</v>
+        <v>Intégrate a una empresa con más de 35 años en el mercado, genera estabilidad y crecimiento profesional como: Developer FrontEnd.Descripción del PuestoEl desarrollador frontend se encarga de crear la interfaz de un sitio web o aplicación a través de código Para este proyecto el candidato debe de contar con el conocimiento necesario para poder darle mantenimiento a una aplicación web desarrollada en Angular 7.Actividades Principales1: Brindar la atención a los usuarios que presenten incidencias en el uso de la plataforma para resolver dichas incidencias2: Mantener Actualizados las librerías utilizadas por las diversas plataformas Web3: Mantener Actualizadas las diversas versiones sobre las cuales están construidas las plataformas como por ejemplo Versiones de Angular, Versiones de Firebase 4:Robustecer la seguridad actual de las aplicaciones por medio de ofuscamiento de código, implementación de tokens de Seguridad, encriptación de la información, y Best Practices que recomienda Google.5: Optimizar los procesos que hoy se tienen implementados que están más propensos a sufrir fallas, como por ejemplo la sincronización de información6: Elaboración de pruebas unitarias para robustecer la calidad de las plataformas, Mobile7: Modificaciones en la arquitectura de las aplicaciones que nos permita tener modularidad8: Robustecer la Aplicación Web para evitar errores en la captura de información. 9:Robustecer la calidad de la información que se registra dentro de la base de datos mediante puntos de control.Skills TécnicasRequerido: Angular, Observables, RXJS, NgZorro, Bootstrap, HTML%, CSS, Firebase DataBase, Firebase Cloud Functions, React.JS, Next.JSDeseable: Firebase Hosting, REDUXOfrecemos:Lunes a Viernes de 9:00 a 6:00Zona Polanco en un esquema HíbridoSueldo base neto $30,000 neto al mes + prestaciones de ley</v>
       </c>
       <c r="F12" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrendero-nocturno-en-central-de-abastos-iztapalapa-en-iztapalapa-0F3EFD8ABAA464EE61373E686DCF3405#lc=ListOffers-Score4-10</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-developer-front-end-en-miguel-hidalgo-9014778E2FE3818161373E686DCF3405#lc=ListOffers-Score3-10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Barrenderos / $2,000 a la semana Central de Abastos CDMX</v>
+        <v>Full Stack Mobile Developer</v>
       </c>
       <c r="B13" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Pearl Talent</v>
       </c>
       <c r="C13" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Argentina</v>
       </c>
       <c r="D13" t="str">
-        <v>$2,000</v>
+        <v>$5</v>
       </c>
       <c r="E13" t="str">
-        <v>SOLICITAMOS POR EXPANSION: BARRENDEROSZONA: IZTAPALAPA (CENTRAL DE ABASTOS)SUELDO $2,000 semanales libresPagos semanalesContarás con Prestaciones de LeyHorario: 9:00 am a 6:00 pmLunes a Domingo, 1 día de descanso entre semana</v>
+        <v>DescriptionWork Arrangement: Fully remote, overlapping EST working hours.Job Type: Full-timeSalary Range: based on experience, with performance-based bonuses.Work Schedule: 40 hours per week, with core hours between 10 AM – 6 PM EST (flexible based on sprint deadlines).Locations: Remote, open to candidates globally.About Pearl TalentPearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Hear why we exist, what we believe in, and who we’re building for:Why Work with Us?We’re not just another recruiting firm—we focus on placing candidates with exceptional US and EU founders who prioritize the long-term success of their team members. We also provide retention bonuses at 3, 6, 9, and 12 months, as well as community-driven benefits like an annual retreat.About the CompanyThe company is a fast-growing, design-driven startup at the intersection of social commerce and mobile tech. Backed by strong early traction, they empower creators to express their personal style through a visually rich, community-first experience. The team moves fast, values clean design and code, and gives every engineer a visible impact on product direction.Role OverviewAs a Flutter Full Stack Mobile Engineer, you’ll be responsible for building and maintaining a high-performance mobile app using Flutter and Firebase. You’ll implement UI based on Figma designs, manage backend services with Firebase (Firestore, Auth, Cloud Functions), and contribute across the full development cycle—from feature development to deployment and maintenance. This is a key role for someone who thrives in fast-paced environments and values both technical quality and user experience.Key ResponsibilitiesFront-End Development:Own the Flutter mobile app end to end; implement sleek, responsive UI aligned with the platform’s design vision.Translate Figma designs into clean, maintainable Dart code with pixel-level precision.Work closely with product and design teams to iterate quickly on user-facing features.Back-End Development:Manage all Firebase services, including Firestore, Cloud Functions, Auth, and Storage.Optimize database structure and queries for performance and scalability.Implement secure serverless functions for key operations like permissions and user interactions.Deployment &amp; QA:Maintain a clean codebase with proper version control, CI/CD pipelines (e.g., Bitrise or GitHub Actions), and testing standards.Lead debugging, performance monitoring, and ensure stable releases to iOS and Android.Cross-functional Collaboration:Collaborate with product and design stakeholders to align on priorities and technical feasibility.Help translate feature ideas into actionable development plans.RequirementsMust-Have:5+ years professional experience in Flutter &amp; Firebase stackStrong understanding of asynchronous Dart programming, widget lifecycle, and state management (e.g., Bloc, Riverpod)Hands-on experience with Firebase: Firestore, Functions, Auth, Cloud StorageClean, maintainable, modular coding habitsStartup-minded: comfortable with ambiguity, self-directed, fast iteration cyclesExcellent communication and remote collaboration skillsNice-to-Have:Prior experience in social apps, eCommerce, or creator toolsBackground in UI/UX design or strong appreciation for design systemsFamiliarity with App Store &amp; Play Store deploymentExperience integrating third-party APIs (e.g., Shopify, Instagram, Stripe)BenefitsCompensation PackageCompetitive Salary: Based on experience and skillsRemote Work: Fully remote—work from anywhereGenerous PTO: Ample paid time off to rest and rechargeHealth Coverage: HMO coverage after 3 months for full-time employeesDirect Mentorship: Grow through guidance from international industry expertsLearning &amp; Development: Ongoing access to resources for professional growthGlobal Networking: Work and connect with professionals around the worldWork-Life Balance: Flexible hours that support a healthy work-life balanceOur Recruitment ProcessApplicationScreeningTop-grading InterviewSkills AssessmentClient InterviewJob OfferClient OnboardingReady to Join Us?If this role aligns with your skills and career goals, we’d love to hear from you. Apply now to take the next step in your journey with Pearl.</v>
       </c>
       <c r="F13" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-barrenderos-2000-a-la-semana-central-de-abastos-cdmx-en-iztapalapa-75FC0F398FF27B2C61373E686DCF3405#lc=ListOffers-Score4-11</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-full-stack-mobile-developer-en-argentina-3D05C6B6A8BAD64161373E686DCF3405#lc=ListOffers-Score3-11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Auxiliar limpieza - Central de Abastos</v>
+        <v>Patient Care Scheduler</v>
       </c>
       <c r="B14" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Pearl Talent</v>
       </c>
       <c r="C14" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Chihuahua, Chihuahua</v>
       </c>
       <c r="D14" t="str">
-        <v>$ 8,000.00</v>
+        <v>$ 26,600.00</v>
       </c>
       <c r="E14" t="str">
-        <v>Estamos en búsqueda de tu talento como:TENEMOS DISPONIBLES 2 VACANTES DE AUXILIAR DE LIMPIEZA:BARRENDEROTurno: Nocturno (De 6:00PM a 6:00AM)Sueldo: $10,000 mensualesBARRENDEROTurno: Vespertino (De 10:00AM a 7:00AM)Sueldo: $8,000 mensuales¡NO NECESITAS EXPERIENCIA! - INGRESO INMEDIATOSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>DescriptionJob Position: Patient Care Scheduler (Provider Liaison)Work Arrangement: Fully Remote – Based in the Philippines or LATAMJob Type: Full-time, Independent ContractorWork Schedule: Monday–Friday, 9:00 AM to 6:00 PM Eastern TimeAbout Pearl Talent:Pearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Hear why we exist, what we believe in, and who we’re building for:Why Work with Us?We’re not just another recruiting firm—we focus on placing candidates with exceptional US and EU founders who prioritize the long-term success of their team members. We also provide retention bonuses at 3, 6, 9, and 12 months, as well as community-driven benefits like an annual retreat.About the CompanyOur client is a U.S.-based healthcare organization focused on increasing access to life-saving medications for patients with chronic conditions. They partner with leading hospitals, pharmacies, and healthcare providers across the U.S. to simplify the patient care process and ensure timely, affordable treatment.We’re looking for a Patient Care Scheduler to support our rapidly growing provider network. This is a mission-driven role ideal for someone who is organized, persistent, and passionate about creating better health outcomes.Role Overview:As a Provider Liaison &amp; Scheduler, you’ll be responsible for coordinating with healthcare providers and pharmacies to secure signed Collaborative Practice Agreements (CPAs) and schedule clinical consultations between patients and pharmacists. You’ll handle high-volume outreach, document communications in our CRM system, and ensure patients move efficiently through the scheduling process.This role is ideal for someone with a healthcare coordination background, strong communication skills, and the ability to follow through across multi-step processes.Purpose of Your RoleTo ensure that every patient referred into our program can quickly access the clinical care they need—by securing CPA signatures from providers and efficiently scheduling consultations. You’ll streamline the path between physician, pharmacist, and patient, directly improving patient access and care timelines.Requirements1. Provider Outreach &amp; CPA CoordinationReach out to physician offices via phone, email, and online fax to introduce and secure CPAsExplain the purpose and process of CPAs to medical staffPersistently follow up on unsigned agreements using standardized scripts and sequencesAccurately log all communication and document status in the CRM2. Patient Scheduling SupportOnce CPAs are secured, schedule patients for consultations with pharmacy partnersCoordinate schedules between patients and clinical teamsConfirm and document all appointments, reschedules, and follow-ups3. Data Management &amp; ReportingMaintain clean, up-to-date CRM records for every provider and patient caseIdentify and escalate unresponsive or rejecting providers to U.S. teamSubmit weekly activity and performance reports to the operations team4. Workflow Optimization (Growth Opportunity)Proactively identify bottlenecks or inefficiencies in outreach and scheduling processesRecommend improvements or new SOPs to streamline operationsCollaborate with other schedulers (as the team grows) to share learnings and best practicesPreferred Experience1–2+ years in U.S. healthcare operations, patient coordination, or provider support rolesProven experience speaking with physicians, clinic staff, or healthcare providersFamiliar with CRMs (e.g., Telescope), online fax tools, Google Sheets, and remote collaboration tools like Slack and WhatsAppPast experience working with U.S.-based teams in a fully remote roleKey Skills &amp; AttributesClear, confident communicator – able to explain complex workflows to medical professionalsPersistent and detail-oriented – follows up thoroughly and tracks progress accuratelyCritical thinker – makes suggestions to improve processes and flag issuesIndependent and proactive – thrives in a remote setting with minimal hand-holdingBilingual (Spanish a plus) – many patients prefer or benefit from Spanish-speaking supportBenefitsPotential for profit share based on performanceFully WFH, foreverAnnual team retreatUnlimited PTOPotential Growth OpportunitiesOur Recruitment Process:ApplicationScreeningSkills AssessmentTop-grading InterviewFinal InterviewJob OfferOnboardingReady to Join Us?If this role aligns with your skills and career goals, we’d love to hear from you. Apply now to take the next step in your journey with Pearl.</v>
       </c>
       <c r="F14" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-limpieza-central-de-abastos-en-iztapalapa-37C5E76C32BA148461373E686DCF3405#lc=ListOffers-Score3-12</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-patient-care-scheduler-en-chihuahua-8DCD27C2FD0C59D261373E686DCF3405#lc=ListOffers-Score3-12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Auxiliar de Limpieza sin Experiencia para Iztapalapa Turno Nocturno - $10,000 mensual Contratación el mismo dia</v>
+        <v>Customer Service Manager</v>
       </c>
       <c r="B15" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Human Quality.</v>
       </c>
       <c r="C15" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Monterrey, Nuevo León</v>
       </c>
       <c r="D15" t="str">
-        <v>$10,000</v>
+        <v>$ 30,000.00</v>
       </c>
       <c r="E15" t="str">
-        <v>"Importante marca de Limpieza está en busca de tu talento"Solicita Axiliar de limpieza (Barrendero) sin ExperienciaRequisitos:Tener disponibilidad de HorarioBuena ActitudLunes a Domingo con descanso entre semanaEdad: entre 18 a 55 añosNo contar con Infonavit de preferenciaSin tatuajes o perforaciones de preferenciaZona de trabajo: IztapalapaOFRECEMOS:Sueldo base Neto semana $2500 semanalNocturno 5pm a 5am $2500 semanalesPago SemanalVacante FijaSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>We’re Hiring: Customer Service Manager | Monterrey, NLDo you speak logistics? Are you the kind of leader who turns challenges into opportunities while keeping customers delighted? Then this might be your next big move.We’re looking for a Customer Service Manager who leads with passion, energy, and a sense of humor. Someone who thrives in the fast-paced logistics world, builds high-performing teams, and makes customer satisfaction a personal mission.Location: Monterrey, Nuevo LeónPosition Type: Full-time with superior benefitsSalary: Competitive salary + Performance bonusKey Responsibilities:Lead, coach, and inspire the customer service team.Maintain smooth communication between customers, account managers, and operations teams.Conduct business reviews to identify growth opportunities.Develop and implement SOPs with customers and the Quality team.Monitor KPIs to ensure on-time performance.Promote a positive and solutions-focused work environment.Requirements:Bilingual: English/Spanish – required.Valid U.S. visa and passport – must be available to travel.Bachelor’s degree and 3 years of experience in logistics, or 5 years of solid industry experience.Minimum 1 year of experience leading teams.Excellent problem-solving and interpersonal skills.Bonus points if you’re familiar with AS400, McLeod, or CTPAT.If you’re ready to lead with purpose, connect with people, and make things happen, we’d love to meet you.</v>
       </c>
       <c r="F15" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-de-limpieza-sin-experiencia-para-iztapalapa-turno-nocturno-10000-mensual-contratacion-el-mismo-dia-en-iztapalapa-F37FE05104C1EFD961373E686DCF3405#lc=ListOffers-Score3-13</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-customer-service-manager-en-monterrey-B5549FC52699318D61373E686DCF3405#lc=ListOffers-Score3-13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Auxiliar de Limpieza sin Experiencia para Iztapalapa Turno Intermedio - $8000 mensual Contratación el mismo dia</v>
+        <v>Real Estate Expansion and Market Analyst</v>
       </c>
       <c r="B16" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Pearl Talent</v>
       </c>
       <c r="C16" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Puerto Rico</v>
       </c>
       <c r="D16" t="str">
-        <v>$8000</v>
+        <v>$5</v>
       </c>
       <c r="E16" t="str">
-        <v>"Importante marca de Limpieza está en busca de tu talento"Solicita Axiliar de limpieza (Barrendero) sin ExperienciaRequisitos:Tener disponibilidad de HorarioBuena ActitudLunes a Domingo con descanso entre semana 10 am a 7pmEdad: entre 18 a 55 añosNo contar con Infonavit de preferenciaSin tatuajes o perforaciones de preferenciaZona de trabajo: IztapalapaOFRECEMOS:Sueldo base Neto semanal $2000 semanalIntermedio 10am a 7pm $2000 semanalesPago SemanalVacante FijaSi estas interesada/o postúlate con tu CV actualizado</v>
+        <v>DescriptionAbout Pearl TalentPearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Hear why we exist, what we believe in, and who we’re building for:Why Work with Us?We’re not just another recruiting firm—we focus on placing candidates with exceptional US and EU founders who prioritize the long-term success of their team members. We also provide retention bonuses at 3, 6, 9, and 12 months, as well as community-driven benefits like an annual retreat.About the CompanyWe are seeking a highly analytical and proactive Market Research Analyst, rapidly growing real estate development company based in Florida. This role is ideal forsomeone with strong research capabilities, data analysis skills, and the ability to identifyemerging market opportunities before the competition. You will work directly with seniorleadership to provide critical market intelligence that drives multi-million dollarinvestment decisions.RequirementsProven background in market research, data analysis, or real estate industryexperienceAdvanced Excel skills with ability to analyze large datasets and identify trendsExperience gathering information from government databases, public records, and industry sourcesPreferred: Background in real estate, urban planning, economic development, or related fieldsBonus: Familiarity with Florida markets, municipal planning processes, or GIS/mapping softwareDemonstrated ability to synthesize complex research into clear, actionable insightsExperience creating presentations and reports for executive decision-makingComfort with learning new software platforms and database management systemsKey Responsibilities:Monitor Department of Transportation infrastructure plans (road expansions, newinterchanges, highway upgrades)Monitor Department of Economic Development budgeting plans and targetingindustry growth sectors &amp; expansions effortsTrack population migration trends, demographic shifts, and employment growth patternsIdentify new commercial developments, major retailer expansions, and industrial projectsCreate and maintain centralized market intelligence database with automated tracking systemsDevelop systematic processes for consistent market monitoring across multiple Florida marketsBuild relationships with targeted brokers to identify land opportunities – finding and keeping track of upcoming events for land acquisition team to attend (i.e builder events, broker events)Support creation of compelling market presentations for builder pitches and investor meetingsDevelop an on-going Google notification system to keep tabs of development, infrastructure, and employment hubs article coverage.Generate bi-weekly snapshots of findings, highlighting the analytics or development pipeline which makes the market a target.Not meant to be an overloaded report of data but more with interpretation &amp; guidanceConduct a search on national home builder &amp; broker meet-ups.Large conferences to small gatheringsBenefitsCompetitive Salary: Up to $1,500 per month, based on experience and skillsRemote Work: Fully remote—work from anywhereGenerous PTO: 10 days PTO per year, plus public US holidaysDirect Mentorship: Grow through guidance from international industry expertsLearning &amp; Development: Ongoing access to resources for professional growthGlobal Networking: Work and connect with professionals around the worldWork-Life Balance: Balanced schedule that supports a healthy work-life balance.Our Recruitment Process:ApplicationScreeningTop-grading InterviewSkills AssessmentClient InterviewJob OfferClient OnboardingReady to Join Us?If this role aligns with your skills and career goals, we'd love to hear from you. Apply now to take the next step in your journey with Pearl.</v>
       </c>
       <c r="F16" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliar-de-limpieza-sin-experiencia-para-iztapalapa-turno-intermedio-8000-mensual-contratacion-el-mismo-dia-en-iztapalapa-21DBF84AE98E8B6161373E686DCF3405#lc=ListOffers-Score3-14</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-real-estate-expansion-and-market-analyst-en-puerto-rico-22259E07DDB14C5661373E686DCF3405#lc=ListOffers-Score3-14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Auxiliares de limpieza contratación inmediata - Iztapalapa Central de abastos</v>
+        <v>Asesor Telefonico - Experiencia en Productos Financieros</v>
       </c>
       <c r="B17" t="str">
-        <v>Idea Market Solutions</v>
+        <v>Hogares Union</v>
       </c>
       <c r="C17" t="str">
-        <v>Iztapalapa, Ciudad de México DF</v>
+        <v>Cuajimalpa de Morelos, Ciudad de México DF</v>
       </c>
       <c r="D17" t="str">
-        <v>$ 10,000.00</v>
+        <v>$ 24,999</v>
       </c>
       <c r="E17" t="str">
-        <v>Importante empresa de residuos está en busca de tu talentoSolicitamos personal de limpieza (diversas áreas)BarrenderosAuxiliares de limpieza de pasillosLavadores de camionesZONA IZTAPALAPAOFRECEMOS:Sueldo semanal (dependiendo de la posición)Horario dependiendo de la operaciónPagos semanalesRequisitos:Disponibilidad de horarioExperiencia no necesaria o mínimaZona de trabajoCENTRAL DE ABASTOS IZTAPALAPASi estas interesada/o postúlate con tu CV actualizado o marca al 5580109495</v>
+        <v>Vacante: Asesor Telefónico con Experiencia en Productos FinancierosDepartamento: Engagement CenterUbicación: Santa Fe CorporativoModalidad: PresencialHorario: Lunes a viernes de 9:00 a.m. a 7:00 p.m., con una hora y media para comer. Contamos con comedor subsidiado al 75%.Descripción del puesto:En Hogares Unión, empresa líder en desarrollos inmobiliarios, buscamos personas con experiencia en ventas telefónicas de productos financieros (créditos, seguros, tarjetas de crédito, etc.) para integrarse a nuestro equipo como Asesor Telefónico. Este rol es clave para contactar, calificar y canalizar prospectos interesados en adquirir una vivienda, brindando una atención profesional y orientada al cierre.Que harás en este puesto:Contactar a prospectos interesados en adquirir una vivienda a través de nuestros canales digitalesDetectar necesidades financieras del cliente y orientar sobre productos hipotecarios disponiblesCalificar prospectos con base en criterios financieros y canalizarlos al equipo comercialRegistrar y actualizar información en el sistema CRMAsegurar una atención telefónica profesional, empática y enfocada en resultadosRequisitos indispensables:Experiencia mínima de 1 año en ventas telefónicas de productos financieros, como:Créditos personales o hipotecariosTarjetas de créditoSeguros (vida, auto, gastos médicos)Servicios financieros bancarios o fintechBachillerato concluido (comprobable)Facilidad de palabra, enfoque comercial y excelente actitud de servicioManejo de PC y herramientas digitalesDisponibilidad para trabajar en el horario establecidoOfrecemos:Sueldo base competitivoComisiones atractivas sin topeIngreso promedio mensual entre 16,000 y 20,000 pesosCapacitación pagadaOportunidad de crecimiento y desarrollo profesionalExcelente ambiente laboralBeneficios adicionales:BienestarTotal Pass: Acceso a mas de 450 gimnasios sin inscripcion ni anualidadLaboratorio Medico Polanco: 40 por ciento de descuento en analisis clinicos y de gabineteEntretenimientoPaquetes de viaje: Playas mexicanas (3 dias y 2 noches), pagos hasta en 36 quincenasAcuario Inbursa: 15 por ciento de descuento en entradas y fotosTicketmaster: 20 a 50 por ciento de descuento en conciertos, obras y mercanciaSix Flags y Hurricane Harbor: Descuentos preferencialesKataplum: 15 por ciento de descuento en efectivo, 10 por ciento con tarjetaDescuentos en campamentos de verano y fiestas infantilesEducaciónOpen English y NextU: 70 por ciento de descuento en idiomas y cursos digitalesUniversidad Tres Culturas:Examen de admisión sin costo10 por ciento en colegiaturas y acreditaciónBeneficio extensivo a familiares directosUniversidad ICEL:20 a 30 por ciento en preparatoria20 a 40 por ciento en carreras ejecutivas y maestrías (requiere promedio mínimo de 80)Sobre nosotros:En Hogares Unión, somos una empresa 100 por ciento mexicana con mas de 45 años de experiencia desarrollando comunidades y construyendo hogares.Nos especializamos en ofrecer soluciones habitacionales accesibles, funcionales y de calidad.¿Te interesa formar parte de un equipo que transforma vidas?Postúlate y ayúdanos a seguir construyendo el futuro de miles de familias mexicanas.</v>
       </c>
       <c r="F17" t="str">
-        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-auxiliares-de-limpieza-contratacion-inmediata-iztapalapa-central-de-abastos-en-iztapalapa-65BB4A5C627E4E3761373E686DCF3405#lc=ListOffers-Score3-15</v>
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-asesor-telefonico-experiencia-en-productos-financieros-en-cuajimalpa-de-morelos-223553C5AEF6A63361373E686DCF3405#lc=ListOffers-Score3-15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Corporate Talent Acquisition Manager - Gerente Reclutamiento</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Importante empresa del sector</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Mérida, Yucatán</v>
+      </c>
+      <c r="D18" t="str">
+        <v>$ 60,000.00</v>
+      </c>
+      <c r="E18" t="str">
+        <v># Gerente de Reclutamiento# Gerente de Atracción de TalentoCorporate Talent Acquisition ManagerLocation: Mérida, YucatánConfidential AAA CompanyFull-time | On-site with international interactionAre you passionate about attracting top talent in a fast-paced and constantly evolving environment?We are looking for a strategic, results-driven, and dynamic Corporate Talent Acquisition Manager to lead, standardize, and elevate our recruitment processes globally.The ideal candidate has solid experience in large multinational organizations and thrives in environments of transformation and growth.Key Responsibilities:Ensure timely and high-quality fulfillment of operational, entry-level, middle management, senior management, and C-level roles to meet short-, mid-, and long-term business growth goals.Design, implement, and standardize best-in-class talent acquisition strategies across all levels and business units.Lead and coach a team of recruiters, ensuring alignment with KPIs and continuous development.Conduct behavioral interviews using STAR methodology (Manager &amp; team).Build and maintain strong relationships with stakeholders and hiring managers across different countries and business units.Manage and optimize modern recruitment tools and platforms:ATS systems: Greenhouse, Lever, SmartRecruiters, SAP SuccessFactors, etc.Sourcing tools: LinkedIn Recruiter, Boolean Search, Talent Pools, headhunting techniques, and social media recruiting.Employer Branding: EVP development, inbound recruiting, market mapping.Collaborate with external recruitment vendors and partners.Oversee recruitment processes within Shared Services structures.Manage IT recruitment needs (developers, programmers, infrastructure, and networks).Apply and interpret psychometric and technical assessments.Deliver accurate, data-driven reports using Excel. Analyze recruitment metrics and generate executive dashboards for continuous improvement and strategic decision-making.Monitor and improve candidate experience throughout the hiring lifecycle.Drive initiatives to enhance employer brand positioning and talent market penetration.Contribute to broader organizational projects such as growth strategies, international expansions, and change management initiatives.Requirements:Bachelor's degree in Psychology, Business Administration, or a related field (required).Advanced English (oral and written B2+) – mandatory assessment.Relevant HR certifications or postgraduate studies in Human Resources (preferred).Minimum 5 years of experience leading talent acquisition in large corporations with 5,000+ employees globally.Proven track record of hiring across all levels, including international and multicultural environments.Experience working directly with HR Directors or as part of corporate HR leadership.Solid understanding of recruitment for IT and technical roles.Comfortable working in environments of constant change, growth, mergers, or restructures.Strong stakeholder management, organizational skills, and execution capacity.Data-driven mindset with a strong focus on results and continuous improvement.Excellent professional ethics, collaboration spirit, urgency, and adaptability.Intermediate/advanced Excel.We Offer:Join a top-tier international organization with a strong reputation and growth trajectory.Collaborative and agile work culture.Clear career development opportunities.Competitive compensation package aligned with experience and performance.Key KPIs:Time-to-fill for critical and key positions.Quality of hires (based on onboarding feedback and performance evaluations).Recruitment process adoption and compliance across regions.Employer brand development and market recognition in target talent pools.Percentage of total approved headcount filled.If you meet the above qualifications and are excited to take your career to the next level, apply now. All applications will be treated with strict confidentiality.Only candidates meeting the full criteria will be considered.</v>
+      </c>
+      <c r="F18" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-corporate-talent-acquisition-manager-en-merida-C9CEF22324C60C6161373E686DCF3405#lc=ListOffers-Score3-16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Growth Optimization Lead - CRO and Marketing Automation</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Go Bravo</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D19" t="str">
+        <v>$ 40,000.00</v>
+      </c>
+      <c r="E19" t="str">
+        <v>About Bravo:Bravo is a fintech company with 15 years of experience helping people in Latin America and Europe improve their financial health. With operations in 6 countries and a strong acquisition engine, we are committed to innovation, scale, and impact. Were now looking for someone to take conversion and lead nurturing to the next level.Role Overview:Were looking for a strategic and analytical Growth Optimization Lead who can drive impact across two critical areas: Conversion Rate Optimization (CRO) and Marketing Automation. Youll be responsible for improving lead-to-client conversion by optimizing our web funnel and boosting our automation flows to move leads down the funnel efficiently. You wont be aloneyoull lead through collaboration with two highly capable teammates:Aldo, our technical CRO implementer (web development, tracking, events)Marcos, who leads marketing automation across all countriesThis is not a design or UI role. You wont manage designers or be responsible for visual assets. This is a data-informed, performance-driven, execution-focused role.Key Responsibilities:Own and lead the CRO roadmap: prioritize tests and improvements to landing pages and formsWork closely with Aldo to implement A/B tests, tracking, and performance enhancementsCollaborate with product and engineering to unlock improvements (site speed, UX bugs, event tracking)Identify and launch marketing automation opportunities (lead scoring, nurturing, email journeys, WhatsApp flows)Coordinate with Marcos to improve lead conversion through automation, especially in Mexico and potentially ColombiaTrack performance KPIs: conversion rate, open rate, click-through rate, cost per qualified leadBring an experimental mindsetrun and learn from data-driven experimentsAct as a bridge between marketing, tech, and product to keep growth priorities alignedWhat Were Looking For:36 years of experience in digital growth, CRO, marketing automation, or product growthStrong understanding of landing page best practices, tracking, and A/B testing tools (GA4, GTM, Hotjar, Optimize, etc.)Experience working with email/CRM tools like Iterable, Braze, HubSpot, or similarAnalytical mindset with ability to extract actionable insights from performance dataExcellent project management and prioritization skillsAbility to work cross-functionally with developers, marketers, and product teamsBonus: Experience in fintech, financial services, or lead generation companiesBonus: SQL or light technical background (not required but valued)What We Offer:The opportunity to lead high-impact projects across key growth leversA collaborative, high-performance culture that values ownership and experimentationCareer path growth opportunitiesCompetitive salary and benefitsHybrid work environment (some on-site presence in Mexico City required)</v>
+      </c>
+      <c r="F19" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-growth-optimization-lead-cro-and-marketing-automation-en-miguel-hidalgo-8A0A7155ECC9F3F561373E686DCF3405#lc=ListOffers-Score3-17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Night Shift Technical Support Agent (Bilingual) - MXN 19K Salary</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Importante empresa del sector</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D20" t="str">
+        <v>$ 16,000.00</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Night Owl Opportunity: Tier 1 Technical Support Agent (Overnight Shift)Are you ready to become part of a thriving corporate environment with an international scope? GlobalTech Corporation, a leader in providing technological solutions for the U.S. tax sector, is looking for dedicated professionals for our Tier 1 Technical Support team. This role focuses on delivering exceptional service and resolving technical incidents for our corporate clients.Your Role and Responsibilities:• Provide first-level technical support and resolve incidents remotely.• Accurately log all case details in our ticketing system.• Ensure timely follow-up on service requests and escalate complex problems when necessary.• Maintain a clear, professional, and solution-driven user experience for all clients.• Collaborate effectively with cross-functional technical and operational teams.Ideal Candidate Profile:• Education: High school diploma (minimum); a Bachelor's degree or technical certification is preferred.• Language: Advanced English (C1 level is essential).• Experience: Minimum of 6 months to 1 year of proven experience in technical support or customer service.• Technical Skills: Basic knowledge of ticketing platforms, remote support tools, and various digital applications.• Key Skills: Strong communication, organizational, and customer-centric abilities.• Work Schedule: Availability to work Monday to Friday, from 12:00 AM to 7:00 AM (Overnight Shift).Benefits &amp; Compensation:• Comprehensive Monthly Salary: $19,000 MXN (night bonus already included).• Direct Hire: Immediate direct hiring by GlobalTech Corporation.• Training: Full initial technical training provided to ensure your success.• Stability &amp; Growth: Enjoy job stability with clear opportunities for professional advancement.• Work Environment: A supportive and excellent work environment.• Payment: Punctual bi-weekly payments.Work Location:• Alcaldía Miguel Hidalgo, CDMX• Modality: On-site.• Availability: Immediate.Take the next step in your tech career. Apply for our Overnight Support role!</v>
+      </c>
+      <c r="F20" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-night-shift-technical-support-agent-bilingual-mxn-19k-salary-en-miguel-hidalgo-97989574325DEC5661373E686DCF3405#lc=ListOffers-Score3-18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Desarollador FullStack - Sr</v>
+      </c>
+      <c r="B21" t="str">
+        <v>AVASA</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Mérida, Yucatán</v>
+      </c>
+      <c r="D21" t="str">
+        <v>$ 11,239</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Buscamos sumarte a nuestro equipo de trabajo, para desarrollarte como:DESARROLLADOR FULLSTACKOfrecemos:-Atractivo sueldo acorde a aptitudes-Prestaciones de ley (inmediatas)-Beneficios internos-Oportunidades de desarrollo y crecimientoFunciones:-Diseño y desarrollo de aplicaciones web (Next.js)-Implementar y mantener APis y servicios backend en Node,js-Code reviews-Colaborar con el product ownerImportante-Experiencia mínima 5 años-Disponibilidad para trabajar presencialmente</v>
+      </c>
+      <c r="F21" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarollador-fullstack-sr-en-merida-42BA7ED74045742861373E686DCF3405#lc=ListOffers-Score3-19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Remote Senior Frontend Dev - React Native (Mobile or Web)</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Vivian Vazquez Recruitment</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Querétaro, Querétaro</v>
+      </c>
+      <c r="D22" t="str">
+        <v>$ 90,000.00</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Location: Remote (LatAm preferred)Team: Product Engineering | Tech: React, React Native, Next.js, TypeScriptA fast-growing product team is looking for Senior Frontend Engineers to help build high-performing web and mobile experiences at scale. Whether you specialize in Next.js for advanced web applications or React Native for seamless cross-platform mobile apps, this role offers the chance to shape user-facing products from the ground up.You’ll work closely with product managers, designers, and backend engineers to ship interfaces that are fast, responsive, and conversion-optimized. This is an opportunity to drive frontend architecture decisions and bring exceptional user experiences to life.What You’ll DoArchitect and develop scalable, high-performance UIs (Web or Mobile)Translate Figma designs into pixel-perfect, responsive interfacesOptimize performance, accessibility, and SEO (for web) or device-specific performance (for mobile)Collaborate cross-functionally on API integration and data-fetching strategiesContribute to code quality, CI/CD pipelines, and testing best practicesWhat We're Looking For5+ years of frontend engineering experience with modern frameworksWeb: Deep expertise with React and Next.jsMobile: Strong proficiency with React NativeSolid experience with TypeScript, reusable components, and clean architectureFamiliarity with modern styling tools (Tailwind, Styled Components, CSS Modules, etc.)Testing experience (Jest, React Testing Library, Detox, etc.)Strong Git and version control habits; experience working in CI workflowsNice to HaveExperience working in high-scale product environments (e.g., gaming, fintech, streaming)Familiarity with GraphQL, Firebase, or native modules (for mobile)Experience collaborating in Agile teams with international stakeholdersWhy This RoleYou’ll be joining a product-led team building real-time, high-impact software in a collaborative and remote-friendly environment. You’ll have real ownership over the frontend experience—whether on the web or mobile—and work with a team that values clean code, good design, and performance.</v>
+      </c>
+      <c r="F22" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-remote-senior-frontend-dev-react-native-mobile-or-web-en-queretaro-AF6A670FBACBE70161373E686DCF3405#lc=ListOffers-Score3-0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Hyatt Abogado Jr - Corporate Cancun</v>
+      </c>
+      <c r="B23" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D23" t="str">
+        <v>$ 18,000.00</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Who We AreAt Hyatt, we believe in the power of belonging and creating a culture of care, where our colleagues become family. Since 1957, our colleagues and guests have been at the heart of our business and helped Hyatt become one of the world's best and fastest-growing hospitality brands. Our transformative growth and the addition of new hotels, brands, and business lines can open the door for exciting career and growth opportunities for our colleagues.As we continue to grow, we never lose sight of what’s most important: People. We turn trips into journeys, encounters into experiences, and jobs into careers.Why Now?This is an exciting time to be at Hyatt. We are growing rapidly and are looking for passionate changemakers to be a part of our journey. The hospitality industry is resilient and continues to offer dynamic opportunities for upward mobility, and Hyatt is no exception.How We Care For Our PeopleOur purpose sets us apart—to care for people so they can be their best. Every business decision is made through the lens of our purpose, and it informs how we have and will continue to support each other as members of the Hyatt family. Our care for our colleagues is the key to our success. We’re proud to have earned a place on Fortune’s prestigious 100 Best Companies to Work For® list for the last ten years. This recognition is a testament to how our Hyatt family continues to come together to care for one another, our commitment to a culture of inclusivity, empathy, and respect, and making sure everyone feels like they belong.At HYATT We are looking for Abogado Jr, you will play a key role in the legal department, supporting corporate and contractual management.Your Responsibilities:• You will draft and review contracts• You will manage legal files and corporate books• You will consult and follow up on legal matters• You will assist in litigation and dispute resolution• You will coordinate notarial and administrative proceduresYour Profile:• Law degree• 1-2 years of experience in a similar role• Intermediate-Advanced English• Proficiency in Microsoft Office Suite and video conferencing tools.Apply now and take the next step in your IT career!Care Connects Us!We care for people so they can be their best!</v>
+      </c>
+      <c r="F23" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-hyatt-abogado-jr-corporate-cancun-en-benito-juarez-C71AB1537FC1E3D261373E686DCF3405#lc=ListOffers-Score3-1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Night Shift Technical Support Agent (Bilingual) - MXN 19K Salary</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Importante empresa del sector</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Cuauhtémoc, Ciudad de México DF</v>
+      </c>
+      <c r="D24" t="str">
+        <v>$ 16,000.00</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Night Owl Opportunity: Tier 1 Technical Support Agent (Overnight Shift)Are you ready to become part of a thriving corporate environment with an international scope? GlobalTech Corporation, a leader in providing technological solutions for the U.S. tax sector, is looking for dedicated professionals for our Tier 1 Technical Support team. This role focuses on delivering exceptional service and resolving technical incidents for our corporate clients.Your Role and Responsibilities:• Provide first-level technical support and resolve incidents remotely.• Accurately log all case details in our ticketing system.• Ensure timely follow-up on service requests and escalate complex problems when necessary.• Maintain a clear, professional, and solution-driven user experience for all clients.• Collaborate effectively with cross-functional technical and operational teams.Ideal Candidate Profile:• Education: High school diploma (minimum); a Bachelor's degree or technical certification is preferred.• Language: Advanced English (C1 level is essential).• Experience: Minimum of 6 months to 1 year of proven experience in technical support or customer service.• Technical Skills: Basic knowledge of ticketing platforms, remote support tools, and various digital applications.• Key Skills: Strong communication, organizational, and customer-centric abilities.• Work Schedule: Availability to work Monday to Friday, from 12:00 AM to 7:00 AM (Overnight Shift).Benefits &amp; Compensation:• Comprehensive Monthly Salary: $19,000 MXN (night bonus already included).• Direct Hire: Immediate direct hiring by GlobalTech Corporation.• Training: Full initial technical training provided to ensure your success.• Stability &amp; Growth: Enjoy job stability with clear opportunities for professional advancement.• Work Environment: A supportive and excellent work environment.• Payment: Punctual bi-weekly payments.Work Location:• Alcaldía Miguel Hidalgo, CDMX• Modality: On-site.• Availability: Immediate.Take the next step in your tech career. Apply for our Overnight Support role!</v>
+      </c>
+      <c r="F24" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-night-shift-technical-support-agent-bilingual-mxn-19k-salary-en-cuauhtemoc-64ACBA516D7DE51361373E686DCF3405#lc=ListOffers-Score3-2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Web master</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Mia hotels and Resorts</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D25" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E25" t="str">
+        <v>El corporativo Mia Hotels &amp; Resorts está en búsqueda de Web Master.ObjetivoEl Web máster será responsable de la administración, mantenimiento y optimización del sitio web de MÍA Reef Isla Mujeres. Su objetivo principal es garantizar una experiencia de usuario óptima, supervisar el rendimiento del sitio y coordinar con los departamentos de marketing y ventas para implementar estrategias que aumenten la conversión y retención de clientes.PerfilExperiencia de 3 años máximoExperiencia en hoteleríaConocimiento en RoibackRequerimientos: Lenguajes que debe dominar sí o sí: HTML5, CSS3, JavaScript (nivel medio, NEXT JS 10), jQuery, Bootstrap.Experiencia previa recomendada: CMS Roiback o manejo de CMS hoteleros similares.Deseable: manejo de SEO, Tag Manager y conocimientos básicos de análisis de datos (ej. carritos abandonados, conversiones).OfrecemosSalario competitivo, prestaciones de ley, seguro de vida, servicios de telemedicina 24/7.</v>
+      </c>
+      <c r="F25" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-web-master-en-benito-juarez-908410F3B60356AD61373E686DCF3405#lc=ListOffers-Score3-3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Customer Service Especialist - Bepensa (Base salary and additional benefits)</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Bepensa</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Mérida, Yucatán</v>
+      </c>
+      <c r="D26" t="str">
+        <v>$ 8,212</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Objective Collect past due payments to prevent accounts from rolling forward to the next bucket of delinquency. Follow all company policies and state and federal laws applicable to debt collection.We are looking for a vacancy:Customer Service RepresentativeAcademic studies:High school diploma (minimum) or Business Administration Career or RelatedWork Experience:1 year of customer service experience attending clients via phone (calls).Knowledge and skills:Customer service, administrative operations, collect past due payments, account managment, debt collectión, prevent repossesions and losses through negotiation and utilization of available programs, office (word, excel, powerpoint), advanced english (speaking proficiency).Schedule availability:Flexible schedule.</v>
+      </c>
+      <c r="F26" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-customer-service-especialist-bepensa-base-salary-and-additional-benefits-en-merida-93A07AD8D477E0C161373E686DCF3405#lc=ListOffers-Score3-4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Customer Support Representative - Salesforce Focused</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Pearl Talent</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Argentina</v>
+      </c>
+      <c r="D27" t="str">
+        <v>$5</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Work Arrangement: Fully remote, Overlap with EST working hours, US HolidaysJob Type: Full-timeWork Schedule: Monday to Friday, 9:00 AM – 5:00 PM EST (with flexibility based on client/user needs)Location: Remote, open only to candidates based in ArgentinaAbout Pearl Talent:Pearl works with the top 1% of candidates from around the world and connects them with the best startups in the US and EU. Our clients have raised over $5B in aggregate and are backed by companies like OpenAI, a16z, and Founders Fund. They’re looking for the sharpest, hungriest candidates who they can consistently promote and work with over many years. Candidates we’ve hired have been flown out to the US and EU to work with their clients, and even promoted to roles that match folks onshore in the US.Why Work with Us?We mean what we say that we’re building a different recruiting company here. We only work with exceptional founders from the US and EU who care about the long-term success of their team members. We also provide you with attainable 3, 6, 9, 12 month, and beyond retention bonuses in addition to community oriented opportunities like an annual retreat.About the CompanyThe company is a fast-growing SaaS company revolutionizing the insurance industry with the most advanced all-in-one CRM and Agency Management System, built entirely on Salesforce. The platform enables modern insurance agencies to accelerate growth, improve productivity, and streamline operations on a single, highly configurable solution. They promote a forward-thinking, agile work environment that values innovation, continuous improvement, and exceptional customer experiences. With a collaborative and remote-friendly culture, the company is deeply committed to transparency, initiative, and long-term client success.Company ValuesClient Obsession: Our success begins with theirs. The CSR is the first line of defense in ensuring a smooth, efficient, and positive client experience.SaaS with Soul: We believe in tech that’s human-centered. The CSR must embody empathy, patience, and clarity in every customer interaction.Operational Excellence: Accuracy, accountability, and problem resolution are key to building trust.Team Over Ego: No silos. Our CSRs collaborate tightly with Product, Sales, and Engineering to close the loop.The ideal candidate will align with these values by owning every support ticket with urgency and care, proactively suggesting improvements, and treating each customer interaction as a chance to build lasting loyalty.Main Functions (Day-to-Day Responsibilities)The Customer Support Representative will serve as a key player in the company's client success journey, providing responsive and knowledgeable support across its CRM + AMS platform.Triage, troubleshoot, and resolve client issues via Salesforce, email, and chat.Provide Salesforce-admin-level troubleshooting support—escalating complex issues when appropriate.Educate clients on best practices for using the company's platform, including workflows, integrations, and automation.Serve as a product expert capable of translating technical concepts into clear, user-friendly instructions.Document issues clearly and update internal knowledge bases for continuous team learning.Identify support trends and collaborate with Product and Engineering to resolve root causes.Maintain an internal loop with Customer Success Managers and Account Executives to ensure high-touch client support.Immediate Tasks (Week 1 Ownership):Complete onboarding and immersion into the company's Salesforce-based AMS platform.Shadow existing CSRs to understand tone, expectations, and typical support volumes.Deep-dive into internal knowledge base, current support SLAs, and past ticket history.Begin handling low-complexity tickets independently by end of week one.Set up personal Zendesk dashboard and begin logging response metrics.Join internal syncs with CSM and Product teams to understand cross-functional dependencies.RequirementsMust-Haves:Salesforce Admin Certification (active and up to date)2+ years of experience in customer support or technical support for SaaS or software productsStrong problem-solving skills, especially in environments built on Salesforce or similar CRMsExcellent verbal and written English communicationAbility to translate complex system behavior into client-friendly languageStrong documentation habits and proactive communication with internal teamsNice-to-Haves:Experience in the insurance, fintech, or agency management software spaceFamiliarity with Zendesk, HubSpot, and JiraExperience working in a high-growth SaaS environmentBenefitsCompensation Package:Competitive Salary: To be discussed during the interviewRemote Work: Fully remote—work from anywhereGenerous PTO: Ample paid time off to rest and rechargeDirect Mentorship: Grow through guidance from international industry expertsLearning &amp; Development: Ongoing access to resources for professional growthGlobal Networking: Work and connect with professionals around the worldWork-Life Balance: Flexible hours that support a healthy work-life balanceOur Recruitment Process:ApplicationScreeningTop-grading InterviewSkills AssessmentClient InterviewJob OfferClient OnboardingReady to Join Us?If this role aligns with your skills and career goals, we’d love to hear from you. Apply now to take the next step in your journey with Pearl!</v>
+      </c>
+      <c r="F27" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-customer-support-representative-salesforce-focused-en-argentina-891CB23A622A015D61373E686DCF3405#lc=ListOffers-Score3-5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>JDE System Specialist</v>
+      </c>
+      <c r="B28" t="str">
+        <v>ASOCIACION DE NORMALIZACION Y CERTIFICACION SA DE CV</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Gustavo A. Madero, Ciudad de México DF</v>
+      </c>
+      <c r="D28" t="str">
+        <v>$ 65,000.00</v>
+      </c>
+      <c r="E28" t="str">
+        <v>We are looking for talent, participate in our great work team.we look for our next: : JDE System SpecialistJob Summary:The JDE System Analyst will be responsible for providing technical support and maintenance for the JD Edwards (JDE) enterprise resource planning (ERP) system in the LAM region. This role will work closely with end-users to understand their requirements, troubleshoot issues, and implement solutions to enhance the functionality and efficiency of the JDE system.Key Responsibilities:1. Provide technical support and troubleshooting for the JDE system, including resolving user issues, identifying and addressing system errors, and implementing system updates and patches.2. Collaborate with end-users to understand their business requirements and translate them into functional and technical specifications for the JDE system.3. Perform system configuration, customization, and integration tasks to meet the specific needs of the LAM region.4. Develop and maintain JDE system documentation, including user manuals, training materials, and process workflows.5. Conduct user training and provide ongoing support to ensure effective utilization of the JDE system.Qualifications and Skills:• Bachelor's degree in Computer Science, Information Technology, or a related field, It is essential to have a professional degree• 3 years of experience as a JDE System Analyst or in a similar role• Proficiency in the Spanish &amp; English language is highly valued.• Proficient in JDE system administration, configuration, and customization• Strong understanding of JDE modules, such as Financials, Supply Chain, and Manufacturing• Experience in integrating JDE with other enterprise systems (e.g., ERP, CRM, HR)• Excellent problem-solving and analytical skills to identify and resolve complex technical issues• Effective communication and interpersonal skills to collaborate with end-users and cross-functional teams• Willingness to travel within the LAM region as neededBenefits:Superior benefits: 5% savings fund, vouchers, Life insuranceIf you are interested in the vacancy, apply here and we will contact you!</v>
+      </c>
+      <c r="F28" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-jde-system-specialist-en-gustavo-a-madero-0F170C733C75B65161373E686DCF3405#lc=ListOffers-Score3-6</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Night Shift Technical Support Agent (Bilingual) - MXN 19K Salary</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Importante empresa del sector</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Iztacalco, Ciudad de México DF</v>
+      </c>
+      <c r="D29" t="str">
+        <v>$ 16,000.00</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Night Owl Opportunity: Tier 1 Technical Support Agent (Overnight Shift)Are you ready to become part of a thriving corporate environment with an international scope? GlobalTech Corporation, a leader in providing technological solutions for the U.S. tax sector, is looking for dedicated professionals for our Tier 1 Technical Support team. This role focuses on delivering exceptional service and resolving technical incidents for our corporate clients.Your Role and Responsibilities:• Provide first-level technical support and resolve incidents remotely.• Accurately log all case details in our ticketing system.• Ensure timely follow-up on service requests and escalate complex problems when necessary.• Maintain a clear, professional, and solution-driven user experience for all clients.• Collaborate effectively with cross-functional technical and operational teams.Ideal Candidate Profile:• Education: High school diploma (minimum); a Bachelor's degree or technical certification is preferred.• Language: Advanced English (C1 level is essential).• Experience: Minimum of 6 months to 1 year of proven experience in technical support or customer service.• Technical Skills: Basic knowledge of ticketing platforms, remote support tools, and various digital applications.• Key Skills: Strong communication, organizational, and customer-centric abilities.• Work Schedule: Availability to work Monday to Friday, from 12:00 AM to 7:00 AM (Overnight Shift).Benefits &amp; Compensation:• Comprehensive Monthly Salary: $19,000 MXN (night bonus already included).• Direct Hire: Immediate direct hiring by GlobalTech Corporation.• Training: Full initial technical training provided to ensure your success.• Stability &amp; Growth: Enjoy job stability with clear opportunities for professional advancement.• Work Environment: A supportive and excellent work environment.• Payment: Punctual bi-weekly payments.Work Location:• Alcaldía Miguel Hidalgo, CDMX• Modality: On-site.• Availability: Immediate.Take the next step in your tech career. Apply for our Overnight Support role!</v>
+      </c>
+      <c r="F29" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-night-shift-technical-support-agent-bilingual-mxn-19k-salary-en-iztacalco-5D66C820D011250E61373E686DCF3405#lc=ListOffers-Score3-7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Desarrollador front end Senior Java Script, React - Java Script, React</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Asteci</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D30" t="str">
+        <v>$ 29,181</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Somos una Consultora de TI con diversos clientes nacionales e internacionales.Buscamos un Desarrollador Frontend Senior enfocado al desarrollo moderno con sólida experiencia en Java Script, Type Script y React Js.Requisitos clave:+ 5 años de experiencia en el desarrollo del sofware.Java Script, TypeScript.Frameworks : ReactJS, NestJS, NextJSTesting: Jest, testing en generalUso de patrones de Diseño.Seguridad: Fortify, Checkmarx, BlackduckHerramientas CI: Jenkins, Git, GitFlow, Bitbucket, JIRA, Confluence, Sonar,Checkmarx, fortifyDynatrace, SplunkBlack duckMetolologías Agil, Scrum.Conocimiento de Desarrollo e Integración con REST APIs.Inglés 80%Actividades:Diseño, desarrollo, integración, pruebas e implementación eficaces de requisitos empresariales complejos.Aplicación de conocimientos tecnológicos al diseño de modelos y/o sistemas, formulación de diseños técnicos detallados, investigación y recomendación de soluciones técnicas, desarrollo y entrega de aplicaciones mediante metodologías de desarrollo ágil.Capacidad para trabajar al más alto nivel técnico en el desarrollo de sistemas, manteniendo un sólido conocimiento de las estrategias y aplicaciones empresariales de gestión patrimonial.Liderazgo técnico, coordinación entre laboratorios, soporte a la producción y soporte a la implementación de versiones.Ofrecemos:Salario competitivo.Prestaciones de Ley.Seguro de gastos médicos menores y mayores.Esquema hibrido.Apoyo económico por teletrabajo.INTERESADOS FAVOR DE POSTULARSE ATRAVES DE ESTE MEDIO PARA AGENDAR UNA ENTREVISTA DE TRABAJO.</v>
+      </c>
+      <c r="F30" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrollador-front-end-senior-java-script-react-java-script-react-en-miguel-hidalgo-E5060CC1D092E88461373E686DCF3405#lc=ListOffers-Score3-8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Work From Home Shopify Engineer / Ref. 0176</v>
+      </c>
+      <c r="B31" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Aguascalientes, Aguascalientes</v>
+      </c>
+      <c r="D31" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E31" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Shopify Engineer at BairesDevWe are looking for a Shopify Engineer to join our Development team and help the client take its eCommerce platform to the next level. The Shopify Engineer will be responsible for designing, developing, and maintaining the clients Shopify website and integrations with other systems. This is an excellent opportunity for those professionals looking to develop in one of the fastest-growing companies in the industry!What You Will Do:- Collaborate with the eCommerce team to understand business requirements and translate them into technical solutions.- Design and implement custom Shopify themes and templates.- Build and maintain custom Shopify apps and plugins.- Integrate Shopify with other systems such as CRM, ERP, and payment gateways.- Ensure website performance and security are optimized.- Troubleshoot and resolve website issues.Heres what we are looking for:- 3+ years of experience with Shopify Liquid.- 2+ years of experience with a JS Framework (React, NextJS, VueJS, etc).- Proven track record in Shopify App development.- Shopify headless architecture experience (stores/apps) is desirable, but not mandatory.- Upper English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F31" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-shopify-engineer-ref-0176-en-aguascalientes-2F8573081BEEE1A961373E686DCF3405#lc=ListOffers-Score3-9</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Customer Service - Automotive Industry</v>
+      </c>
+      <c r="B32" t="str">
+        <v>IMS Gear, S.A. de C.V.</v>
+      </c>
+      <c r="C32" t="str">
+        <v>El Marqués, Querétaro</v>
+      </c>
+      <c r="D32" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Drive Your Career Forward with IMS Gear!At IMS Gear, were not just creating drive solutions; were driving innovation. With over 3,100 passionate employees worldwide, we engineer and produce cutting-edge drive systems for global markets, from automotive to e-mobility and industrial applications.Why IMS Gear?Innovate and Grow: Be part of a forward-thinking team that values your ideas and empowers your professional development.Global Impact, Local Community: Enjoy the best of both worlds with international opportunities and a supportive workplace environment.Comprehensive Benefits: We offer competitive compensation, health benefits and vacation time to support your well-being and work-life balance.Your Role: Logistics SpecialistAs a Logistics Specialist and key member of our Team, you will be responsible for the proper functioning of all the material and logistics processes at IMS Gear (planning and procurement of materials, planning and effective communication of production plans, release and delivery of materials to meet forecasted demand and actual sales orders and the planning and communication of delivery plans)Key Responsibilities:Customer Service: Responsible to bring in all Customer release/order data as well as supplier order data to the IMS ERP and production scheduling systems. Coordinates receipt of accurate sales requirements and release data from all customers and integrate into IMS Gear ERP and Production Scheduling systemsInventory: Manages the inventory in line with company goals to achieve the needed accuracy and overall level. Reviews all stock levels and ensures support of the production planShipments: Receives in and ship out material according to sales order scheduleERP System Accuracy: Ensure consistency and accuracy within the ERP systemLeadership and CollaborationDynamic Contributions: Perform additional duties as assigned to support the Logistics Teams success.Your Qualifications:Educational Background: Bachelors Degree in Business Administration with Logistics/ Purchasing experience.Professional Experience: Minimum of 3 years in a manufacturing environment, Automotive Industry preferrableTechnical Proficiency: Advanced expertise in Microsoft Excel, Previous ERP/MRP experience, Hands-on capabilities and experience in controlling inventory, Excellent Computer skills (MS Office).Communication and Initiative: Excellent interpersonal and communication skills, with a proactive and self-motivated approach to problem-solving.Ready to Accelerate Your Career?If youre driven by teamwork, flexibility, and a commitment to excellence, IMS Gear is your next destination. Join us and help shape the future of drive solutions.Apply Today and Start Driving Innovation with IMS Gear!</v>
+      </c>
+      <c r="F32" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-customer-service-automotive-industry-en-el-marques-89332477209D804E61373E686DCF3405#lc=ListOffers-Score3-10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Work From Home Java Team Lead / Ref. 0003E</v>
+      </c>
+      <c r="B33" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Guanajuato, Guanajuato</v>
+      </c>
+      <c r="D33" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E33" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Java Team Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a Java Team Lead in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Technically own different modules of the platform, including design, development, &amp; integration.- Design and write clean, robust, server-side code.- Perform research and development to evaluate new technologies, and ideas and communicate value for the company.Heres what we are looking for:- 7+ years of experience in Java.- Advance agile methodologies management.- Advanced Design Patterns knowledge.- Advanced IT infrastructure knowledge.- Experience with Security.- Experience developing/integrating with large-scale applications.- Fully specialized in Backend, Frontend development areas.- Strong experience in coding reviews and managing CI/CD pipelines.- Expert understanding of the benefits/weaknesses of the clients requirements.- Advanced knowledge of the tradeoffs of choosing a certain technology.- Strong experience participating in meetings with clients, users, and stakeholders.- Experience leading teams, allocating tasks, identifying risks, decision making, estimating tasks, managing conflicts, and planning.- Advanced English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F33" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-java-team-lead-ref-0003e-en-guanajuato-B2FF4AB2D3D59A3761373E686DCF3405#lc=ListOffers-Score3-11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Work From Home Python Tech Lead / Ref. 0071</v>
+      </c>
+      <c r="B34" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Mérida, Yucatán</v>
+      </c>
+      <c r="D34" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E34" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Python Tech Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a Python Tech Leader in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing the innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Work closely alongside their Engineering and Business Stakeholders to support the delivery of the project.- Be able to manage your time effectively to focus on coding as well as supporting junior members.- Integrate with the DevOps team to maintain tasks.- Make architectural decisions keeping the future of a growing business in mind.Heres what we are looking for:- Advance agile methodologies management.- Advanced Design Patterns knowledge.- Advanced IT infrastructure knowledge.- Experience with Security.- Experience developing/integrating with large-scale applications.- Fully specialized in Backend, Frontend development areas.- Strong experience in coding reviews and managing CI/CD pipelines.- Expert understanding of the benefits/weaknesses of clients requirements.- Advanced knowledge of the tradeoffs of choosing a certain technology.- Strong experience participating in meetings with clients, users, and stakeholders.- Experience leading teams, allocating tasks, identifying risks, decision making, estimating tasks, managing conflicts, planning.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F34" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-python-tech-lead-ref-0071-en-merida-8E1C16287F7BBB5661373E686DCF3405#lc=ListOffers-Score3-12</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Desarrollador fullstack - Desarrollador jr pasante o recien egresado</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Disrupting</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Puebla, Puebla</v>
+      </c>
+      <c r="D35" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Modalidad: RemotoTipo de Contrato: Tiempo Completo / PasantíaNivel: Junior (Recién Egresados o Pasantes)Resumen del Puesto¡Buscamos a un entusiasta y talentoso Desarrollador Full-Stack Junior para unirse a nuestro equipo de tecnología! Esta es una oportunidad única para recién egresados o estudiantes en el último año de su carrera que deseen iniciar su trayectoria profesional en el desarrollo de software. Como parte de nuestro equipo, tendrás la oportunidad de trabajar con tecnologías de vanguardia como Go (Golang) en el backend y Next.js en el frontend, todo mientras colaboras en un entorno 100% remoto. Si eres una persona proactiva, con una gran pasión por aprender y con ganas de construir aplicaciones web modernas, ¡queremos conocerte!Responsabilidades ClaveComo Desarrollador Full-Stack Junior, tus responsabilidades incluirán:Desarrollo Frontend: Colaborar en la creación de interfaces de usuario interactivas y responsivas utilizando Next.js y React.Desarrollo Backend: Participar en el diseño, desarrollo y mantenimiento de APIs RESTful robustas y eficientes con Go.Colaboración en Equipo: Trabajar de la mano con otros desarrolladores, diseñadores y líderes de producto en un entorno ágil para entregar soluciones de alta calidad.Mantenimiento de Código: Escribir código limpio, bien documentado y mantenible, siguiendo las mejores prácticas de la industria.Administración de Servidores: Apoyar en el despliegue y mantenimiento de aplicaciones en servidores Linux.Aprendizaje Continuo: Mantenerte actualizado sobre las nuevas tendencias y tecnologías en el desarrollo de software para proponer mejoras e innovaciones.Requisitos y HabilidadesRequisitos Indispensables:Formación Académica: Recién egresado o estudiante de los últimos semestres de Ingeniería en Sistemas, Ciencias de la Computación o carreras afines.Conocimientos en Go: Comprensión básica o académica del lenguaje de programación Go (Golang) para el desarrollo de backend.Conocimientos en Frontend: Experiencia básica o académica con Next.js, React y JavaScript (ES6+).Bases de Datos: Familiaridad con bases de datos relacionales (como PostgreSQL o MySQL) y/o no relacionales (como MongoDB).Entorno Linux: Conocimientos básicos en el manejo de la línea de comandos de Linux.Control de Versiones: Experiencia básica con Git y plataformas como GitHub o GitLab.Habilidades Deseables (¡No te preocupes si no las tienes todas!):Conocimiento en la creación y consumo de APIs RESTful.Familiaridad con Docker para la contenedorización de aplicaciones.Interés en metodologías de desarrollo ágil como Scrum.Excelentes habilidades de comunicación y trabajo en equipo.Capacidad para resolver problemas de manera creativa y proactiva.Autogestión y disciplina para trabajar de manera remota.¿Qué Ofrecemos?Trabajo 100% Remoto: Trabaja desde cualquier lugar de México.Crecimiento Profesional: Una ruta de aprendizaje clara con mentoría de desarrolladores senior para impulsar tu carrera.Cultura de Colaboración: Un ambiente de trabajo amigable y colaborativo donde tus ideas son valoradas.Flexibilidad: Horarios flexibles para un mejor equilibrio entre la vida personal y profesional.Experiencia Real: La oportunidad de trabajar en proyectos desafiantes y con impacto real desde el primer día.</v>
+      </c>
+      <c r="F35" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrollador-fullstack-desarrollador-jr-pasante-o-recien-egresado-en-puebla-7BAF0406D52DE5C261373E686DCF3405#lc=ListOffers-Score3-13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Work From Home React Native Tech Lead / Ref. 0198</v>
+      </c>
+      <c r="B36" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Puebla, Puebla</v>
+      </c>
+      <c r="D36" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E36" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.React Native Tech Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a React Native Tech Leader in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing the innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Lead a front end team of approximately 5 developers located locally and remotely.- Oversee front end coding/logic.- Integrate UI /UX and animation features.- Collaborate with engineers, designer, and product managers in an agile environment.- Plan projects (understand requirements, effort, time, budget, etc.).Heres what we are looking for:- 7+ years of experience in Front End development with strong skills in Javascript, CSS3 and HTML5.- 2+ years of experience developing Web applications using ReactJS, Flux, Redux, Relay, etc.- 2+ years of experience working with RoR.- Familiar with the concepts of basic programming, JavaScript and data structures, types of variables and idiosyncrasies.- Advanced English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F36" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-react-native-tech-lead-ref-0198-en-puebla-F8609ED15990789861373E686DCF3405#lc=ListOffers-Score3-14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Work From Home Golang Tech Lead / Ref. 0138</v>
+      </c>
+      <c r="B37" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C37" t="str">
+        <v>San Luis Potosí, San Luis Potosí</v>
+      </c>
+      <c r="D37" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E37" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Golang Tech Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a Golang Tech Leader in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing the innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Fostering a high-performance engineering culture whilst growing and leading your tribe.- Reviewing and contributing to code whilst utilizing best practices to balance the creation of new functionalities whilst meeting the needs of existing customers.- Collaborating with cross-regional teams to collectively design, develop and release localised MVPs.Heres what we are looking for:- 10+ years of experience working as a developer.- 7+ years of experience in Golang.- Advance agile methodologies management.- Advanced Design Patterns knowledge.- Advanced IT infrastructure knowledge.- Experience with Security.- Experience developing/integrating with large-scale applications.- Fully specialized in Backend, Frontend development areas.- Strong experience in coding reviews and managing CI/CD pipelines.- Expert understanding of the benefits/weaknesses of clients requirements.- Advanced knowledge of the tradeoffs of choosing a certain technology.- Strong experience participating in meetings with clients, users, and stakeholders.- Experience leading teams, allocating tasks, identifying risks, decision making, estimating tasks, managing conflicts, planning.- Advanced English Level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F37" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-golang-tech-lead-ref-0138-en-san-luis-potosi-63EDF3D1026B19E461373E686DCF3405#lc=ListOffers-Score3-15</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Work From Home Fullstack Node + Nest + React Tech Lead / Ref. 0111</v>
+      </c>
+      <c r="B38" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Centro, Tabasco</v>
+      </c>
+      <c r="D38" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E38" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Fullstack Node + Nest + React Tech Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a Node Tech Leader in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Architect Bandit backend systems using the best practices.- Implement and iterate features in a tactical manner and at a rapid pace.- Work collaboratively and efficiently across functional teams in a fast-paced early-stage startup environment.- Design, extend, and implement APIs.- High engineering quality standards through code reviews, unit tests, and analytics.- Create engineering efficiencies through automation and development of tools.- Define engineering processes for product launches and releases.- Help us grow the world-class engineering team by running technical interviews.Heres what we are looking for:- 7+ years of experience in React/Node.- Experience with SQL and NoSQL Databases.- Experience with Microservices and the Cloud.- Experience using the Nest.js framework.- IT infrastructure knowledge.- Intermediate agile methodologies management.- Strong understanding of best practices, SOLID principles, CLEAN Code, and scalable solutions.- Knowledge of AWS (RDS, SNS, SQS, Lambda), REST, GraphQL, TypeScript, Terraform and CircleCI.- Experience developing entire applications from scratch.- Experience in automated tests, and CI/CD pipelines.- Strong experience with Version control.- Advanced English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F38" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-fullstack-node-nest-react-tech-lead-ref-0111-en-centro-BA5B870BD4B2ABD261373E686DCF3405#lc=ListOffers-Score3-16</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Work From Home Node Backend Tech Lead / Ref. 0111</v>
+      </c>
+      <c r="B39" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Juárez, Chihuahua</v>
+      </c>
+      <c r="D39" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E39" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Node Backend Tech Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a Node Backend Tech Lead in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Works with the team to determine the needs of the global technical architecture.- Identifies the integration points for third-party and existing systems.- Validates that all technical choices will integrate with the final solution and adhere to the technical contracts defined for integration.Heres what we are looking for:- 7+ years of experience in Node development.- Advance agile methodologies management.- Advanced Design Patterns knowledge.- Advanced IT infrastructure knowledge.- Experience with Security.- Experience developing/integrating with large-scale applications.- Fully specialized in Backend, Frontend development areas.- Strong experience in coding reviews and managing CI/CD pipelines.- Expert understanding of the benefits/weaknesses of a clients requirements.- Advanced knowledge of the tradeoffs of choosing a certain technology.- Strong experience participating in meetings with clients, users, and stakeholders.- Experience leading teams, allocating tasks, identifying risks, decision making, estimating tasks, managing conflicts, and planning.- Advanced English level.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F39" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-node-backend-tech-lead-ref-0111-en-juarez-A078674A1890317A61373E686DCF3405#lc=ListOffers-Score3-17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Work From Home Python Tech Lead / Ref. 0071</v>
+      </c>
+      <c r="B40" t="str">
+        <v>BairesDev LLC</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Querétaro, Querétaro</v>
+      </c>
+      <c r="D40" t="str">
+        <v>$ 3,700</v>
+      </c>
+      <c r="E40" t="str">
+        <v>At BairesDev®, weve been leading the way in technology projects for over 15 years. We deliver cutting-edge solutions to giants like Google and the most innovative startups in Silicon Valley.Our diverse 4,000+ team, composed of the worlds Top 1% of tech talent, works remotely on roles that drive significant impact worldwide.When you apply for this position, youre taking the first step in a process that goes beyond the ordinary. We aim to align your passions and skills with our vacancies, setting you on a path to exceptional career development and success.Python Tech Lead at BairesDevIf you are a natural leader with mentoring experience, this job is for you! As a Python Tech Leader in our Development Team, your mission will be technically overseeing a team of experienced front and back developers. You will work in a fast-paced global team in charge of pushing the innovation to the next level. Innovation is at the heart of the BairesDev strategy.What You Will Do:- Work closely alongside their Engineering and Business Stakeholders to support the delivery of the project.- Be able to manage your time effectively to focus on coding as well as supporting junior members.- Integrate with the DevOps team to maintain tasks.- Make architectural decisions keeping the future of a growing business in mind.Heres what we are looking for:- Advance agile methodologies management.- Advanced Design Patterns knowledge.- Advanced IT infrastructure knowledge.- Experience with Security.- Experience developing/integrating with large-scale applications.- Fully specialized in Backend, Frontend development areas.- Strong experience in coding reviews and managing CI/CD pipelines.- Expert understanding of the benefits/weaknesses of clients requirements.- Advanced knowledge of the tradeoffs of choosing a certain technology.- Strong experience participating in meetings with clients, users, and stakeholders.- Experience leading teams, allocating tasks, identifying risks, decision making, estimating tasks, managing conflicts, planning.How we do make your work (and your life) easier:- 100% remote work (from anywhere).- Excellent compensation in USD or your local currency if preferred- Hardware and software setup for you to work from home.- Flexible hours: create your own schedule.- Paid parental leaves, vacations, and national holidays.- Innovative and multicultural work environment: collaborate and learn from the global Top 1% of talent.- Supportive environment with mentorship, promotions, skill development, and diverse growth opportunities.Apply now and become part of a global team where your unique talents can truly thrive!</v>
+      </c>
+      <c r="F40" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-work-from-home-python-tech-lead-ref-0071-en-queretaro-662A384C936D3A8161373E686DCF3405#lc=ListOffers-Score3-18</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Desarrollador Senior - Java Script + ReactJs</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Asteci</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D41" t="str">
+        <v>$ 35,000.00</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Somos una Consultora de TI con diversos clientes nacionales e internacionales.Estamos en búsqueda de un Desarrollador Senior enfocado al desarrollo moderno con sólida experiencia en Java Script, Type Script y React JsOFRECEMOS:Salario competitivo.Prestaciones de Ley.Seguro de gastos médicos menores y mayores.Esquema hibrido.Apoyo económico por teletrabajo.ACTIVIDADES:Diseño, desarrollo, integración, pruebas e implementación eficaces de requisitos empresariales complejos.Aplicación de conocimientos tecnológicos al diseño de modelos y/o sistemas, formulación de diseños técnicos detallados, investigación y recomendación de soluciones técnicas, desarrollo y entrega de aplicaciones mediante metodologías de desarrollo ágil.Capacidad para trabajar al más alto nivel técnico en el desarrollo de sistemas, manteniendo un sólido conocimiento de las estrategias y aplicaciones empresariales de gestión patrimonial.Liderazgo técnico, coordinación entre laboratorios, soporte a la producción y soporte a la implementación de versiones.REQUISITOS:+ 5 años de experiencia en el desarrollo del sofware.Java Script, TypeScript.Frameworks : ReactJS, NestJS, NextJSTesting: Jest, testing en generalUso de patrones de Diseño.Seguridad: Fortify, Checkmarx, BlackduckHerramientas CI: Jenkins, Git, GitFlow, Bitbucket, JIRA, Confluence, Sonar,Checkmarx, fortifyDynatrace, SplunkBlack duckMetolologías Agil, Scrum.Conocimiento de Desarrollo e Integración con REST APIs.+ 3 años de experiencia práctica Backend para la capa front-endInglés 80%INTERESADOS FAVOR DE POSTULARSE A TRAVÉS DE ESTE MEDIO PARA AGENDAR UNA ENTREVISTA DE TRABAJO.</v>
+      </c>
+      <c r="F41" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrollador-senior-java-script-reactjs-en-miguel-hidalgo-4A573AD4C04385F761373E686DCF3405#lc=ListOffers-Score3-19</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Líder de Desarrollo Fullstack - Fullstack</v>
+      </c>
+      <c r="B42" t="str">
+        <v>AVASA</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Mérida, Yucatán</v>
+      </c>
+      <c r="D42" t="str">
+        <v>$ 11,239</v>
+      </c>
+      <c r="E42" t="str">
+        <v>¿Quiénes somos?Una compañía líder en el mercado, con presencia a nivel nacional. Hemos crecido de forma sostenida en los últimos años diversificándonos en distintos giros comercial dentro del sector automovilístico, brindando servicios y productos competitivos.Buscamos para nuestras oficinas en Mérida, un Líder técnico Desarrollador FullStack, para administrar nuestro equipo de desarrollo.¿Qué buscamos?4 a 5 años de experiencia como: Líder técnico, líder de desarrollo o Coordinador de Desarrollo.Un Líder de Desarrollo full-stack con amplios conocimientos y experiencia en el desarrollo web, capaz de trabajar tanto en el front-end como en el back-end, con sólidas habilidades de liderazgo, gestión de proyectos y comunicación para dirigir un equipo de desarrollo y garantizar la entrega exitosa de proyectos.Habilidades técnicas:Front-end: HTML, CSS, JavaScript, frameworks y librerías (React.js, Next.js)Back-end: Lenguajes como Python, Java, Node.js, bases de datos (SQL,MySQL Server, MariaDB), APIs.Arquitectura: Conocimiento de arquitecturas web, patrones de diseño, testing y despliegue.Herramientas: Control de versiones (Git, GitLab), sistemas y herramientas de gestión de proyectos como Jira, herramientas de automatización.Habilidades de liderazgo y gestión:Gestión de equipos: Planificación, organización, motivación y evaluación del desempeño.Gestión de proyectos: Definición de objetivos, planificación, seguimiento, resolución de problemas.Comunicación: Capacidad para comunicarse eficazmente con el equipo, clientes y partes interesadas.Resolución de problemas: Capacidad para identificar y solucionar problemas técnicos y de gestión.Funciones:Definir la arquitectura y diseño técnico de la aplicación.Dirigir y coordinar al equipo de desarrollo.Establecer estándares de calidad y buenas prácticas de desarrollo.Realizar revisión de código y garantizar la calidad del software.Colaborar con otros equipos y partes interesadas.Mantenerse actualizado sobre las últimas tecnologías y tendencias.Contribuir al desarrollo técnico del equipo.Asegurar la entrega exitosa de los proyectos.¿Por qué nosotros?Porque somos una empresa buscando la mejora constante e innovación.Oferta: SB (directo, nominal, prestaciones de ley y beneficios internos).Modalidad: 100% Presencial.Horario: lunes a viernes 09:00 a 6:00 pm.Ubicación: Zona norte, Mérida, Yucatán.</v>
+      </c>
+      <c r="F42" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-lider-de-desarrollo-fullstack-fullstack-en-merida-FD4E97ADC1B2828661373E686DCF3405#lc=ListOffers-Score3-0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Engineer - Manufacturing and CNC Process Optimization</v>
+      </c>
+      <c r="B43" t="str">
+        <v>IMS Gear, S.A. de C.V.</v>
+      </c>
+      <c r="C43" t="str">
+        <v>El Marqués, Querétaro</v>
+      </c>
+      <c r="D43" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Location: Gainesville, GAJob Type: Full-Time, On-SiteSchedule: Day Shift | On-call when requiredDepartment: Manufacturing EngineeringReports To: Engineering ManagerPosition OverviewIMS Gear is seeking a highly skilled and motivated Engineer to join our manufacturing operations in Gainesville, Georgia. This position is central to our mission of delivering precision gear components by optimizing and improving our manufacturing processes. Youll work hands-on with equipment, CNC programming, and process innovation to enhance efficiency, reduce waste, and uphold our high quality and safety standards.Key ResponsibilitiesConduct process and machine capability studies; drive improvements.Develop and refine CNC processes, troubleshoot tooling issues, and perform G-code programming.Support APQP, FMEA, and Control Plan creation and reviews.Commission and accept complex equipment and machines.Select suppliers, evaluate technical offers, and coordinate purchases of indirect materials.Define, monitor, and adjust critical process parameters.Write and maintain detailed work instructions and training materials.Lead feasibility studies and implement custom or modified process solutions.Perform root cause analysis on alarms, quality complaints, and process failures.Collaborate cross-functionally on 8D problem-solving and continuous improvement projects.Ensure compliance with ISO14001, safety, and internal quality standards.Support robotic programming and machine control initiatives.Supervise student interns and introduce employees to new systems.Maintain automation maintenance logs and contribute to knowledge sharing (SharePoint).RequirementsEducationBachelors degree in mechanical engineering or a related field.Six Sigma Green Belt certification (preferred).ExperienceMinimum 5 years in high-volume manufacturing (preferably IATF environment).CNC Turning and CAD experience required.Familiarity with Star (Swiss) and conventional turning machines.FANUC CNC controller knowledge (required); Siemens CNC (preferred).Physical &amp; Work Environment RequirementsOccasional lifting (up to 25 lbs.) and pushing/pulling (up to 50 lbs.).Frequent standing, walking, bending, reaching, and using fine motor skills.Exposure to active manufacturing environments PPE required (safety glasses, hearing protection, safety shoes).Benefits401(k) with 4% company match no vesting periodComprehensive Health, Dental, Vision InsuranceCompany-Paid Life and Disability Insurance15 Days PTO + 10 Paid HolidaysRelocation Support (as per policy)Why IMS Gear?At IMS Gear, we believe in shaping the future of mobility through precision and innovation. We are proud to foster a collaborative and inclusive workplace where your contributions matter. Join our team and be part of something that drives the world forward.Equal Opportunity EmployerIMS Gear is an equal opportunity employer. We celebrate diversity and are committed to creating an inclusive environment for all employees regardless of race, color, religion, gender, national origin, disability, or veteran status.Apply Today!Take the next step in your engineering career with IMS Gear. We look forward to welcoming you to our team.Disclaimer: This job description is not designed to cover or contain a comprehensive listing of activities, duties or responsibilities that are required of the position. Duties, responsibilities, and activities may change, or new ones may be assigned at any time with or without notice.</v>
+      </c>
+      <c r="F43" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-engineer-manufacturing-and-cnc-process-optimization-en-el-marques-DF16EA59CBEDE60161373E686DCF3405#lc=ListOffers-Score3-1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Front End Developer Js - Senior</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Asteci</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D44" t="str">
+        <v>$ 35,000.00</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Somos una Consultora de TI con diversos clientes nacionales e internacionales.Buscamos un Front End Senior enfocado al desarrollo moderno con sólida experiencia en Java Script, Type Script y React JsRequisitos clave:+ 5 años de experiencia en el desarrollo del sofware.Java Script, TypeScript.Frameworks : ReactJS, NestJS, NextJSTesting: Jest, testing en generalUso de patrones de Diseño.Seguridad: Fortify, Checkmarx, BlackduckHerramientas CI: Jenkins, Git, GitFlow, Bitbucket, JIRA, Confluence, Sonar,Checkmarx, fortifyDynatrace, SplunkBlack duckMetolologías Agil, Scrum.Conocimiento de Desarrollo e Integración con REST APIs.+ 3 años de experiencia práctica Backend para la capa front-endInglés 80%Actividades:Diseño, desarrollo, integración, pruebas e implementación eficaces de requisitos empresariales complejos.Aplicación de conocimientos tecnológicos al diseño de modelos y/o sistemas, formulación de diseños técnicos detallados, investigación y recomendación de soluciones técnicas, desarrollo y entrega de aplicaciones mediante metodologías de desarrollo ágil.Capacidad para trabajar al más alto nivel técnico en el desarrollo de sistemas, manteniendo un sólido conocimiento de las estrategias y aplicaciones empresariales de gestión patrimonial.Liderazgo técnico, coordinación entre laboratorios, soporte a la producción y soporte a la implementación de versiones.Ofrecemos:Salario competitivo.Prestaciones de Ley.Seguro de gastos médicos menores y mayores.Esquema hibrido.Apoyo económico por teletrabajo.INTERESADOS FAVOR DE POSTULARSE ATRAVES DE ESTE MEDIO PARA AGENDAR UNA ENTREVISTA DE TRABAJO.</v>
+      </c>
+      <c r="F44" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-front-end-developer-js-senior-en-miguel-hidalgo-74D00C28B76CFF9161373E686DCF3405#lc=ListOffers-Score3-2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Food and Beverage Manager - Gerente de alimentos y bebidas</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Alliance Abroad LATAM</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Quintana Roo, Yucatán</v>
+      </c>
+      <c r="D45" t="str">
+        <v>$ 103,000.00</v>
+      </c>
+      <c r="E45" t="str">
+        <v>¡Hola a todos! Nos complace anunciar una nueva oportunidad de empleo en nuestra red de Hoteles.Buscamos un Gerente de Alimentos y Bebidas apasionado, con experiencia y habilidades de liderazgo sólidas parair a trabajar a USA con visado TN (nosotros te guiamos en el proceso del visado).Location: Greenough, MontanaSalary/Wage $62k AnnuallyPosition OverviewJoin the Team at Montanas Premier Luxury Ranch Resort!Nestled on a breathtaking 37,000-acre ranch, The Resort embodies the spirit of the American West. As a family-owned, award-winning destination, we inspire both guests and team members alike.We are seeking a talented Food and Beverage Manager to join our team. The role of the Food and Beverage Manager is to ensure world class service is provided for our guests in our various dining outlets. Responsibilities will encompass all facets of the resort food and beverage in the dining room but may include and not be limited to outside event venues, catered offerings, and special events. The dining manager must manage and maintain The Resort standards of service as well as seeking opportunities to enhance guest experience, while being fiscally responsible with our resources.ResponsibilitiesResponsible for all facets of our various dining outlets, including but not limited to; labor management, menu curation/training, wine inventory/training, purchasing, training, reporting and daily serviceResponsible for all staff scheduling according to volume of business; understand how to be flexible when necessary to meet labor expectations; ability to adjust daily operations to be in line with the budgetResponsible for all employee relations to include accountability and documentationAid in recruiting, hiring, and training and growing exceptional Food &amp; Beverage team members; Plan and provide training and guidance daily, weekly, and monthlyKnow, understand and train others on operating systems such as the POS system, Open Table and others, as requiredKnowledgeable on all menu items including preparation, any allergens, and alternative preparationsWork to continually improve guest dining satisfaction while maintaining the operating budgetImprove service by communicating and assisting to understand and guest needs, providing guidance, feedback, and individual coaching when neededSubmit future goals, operational improvements, and employee management to Director of RestaurantsProvide day-to-day guidance and oversight of Food &amp; Beverage team members; actively promote, train, coach, and recognize performanceIdentify, address and document individual team member performance problems according to standard operating procedureResponsible for all inventories of china, glassware, and silverwareManage operations and ensures compliance with all Food &amp; Beverage policies, sanitation, food standards and proceduresMaintain flexible hours to accommodate guest and special event needs, due to the cyclical nature of the hospitality industry; Position requires full availability including evenings, weekends, holidays or as neededMaintain complete knowledge of and comply with all departmental policies/service procedureRequired skills3+ years experience in Food &amp; Beverage Management in a resort or fine dining settingHousing type-We offer housing for 3 months to allow them to settle in and establish their own place to live. Single occupancy room in The Junction apartment building. Bathroom in unit. Shared facilities (kitchens, laundry), free wifi.-$350 per month ($175 deducted from payroll every 2 weeks). $300 deposit ($100 deducted from payroll for the first 3 paychecks)Additional commentsWe require that they have a drivers license for at least 2 years and a clean motor vehicle report so that they can drive our vehicles while theyre in the process of getting their MT license.For all TN candidates this is the expectation: They will rent a car or rent via Turo (doesnt require a US drivers license) until they are able to purchase their own vehicle.Gas station, convenience store, and bar located next to the apartment building. Ten minute drive to The Resort. Twenty minute drive to the town of Seeley Lake for groceries, restaurants, etc.What We Offer:Medical, Dental, Vision Insurance401K with Employer MatchPaid Time Off 9 Floating Holidays and 15 Personal DaysCareer Development and Advancement OpportunitiesLife Insurance, Long Term, and Short-Term DisabilityEmployee Assistance Program (5 free counseling sessions)Referral Bonus ProgramEmployee Discounts on Merchandise (30% on select items in our retail store)Employee Lunch ProvidedSend your CV through this medium and take the first step towards a new and exciting stage in your professional career.</v>
+      </c>
+      <c r="F45" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-food-and-beverage-manager-gerente-de-alimentos-y-bebidas-en-quintana-roo-ADEB52CF3A13E1EB61373E686DCF3405#lc=ListOffers-Score3-3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Desarrollador Frontend - React, Java Script</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Asteci</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D46" t="str">
+        <v>$ 29,181</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Consultora de TI con diversos clientes a nivel nacional e internacional solicita:Desarrollador Frontend Senior enfocado al desarrollo moderno con sólida experiencia en React JS, Java Script, Type Script.Requisitos:Lenguajes: JavaScript, TypeScriptFrameworks: ReactJS, NestJS, NextJSJest, testing en general.Uso de patrones de diseño.Seguridad: Fortify, Checkmarx, BlackduckHerramientas CI: Jenkins, Git, GitFlow, Bitbucket, JIRA, Confluence, SonarObservabilidad: Dynatrace, SplunkMetolologías Agil, Scrum.Conocimiento de Desarrollo e Integración con REST APIs.Inglés 80%.Actividades:Diseño, desarrollo, integración, pruebas e implementación eficaces de requisitos empresariales complejos.Aplicación de conocimientos tecnológicos al diseño de modelos y/o sistemas, formulación de diseños técnicos detallados, investigación y recomendación de soluciones técnicas, desarrollo y entrega de aplicaciones mediante metodologías de desarrollo ágil.Capacidad para trabajar al más alto nivel técnico en el desarrollo de sistemas, manteniendo un sólido conocimiento de las estrategias y aplicaciones empresariales de gestión patrimonial.Liderazgo técnico, coordinación entre laboratorios, soporte a la producción y soporte a la implementación de versiones.Ofrecemos:Salario competitivo.Prestaciones de Ley.Seguro de gastos médicos menores y mayores.Esquema hibrido.Apoyo económico por teletrabajo.INTERESADOS FAVOR DE POSTULARSE ATRAVES DE ESTE MEDIO PARA AGENDAR UNA ENTREVISTA DE TRABAJO.</v>
+      </c>
+      <c r="F46" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-desarrollador-frontend-react-java-script-en-miguel-hidalgo-CAC9568689E2246761373E686DCF3405#lc=ListOffers-Score3-4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Front Office Manager - Luxury Resort</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Alliance Abroad LATAM</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Los Cabos, Baja California Sur</v>
+      </c>
+      <c r="D47" t="str">
+        <v>$ 100,000.00</v>
+      </c>
+      <c r="E47" t="str">
+        <v>¡Hola a todos! Nos complace anunciar una nueva oportunidad de empleo en nuestra red de Hoteles.Buscamos un Front Desk Manager apasionado, con experiencia y habilidades de liderazgo sólidas para ir a trabajar a USA con visado TN (nosotros te guiamos en el proceso del visado).Location: Greenough, MontanaSalary/Wage $60,000 - $65,000 USD annuallyRequired: Multiple years of Forbes Five Star experienceResponsibilitiesTrains Front Office and Guest Services personnel to Forbes 5-Star standards.Creates weekly schedule for Front Desk and monitors staff scheduling to flex based on business needs.Maintains thorough knowledge of accommodations, package plans, and Resort facilities.Check guests in and out including preparation of folios and authorizing payments.Act as Manger on Duty (MOD).Responds to guest needs and anticipates their unstated ones.Ensure daily checklists are completed in Front Desk and Guest Services.Supportive Functions and ResponsibilitiesRemains flexible with open availability in order to cover the unexpected needs of the Resort.Expert knowledge of Maestro PMS, the hotel app, and all other programs and systems.Ability to lift and carry 50 pounds.Greets guests arriving and departing from the airport.Monitors daily arrivals and ensures accommodations are prepared prior to check in.Ensures the Lexus app is filled out and complete per our Lexus partnership.Audits daily arrivals and departures to ensure accurate guest flight information.Provide feedback to the team, both positive and constructive, to ensure we are hitting our targets.Analyze guest feedback and provide strategic direction to improve overall rating.First point of contact for guest feedback and service recovery situations. Must be comfortable accepting constructive feedback and correcting issues. Responsible for finding a solution for the guest to complete guest follow up.Positive attitude always, especially under pressure.Required skillsExcellent problem-solving and multitasking skills.Leadership skills along with the ability to motivate a team into high performance.Ability to work flexible hours and open availability.Strong sense of responsibility and a professional presentation.BS degree in Hospitality Management, Tourism, Business Administration or relevant field preferred.Valid State Drivers License (mexican).QualificationsRelevant work experience as a Guest Relations Manager, Hotel Manager, or similar role in a luxury environment.Understanding of all hotel management best practices and relevant laws.Hands-on experience with Hotel Management software (PMS).Proficiency in English; knowledge of other languages is a plus.Customer service drive with outstanding communication and active listening skillsHousing type-We offer housing for 3 months to allow them to settle in and establish their own place to live. Single occupancy room in The Junction apartment building. Bathroom in unit. Shared facilities (kitchens, laundry), free wifi.-$350 per month ($175 deducted from payroll every 2 weeks). $300 deposit ($100 deducted from payroll for the first 3 paychecks)Additional commentsWe require that they have a drivers license for at least 2 years and a clean motor vehicle report so that they can drive our vehicles while theyre in the process of getting their MT license.For all TN candidates this is the expectation: They will rent a car or rent via Turo (doesnt require a US drivers license) until they are able to purchase their own vehicle.Gas station, convenience store, and bar located next to the apartment building. Ten minute drive to The Resort. Twenty minute drive to the town of Seeley Lake for groceries, restaurants, etc.</v>
+      </c>
+      <c r="F47" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-front-office-manager-luxury-resort-en-los-cabos-FB9346232B413B5761373E686DCF3405#lc=ListOffers-Score3-5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Upper or Lower Elementary English CoTeacher - Hiring for August 2025</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Escuela John F Kennedy</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Querétaro, Querétaro</v>
+      </c>
+      <c r="D48" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E48" t="str">
+        <v>JOB OPENING!With an over 60-year tradition educating the future leaders of Mexico, John F. Kennedy - The American School of Querétaro is an innovative bilingual K-12 school in central México accredited by the International Baccalaureate Organization (IB), AdvancED (United States), and the Secretaría de Educación Pública (SEP) that serves over 1,400 students from over 28 countries.If you are for an engaging, creative and innovative ENGLISH CO-TEACHER FOR UPPER OR LOWER GRADES interested in an opportunity regarding an innovative environment, following the highest education standards, employing emerging technologies in a multicultural atmosphere share with us your information!About the job…-We are looking for an experienced Elementary School Educator willing to co-teach with the head teacher connecting with students from upper grades offering creative, dynamic and motivating classes using “out-of-the-box” learning strategies.Requirements…- Bachelor’s Degree in Education, Psychology, Pedagogy or related to education, (Title and professional license needed)- Full command of English is required.- Experience working with upper or lower elementary schoolers in English, math, sciences, social studies, etc.- Highly PassionateIf you look for your next professional challenge, please send us your resume as soon as possible, this is an immediate hiring.</v>
+      </c>
+      <c r="F48" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-upper-or-lower-elementary-english-coteacher-hiring-for-august-2025-en-queretaro-10919CC043D3788661373E686DCF3405#lc=ListOffers-Score3-6</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Frontend Developer - React</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Asteci</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D49" t="str">
+        <v>$ 29,181</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Consultora de TI con diversos clientes a nivel nacional e internacional solicita:Front end Web Developer enfocado al desarrollo moderno con sólida experiencia en React JS, Java Script, Type Script.Requisitos:Lenguajes: JavaScript, TypeScriptFrameworks: ReactJS, NestJS, NextJSJest, testing en general.Uso de patrones de diseño.Seguridad: Fortify, Checkmarx, BlackduckHerramientas CI: Jenkins, Git, GitFlow, Bitbucket, JIRA, Confluence, SonarObservabilidad: Dynatrace, SplunkMetolologías Agil, Scrum.Conocimiento de Desarrollo e Integración con REST APIs.Inglés 80%.Actividades:Diseño, desarrollo, integración, pruebas e implementación eficaces de requisitos empresariales complejos.Aplicación de conocimientos tecnológicos al diseño de modelos y/o sistemas, formulación de diseños técnicos detallados, investigación y recomendación de soluciones técnicas, desarrollo y entrega de aplicaciones mediante metodologías de desarrollo ágil.Capacidad para trabajar al más alto nivel técnico en el desarrollo de sistemas, manteniendo un sólido conocimiento de las estrategias y aplicaciones empresariales de gestión patrimonial.Liderazgo técnico, coordinación entre laboratorios, soporte a la producción y soporte a la implementación de versiones.Ofrecemos:Salario competitivo.Prestaciones de Ley.Seguro de gastos médicos menores y mayores.Esquema hibrido.Apoyo económico por teletrabajo.INTERESADOS FAVOR DE POSTULARSE ATRAVES DE ESTE MEDIO PARA AGENDAR UNA ENTREVISTA DE TRABAJO.</v>
+      </c>
+      <c r="F49" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-frontend-developer-react-en-miguel-hidalgo-BD73961FFBEA7F7161373E686DCF3405#lc=ListOffers-Score3-7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Mid Level or Senior Full Stack Developer .NET C# Angular Java</v>
+      </c>
+      <c r="B50" t="str">
+        <v>LOGOS Virtual Assistants LLC</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Estados Unidos</v>
+      </c>
+      <c r="D50" t="str">
+        <v>$1,600</v>
+      </c>
+      <c r="E50" t="str">
+        <v>LOGOS Virtual Assistants is looking for a bilingual English, Full Stack Developer, to work on a medium-long-term project with a U.S. client.The project revolves around a large U.S. healthcare insurance provider, with multiple requirements for:- Supporting Role to the Design/Architecture team- Troubleshooting- Fixing Bugs/Debugging- Implementing new change requests for ongoing development on the existingtech stack.- Analytical Skills---------------------------------------------Essential Tech Stack Skills:The position will lean towards:- 70% Java competency (More work to be done on the Java side)- 30% .NET/C# competency-------------------------------------------Ideal years of experience with tech stack:- Java = [3-5+ Years]- .NET/C# = [3-4+ Years][Ideally in some web development part of .NET (MVC, Razor, Asp.net, etc)- Angular = [3-4 + Years](Multiyear experience with some version of Angular is a MUST. Great if the candidate has some Angular.Js experience, version 1.0)This is an opportunity to work in an English-based environment directly with a US-based IT Consultancy, managing large project requirements for a large healthcare provider supporting government programs such as Medicare/Medicaid.-------------------------------------------Compensation Range:- The position will pay according to experience and also English strength.- Pay is in USD- Pay range would be between $1,600-$3,100 USD, per month, as a fixedmonthly salary. [$28,800-$55,9550 MXN estimate]---------------------------------------------Next Steps:- CVs must be in English- Once your application is received, I will reach out to you directly to schedulean interview with CEO of Logos Virtual Assistants.- If selected, a 2nd short interview with the client.- If selected for final stage, a 3rd interview, which would take about 2-3 hours.- Formal offer will be made if successfully selected.We are looking to make the placement for a start date in middle to late July. We're able to move fast as long as the candidate is available. We anticipate a decision within 2-3 weeks.</v>
+      </c>
+      <c r="F50" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-mid-level-or-senior-full-stack-developer-net-c-angular-java-en-estados-unidos-5F51DB72EBC7E61E61373E686DCF3405#lc=ListOffers-Score3-8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Digital Marketing Specialist</v>
+      </c>
+      <c r="B51" t="str">
+        <v>ALTA INFRAESTRUCTURA Y CONSTRUCCION</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D51" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E51" t="str">
+        <v>We’re Hiring a Digital Marketing Specialist! | IA RemodelingOn-site | Full-Time | Growth-Focused EnvironmentAre you a results-driven marketer with a passion for paid ads, automation, and data? Want to join a fast-growing team in the remodeling &amp; construction space where your creativity and tech skills drive real impact?At IA Remodeling, we don’t just build spaces—we build opportunity. And right now, we’re on the hunt for a Marketing Specialist who’s ready to take our lead generation engine to the next level — on-site with our energetic and collaborative team.What You’ll DoCreate, manage, and optimize advertising campaigns across Meta (Facebook &amp; Instagram) and Google Ads platforms in USA markets.Build and optimize landing pages for campaigns, focusing on conversion rates and user experience.Install and configure tracking pixels (Meta Pixel, Google Tags) to ensure accurate campaign tracking and reporting.Integrate email marketing systems (such as Mailchimp, Klaviyo, or similar) to automate customer journeys and nurture leads.Set up and manage CRM systems to organize leads, customer data, and sales pipelines (e.g., HubSpot, GoHighLevel, Salesforce).Monitor campaign performance, analyze metrics, and provide actionable insights to improve results.Collaborate with design, sales, and operations teams to align marketing initiatives with business goals.What We’re Looking ForBilingual or Advanced English.Minimum 2+ years of experience in digital marketing, with a focus on paid ads in the USA markets, landing pages, CRM, and email marketing.Proven experience managing paid ads inside Meta and Google platforms, optimizing conversion campaigns (CTA, PPC).Experience managing a budget of +10 K USD/month.Experience building high-converting landing pages (WordPress, ClickFunnels, Webflow, or similar tools).Notions of AI tools for design is a plus.Strong understanding of pixel installation, event tracking, and retargeting strategies.Experience with email marketing setup, automation, and performance tracking.Hands-on experience setting up and managing CRMs and marketing automation tools.Analytical mindset with strong attention to detail.Ability to work in a fast-paced environment and manage multiple projects simultaneouslyThink you’re a great fit? Apply now and let’s build something amazing—together, in person.</v>
+      </c>
+      <c r="F51" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-digital-marketing-specialist-en-benito-juarez-54BE2B3D1FB6315F61373E686DCF3405#lc=ListOffers-Score3-9</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Ingeniero Programador Sr. JAVA</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Importante empresa del sector</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Benito Juárez, Ciudad de México DF</v>
+      </c>
+      <c r="D52" t="str">
+        <v>$ 25,000.00</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Vacante: Ingeniero Programador Full StackUbicación: Instalaciones de CFE – Av. Cuauhtémoc, Col. del ValleHorario: Lunes a viernes de 8:00 a 18:00 hrsSomos una empresa líder en el sector de Telecomunicaciones con más de 35 años en el mercado. Estamos en búsqueda de talento comprometido y con iniciativa para integrarse a nuestro equipo como Ingeniero Programador Full Stack.?Perfil RequeridoEscolaridad:Ingeniería en Sistemas o carrera afínRequisitos:Actitud proactiva y disposición para aprenderCompromiso y puntualidadHabilidad para trabajar en equipo y liderar proyectosDisponibilidad de horarioCertificación en Java (en caso de no contar con ella, se deberá obtener con el conocimiento para poder certificarse estando dentro de la empresa)Conocimientos Técnicos:Angular, Next. js, React, Node. jsAdministración de servidores (Windows y Linux)SQL Server, PostgreSQLAnálisis, diseño e integración de bases de datosDesarrollo de interfaces front-endIdentificación de comportamientos anómalos en sistemasContenedores Docker y servicios en la nubeFunciones Principales:Desarrollo de reportes personalizados mediante consultas SQLOptimización y mantenimiento de bases de datosImplementación y modificación de APIs (Java, Angular, Node)Administración de servidores y esquemas de alta disponibilidad (HA / Always On)Diseño y desarrollo de arquitecturas de bases de datosSoporte en infraestructura sobre sistemas operativos Windows y LinuxOfrecemos:Sueldo mensual de $24,000 a $25,000 en esquema mixto (parte nominal y parte facturada)Prestaciones de leyApoyo de despensa mensual de $850Dos seguros de vidaContrato directo con la empresaOportunidad de obtener certificaciones relevantes en el área de telecomunicacionesSi cumples con el perfil y estás interesado en desarrollar tu carrera en una empresa sólida, postúlate enviando tu CV actualizado.</v>
+      </c>
+      <c r="F52" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-ingeniero-programador-sr-java-en-benito-juarez-0DEDD414D2FD95C561373E686DCF3405#lc=ListOffers-Score3-10</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Convocatoria de Becarios Networking - Anzures</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Probecarios</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D53" t="str">
+        <v>$ 4,700.00</v>
+      </c>
+      <c r="E53" t="str">
+        <v>CONVOCATORIA DE BECARIOS NETWORKING – Anzures“Te invitamos a participar en nuestro programa de becarios y poner en práctica tus conocimientos en una gran empresa que ha coleccionado los sellos discográficos más importantes en la historia de la música”Requisitos del ProgramaEstar cursando los primeros semestres de cualquier carrera universitariaTener disponibles los martes por la mañanaInglés Básico - IntermedioExcel Intermedio (gráficas, fórmulas, tablas)Excelente actitud, dinamismo, facilidad para comunicarse en públicoActividadesNextGen es el semillero de talento de Warner Music México, un programadiseñado para estudiantes universitarios de distintas carreras, semestres y áreas deconocimiento que desean vivir la industria musical desde adentro.Durante el programa, los participantes colaboran en equipos multidisciplinariospara desarrollar un proyecto con enfoque en el negocio de la música. A lo largodel camino, viven experiencias formativas, sesiones con especialistas y dinámicasinteractivas que les permiten conocer de cerca el funcionamiento de la industriadel entretenimiento y los roles clave dentro de una compañía global comoWarner.Aprenden directamente de personas expertas en áreas como A&amp;R, Marketing,Comercial y más, y reciben retroalimentación de ejecutivos al presentar suspropuestas. Es un espacio dinámico, creativo y flexible, que fomenta elpensamiento innovador, el trabajo colaborativo y el desarrollo profesional de lapróxima generación de líderes en la música.BeneficiosBeca mensual: $4,700 netos + TDU + Seguro contra accidentes + Mochu University (cursos para el desarrollo de Soft y Hard Skills) + Posibilidad de liberar trámites escolaresHorario: Únicamente se acude los martes de 11:00 am a 1:00 pm (modalidad 100% presencial)Periodo: 6 meses (es importante ser estudiante universitario durante este periodo)Zona: Calle Leibnitz No. 32, Col. Anzures, Alcaldía Miguel Hidalgo, CP 11590, CDMX</v>
+      </c>
+      <c r="F53" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-convocatoria-de-becarios-networking-anzures-en-miguel-hidalgo-BC2FCB37B1F2B3B261373E686DCF3405#lc=ListOffers-Score3-11</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Arquitecto software</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Asteci</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Miguel Hidalgo, Ciudad de México DF</v>
+      </c>
+      <c r="D54" t="str">
+        <v>$ 29,181</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Consultoría especializada en TI con clientes a nivel nacional e internacional está en búsqueda de:Arquitecto de Software con sólida experiencia en desarrollo de soluciones modernas y escalables. El perfil ideal debe dominar múltiples tecnologías frontend y backend.Requisitos:+8 años de experiencia en desarrollo de softwareJavaScriptTypeScriptReact JSJavaKotlinNode.jsPythonDesarrollo de aplicaciones nativas (Android/iOS)Manejo de herramientas como Bitbucket, JIRA, y ConfluenceExperiencia con KafkaFrameworks como NestJS y Next.jsOfrecemos:Salario competitivo.Prestaciones de Ley.Seguro de gastos médicos menores y mayores.Esquema hibrido.Apoyo económico por teletrabajo.INTERESADOS FAVOR DE POSTULARSE ATRAVES DE ESTE MEDIO PARA AGENDAR UNA ENTREVISTA DE TRABAJO.</v>
+      </c>
+      <c r="F54" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-arquitecto-software-en-miguel-hidalgo-9EBC11EFF84132A361373E686DCF3405#lc=ListOffers-Score3-12</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Diseñador/a industrial - Diseñador industrial retail</v>
+      </c>
+      <c r="B55" t="str">
+        <v>NEXT IMPULSE</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Metepec, Estado de México</v>
+      </c>
+      <c r="D55" t="str">
+        <v>$ 21,000.00</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Realizar, gestionar y supervisar todos los procesos de diseño desde su concepción creativa, hasta la entrega de muestras a cliente para su aprobación. Se requiere un profesionista proactivo, con alta capacidad de programación de proyectos y toma de decisiones, con experiencia en el ramo de marketing, diseño de displays para empresa enfocada a clientes AAA.PERFIL PROFESIONAL:-Experiencia en MATERIAL POP (EXHIBIDORES)-Licenciatura terminada en Diseño Industrial-Modelado 3D (SolidWorks) y Renderizado (Keyshot) INDISPENSABLE-Paquetería de Adobe Creative (Photoshop e Illustrator) INDISPENSABLE-Paquetería Office con Excel indispensable-Realización de planos para producción y conocimiento de materiales como: alambre, lámina, madera y plástico.-Ingles básico-intermedio-Conocimiento en impresión digital y corte-Experiencia 2 años comprobablesRESPONSABILIDADES DEL PUESTO:-Generación de propuestas de diseño para clientes de exhibidores, puntos de venta y displays-Modelar, renderizar y realizar planos para producción con especificaciones.-Dar seguimiento a la producción de diseños-Realizaciòn de planos de producción y especificaciones-Revisión y ajuste de muestras-Realización de cotizaciones de los diseños, despiece y análisis de costos de materiales-Programación de producción y coordinación de equipo de impresión, corte y doblez.-Calcular tiempos de producción, volumen de materia prima y coordinación con gerencia de planta.-Propuesta de artes o modificación de archivos para impresión, con base en las necesidades de los clientes-Autorización de artes y renders; Solicitud de fabricación de muestras para aprobación de los clientes-Seguimiento de producción y supervisión de calidad-Propuestas sobre identidad corporativa y empaques*QUE RADIQUE EN TOLUCA, METEPEC O ALREDEDORES, O ESTÉ DISPUESTO A VIAJAR DIARIAMENTE O TENER CAMBIO DE RESIDENCIA A METEPEC.</v>
+      </c>
+      <c r="F55" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-disenadora-industrial-disenador-industrial-retail-en-metepec-D5FA24952BA7F2F461373E686DCF3405#lc=ListOffers-Score3-13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Camarista - $9,000.00 pesos + propinas</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Next Hub Hotel</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Zapopan, Jalisco</v>
+      </c>
+      <c r="D56" t="str">
+        <v>$9,000.00</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Ven y forma parte del mejor hotel en toda la Zona Centro de Zapopan -Hotel NEXT-Como parte de nuestro equipo en la posición de CAMARISTA A.P. tus responsabilidades serán:Limpieza de áreas publicas.Limpieza de habitaciones (2 días mínimo).Reporte de incidencias en habitaciones.Cuidado de los equipos y suministros del hotel.Atención a huéspedes en cuestiones de limpieza y suministros.Atención a eventualidades de la operación diaria.Inventarios mensuales.Atención a proveedor de Lavandería.Deberás contar con:Secundaria terminada,Disponibilidad para laborar fines de semana,Experiencia comprobable en el puesto o afín de al menos 2 años.Atención al detalle.Habilidad para trabajar bajo presión.Habilidad para trabajar en equipo.Facilidad de palabra.Horario laboral de 8:00am a 4:00pm (30min. de alimentos), de lunes a domingo con un descanso entre semana. El horario puede negociarse de 7:00am a 3:00pmContáctanos o visítanos hoy en Hotel Next para hacer una cita de entrevista en horario de 8am a 5pm.</v>
+      </c>
+      <c r="F56" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-camarista-900000-pesos-propinas-en-zapopan-38C5BDE8D3A9485E61373E686DCF3405#lc=ListOffers-Score3-14</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Contador - Bilingüe</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Uplift Talent</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Guadalajara, Jalisco</v>
+      </c>
+      <c r="D57" t="str">
+        <v>$ 30,000.00</v>
+      </c>
+      <c r="E57" t="str">
+        <v>At Uplift Talent, we are seeking a detail-oriented Accountant to join our dynamic team. This is an excellent opportunity for someone passionate about high-quality accounting standards and looking to take the next step in their career with US-based teams.JOB DESCRIPTIONThe Accountant is responsible for overseeing financial transactions, maintaining accurate financial records, preparing financial reports, and ensuring compliance with accounting principles and regulations. They will analyze financial data to provide insights and recommendations to management, as well as assist with budgeting and forecasting processes.RESPONSABILITIES:-Maintain general ledger accounts by verifying, allocating, and posting transactions.-Prepare and analyze financial statements, including balance sheets, income statements, and cash flow statements.-Reconcile financial discrepancies by collecting and analyzing account information.-Ensure compliance with accounting standards, regulations, and company policies.-Assist with budgeting and forecasting processes, providing input and analysis as needed.-Prepare and file tax returns and ensure compliance with tax regulations.-Assist with internal and external audits by providing necessary documentation and explanations.-Analyze financial data and provide insights and recommendations to management.-Monitor financial transactions and recommend improvements to processes and procedures.-Develop and maintain financial databases and spreadsheets.REQUIREMENTS:-Bachelor's degree in Accounting, Finance, related field or equivalent experience.-3+ years experience as an accountant or similar role.-US accounting or finance experience-Excellent knowledge of accounting regulations and procedures, including the -Generally Accepted Accounting Principles (US-GAAP).-Proficiency in accounting software and MS Office, particularly Excel.-Excellent analytical skills and attention to detail.-Strong communication and interpersonal skills.-Ability to prioritize and manage multiple tasks efficiently.-Experience with budgeting, forecasting, and financial analysis.-Familiarity with tax laws and regulations (US based)Salary Range: $30,000 - $40,000 MXN/monthReady to advance your accounting career in a collaborative and growth-focused environment? Apply now and be part of Uplift Talent’s success story!!</v>
+      </c>
+      <c r="F57" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-contador-bilingue-en-guadalajara-448AEB75A2F7079B61373E686DCF3405#lc=ListOffers-Score3-15</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Data Engineer</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Jato Dynamics</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Cuajimalpa de Morelos, Ciudad de México DF</v>
+      </c>
+      <c r="D58" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E58" t="str">
+        <v>About us:JATO Dynamics is a global company and the leading provider of automotive market intelligence. With an insight into over 50 overseas markets, we deliver the world's most complete, accurate and up-to-date automotive data and insights, creating significant competitive advantage to our customers.Role Overview:Do you want to be part of building out next generation SaaS products that power the automotive industry?JATO is currently looking to hire a Data Engineer to join our agile teams. As a Data Engineer, you will work in a product delivery team using your data analysis, ETL and cloud technology skills to discover, model, provision and store data at scale in the cloud.Key Responsibilities:Ingest, warehouse, and store data at scale in the Azure cloud platformWork closely with colleagues in Operations, Architecture, Delivery, Product, and Software Engineering to collaboratively release platform incrementsContribute toward solution level architecture and designOwn your release from development to production following DevOps methodContribute towards ADF and Synapse pipeline design improvement and best practices and following design principlesUnderstand data issues and able to analyse and work with Architects in addressing design challengesAble to migrate data from legacy databases and storage to Azure cloud-based lake and warehouseKey Requirements:Minimum 3+ years’ experience designing and developing complex ETL/ELT pipelines in the cloud (Azure Data Factory or Azure Synapse)Experience of preparing data maps based on high level requirements and taking those to a solution level detailsFirm understanding of data warehousing concepts in the lake and traditional database with experience of working from landing to the reporting layerKnowledge and experience in value-added areas of automation, scriptingKnowledgeable about the different types of cloud-based storage resources and distributed systemsRelational databases (SQL Server, MySQL etc.), NoSQL and writing queriesHands-on analytical, visualisation and exploration skillsExperience of working in Agile methodologyExperience of working with API’s and good knowledge of API-based Integration and Microservices architecturePractical experience of improving data quality and efficiencySolid understanding of DevOps and CI/CDUnderstanding of compliance and lifecycle of data managementCoding experience in any relevant language (Python, Pyspark etc.)Strong communication skills in EnglishExperience collaborating with multinational teamsPlease be aware that this position requires fluency in English, kindly submit your application in English.JATO Dynamics is a global business and our success is attributed to the diversity, skills and experiences of our colleagues across the world. We are proud to be an equal opportunity employer and are committed to equal employment opportunity regardless of race, sex, age, gender identity, sexual orientation, religion or belief, disability, marital status or veteran status.</v>
+      </c>
+      <c r="F58" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-data-engineer-en-cuajimalpa-de-morelos-F72CA035896C536061373E686DCF3405#lc=ListOffers-Score3-16</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Project Engineer - Experiencia en industria de la construcción</v>
+      </c>
+      <c r="B59" t="str">
+        <v>MPI</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Guadalajara, Jalisco</v>
+      </c>
+      <c r="D59" t="str">
+        <v>$ 21,000.00</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Specific tasks or activities:1. Planning and CoordinationConfirm attendance and issues to be discussed at meetings with the Project Manager (PM) and the Supervisor (Superintendent).Participate in regular meetings with the General Contractor to discuss project scheduling.Organize and coordinate the tasks of subcontractors together with the Project Manager.Request a detailed schedule covering the next three weeks from the General Contractor.Manage and update the project schedule.Create the Survey Request and send it to the contractor2. Communication and CoordinationPrepare weekly reports detailing the quantities of material and work performed.Create and maintain a list of key HLE (High Light Electric) contacts for the General Contractor in collaboration with the Project Manager.Write serial letters that can be used for formal communication.Prepare a monthly report summarizing the amounts of work performed and a cost analysis.3. Project Documentation ManagementManage the lifecycle of the corresponding documentation for each of the projects in ClickUp and PROCORE (USA Tickets, RFI, DCR, METS, etc.)Monitor the USA ticket system to identify issues or pending requests.Manage and update tasks related to the Project Final Estimate (PFE) in ClickUp and PROCORE.Create a task in ClickUp and PROCORE to manage RFI tracking and store relevant information in SharePoint.Create the respective submittals for each project in collaboration with the Project Manager.Creation of Change Order Management together with the Project Manager.4. Quality Control and Collaboration with the FIELDMonitor and review the quality of daily work based on the record of daily reported hours (DCR).Review and update plans based on work actually performed on site (ASBUILTS).Prepare and submit requests for quality reviews by the Materials and Equipment Survey System (METS).Generate a list of all submissions made and document Quality Verified (QV) specifications.5. Cost Management and Control.Request and follow up with the Project Manager on quotes for the acquisition of additional materials for work (Extra Work Material Order, EWB)Supervise and manage, together with the Project Manager, the balance and details of purchase orders (PO) and materials, tools, and equipment (MPO).Verify and approve invoices related to the purchase of materials and prepare cost analysis reports (with information approved by the inspector).Monitor costs associated with equipment and materials rentals and report variances to the Project Manager.Prepare and submit payment estimates to contractors and suppliers, with review by the Project Manager prior to submission.Control the material at the project work site for proper use.6. Change and Dispute ManagementSupport, when required by the Project Manager, in drafting a preliminary Notice of Opportunity for Change (NOPC) document.Assist in the calculation and documentation of estimated costs associated with the implementation of proposed changes to the NOPC for Project Manager approval.Support the Project Manager in drafting the documentation package required for an arbitration or Dispute Resolution Board (DRB) process.Monitor and manage costs associated with project disputes or claims.Managing the identification of Request for Information (RFI) to the General Contractor, as well as preparing and submitting the necessary documentation for RFI approval.Creating a cost proposal based on an analysis generated by the Assistant Project Manager and the Project Manager, managing follow-up and actions to be taken based on the cost proposal.</v>
+      </c>
+      <c r="F59" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-project-engineer-experiencia-en-industria-de-la-construccion-en-guadalajara-BF197E30DB35B40061373E686DCF3405#lc=ListOffers-Score3-17</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Especialista de Marketing - Paid Media</v>
+      </c>
+      <c r="B60" t="str">
+        <v>GoStrategy</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Venezuela</v>
+      </c>
+      <c r="D60" t="str">
+        <v>$ 60,000.00</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Especialista de Marketing - Paid MediaModalidad 100% Remota | Full Time (Zona Horaria Argentina)Nuestro Cliente: Una agencia de marketing digital especializada en performance y paid mediaestá buscando sumar a su equipo un/a Analista de Campañas Sr. que garantice los resultadosque esperan sus clientes a través del análisis, planeación, implementación y seguimientoconstante de estrategias y campañas.Este rol tiene como principal objetivo liderar la estrategia y performance de las cuentasasignadas, acompañando a un equipo de Account Strategists para maximizar el impacto decada acción.Buscamos a alguien que sea…Proactivo, con mentalidad estratégica y enfoque 100% en resultados.Apasionado por los datos, las métricas y la optimización constante.Capaz de anticiparse a los problemas y proponer soluciones creativas y efectivas.Con vocación de liderazgo para guiar y potenciar a su equipo.Responsabilidades claveIdentificar necesidades, oportunidades y desafíos de cada cuenta.Planificar y coordinar estrategias de medios alineadas a los objetivos del cliente.Armar y supervisar la correcta implementación del plan de medios.Liderar la gestión y optimización de campañas SEM.Detectar oportunidades de up selling / cross selling.Crear informes de resultados con análisis cualitativo y cuantitativo.Presentar propuestas estratégicas a clientes actuales y potenciales.Coordinar con diseñadores, proveedores y otros partners externos.Construir relaciones sólidas con los stakeholders de cada proyecto.Capacitar y acompañar el desarrollo de su equipo de Account Strategists.Requisitos técnicos:+2 años de experiencia gestionando campañas SEM.Sólido manejo de Google Ads y Meta Ads.Dominio de GA4, Google Merchant Center Next y Looker Studio.Experiencia en campañas full funnel.Alta capacidad de análisis y optimización basada en datos.Manejo avanzado de Excel/Spreadsheets.Creación de reportes automatizados.Deseables / Plus:Search Ads 360 y Amazon AdsFirebase, Adjust o AppsflyerCampañas en Bing AdsCertificaciones Google Ads / GA4Conocimientos en GTM y sistemas de atribución (Floodlights, etc.)Experiencia liderando equipos y/o formando colegasSkills clave que valoramos:Pensamiento analítico y enfoque a resultadosCapacidad de planificación y ejecuciónLiderazgo y acompañamiento de equiposResolución de problemasComunicación clara y efectivaFlexibilidad y adaptabilidad al cambioModalidad y beneficiosJornada Full Time (Argentina): lunes a viernes de 08:00 a 17:00 o de 09:00 a 18:00100% remotoSalario 700 dlsViernes flex todo el añoDía de cumpleaños libreDía libre en tu aniversario laboralAcceso a capacitaciones internas y a plataforma Platzi</v>
+      </c>
+      <c r="F60" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-especialista-de-marketing-paid-media-en-venezuela-E9CC7E5CE22CB80861373E686DCF3405#lc=ListOffers-Score3-18</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Senior Software Developer - Freelance</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Ciudadela</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Colombia</v>
+      </c>
+      <c r="D61" t="str">
+        <v>No especificado</v>
+      </c>
+      <c r="E61" t="str">
+        <v>### Misión- Construye una plataforma que será utilizado por miles de usuarios- Trabaja con el equipo para crear herramientas que ayudan a escalar y automatizar una industria- Propón cambios que ayudan a la experiencia de desarrolladores### Beneficios- Trabajo remoto- Posibilidad de construir producto que va a ser utilizado inmediatamente por miles de usuarios### Requisitos- 5 años de experiencia- Typescript- Node.js- React- Graphql- API development- Git- Next.js- TDD with Jest- DockerN- Github actions- GCloud</v>
+      </c>
+      <c r="F61" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-senior-software-developer-freelance-en-colombia-2298B38A14D41E1E61373E686DCF3405#lc=ListOffers-Score3-19</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Sales Representative - Remote</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Nova NRG</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Cuauhtémoc, Ciudad de México DF</v>
+      </c>
+      <c r="D62" t="str">
+        <v>$ 16,000.00</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Nova NRG is more than just a solar sales company; we’re a powerhouse of innovation and ambition, headquartered in sunny Miami, Florida. Our mission is simple yet impactful: empower homeowners with clean, renewable energy solutions that save money and the planet.At Nova NRG, we celebrate ambition and hard work. Join a dynamic, supportive team that values your drive to succeed. Whether you’re an experienced pro or ready to take your sales career to the next level, we provide the tools, training, and incentives to help you thrive in the booming solar industry.Candidates must submit their CV in English to be considered for the position.What You’ll Do:* Use your persuasive communication skills to reach out to potential customers, introducing them to the exciting benefits of solar energy.*Book high-quality appointments for our expert solar consultants through effective cold calling and rapport-building.* Educate homeowners on solar solutions, answer questions, and create interest in sustainable energy.* Work closely with the sales team to ensure smooth transitions and contribute to team success in a high-energy, results-driven environment.What We Offer:* Salary base 800 USD monthly (paid weekly) + commissions.* Comprehensive training and mentorship to help you succeed and advance your career.* Exciting contests, incentives, and perks for top performers who go above and beyond.* Access to industry-leading software and technology to maximize your efficiency and success.* Join a vibrant, ambitious team where your achievements are celebrated.Qualifications:* Minimum of 2 years of cold calling or telemarketing experience, with a history of setting appointments or closing deals.* Fluent in both English and Spanish to connect with a diverse range of customers.* A driven individual passionate about exceeding targets and delivering exceptional customer service.* Strong interpersonal and negotiation skills to engage effectively in a fast-paced environment.* Motivated, ambitious, and eager to contribute to team success with a positive, can-do attitude.* Must have a reliable computer, headset, and stable internet connection to work remotely.Join Us and Unleash Your Potential!This is your chance to elevate your sales career with Nova NRG. Be part of a company that rewards ambition and hard work with unparalleled growth and financial success opportunities. Apply now to take the first step toward achieving greatness with us. Together, we’ll light up the future!</v>
+      </c>
+      <c r="F62" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-sales-representative-remote-en-cuauhtemoc-72D96FEC248FBE0A61373E686DCF3405#lc=ListOffers-Score3-0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Junior/Mid System Administrator - Full time, Hybrid, English</v>
+      </c>
+      <c r="B63" t="str">
+        <v>CloudSigma AG</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Guadalajara, Jalisco</v>
+      </c>
+      <c r="D63" t="str">
+        <v>$ 55,000.00</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Join the Future of Cloud Technology at CloudSigma!CloudSigma is a fast-growing provider of cutting-edge cloud solutions (IaaS, CaaS, and PaaS) serving businesses worldwide. As an industry leader, we’re expanding our talented team and looking for a Junior System Administrator to support our global infrastructure and contribute to the next phase of our growth.If you’re passionate about Linux, networking, cloud technologies, and incident management, and eager to work in a dynamic, international environment, we’d love to hear from you!Your Role &amp; Responsibilities:- Maintain and administer Linux and Unix-based physical and virtual servers across 20+ global locations.- Monitor systems, analyze logs, and manage incidents to ensure optimal performance and security.- Deploy, troubleshoot, and maintain applications in cloud and on-prem environments.- Support internal office infrastructure, test environments, and production systems.- Assist the support team in resolving issues beyond their competence and provide guidance on what information to collect for effective case resolution.What You Bring:* 1+ years of experience working with Linux/Unix-based systems (home projects, internships, or previous job).* Basic knowledge or exposure to virtualization technologies (KVM, VMware, or similar).* Interest or basic familiarity with container technologies like Docker or K8s.* Understanding of monitoring concepts — why systems need to be monitored and how incidents are managed.* Basic skills in installing and monitoring databases (such as PostgreSQL, MongoDB, or MySQL)* Experience working with incident management tools like Jira Service Management is a plus.* Awareness of Agile and Scrum methodologies is considered an advantage.* Fluent in English (both written and verbal).# Bonus Skills (a plus, but not required!):* Experience with Zabbix, Pingdom, ELK stack, or Grafana.* Experience with JIRA and Confluence.* Experience with version control systems like GIT or Mercurial.Who You Are:+ Highly detail-oriented and responsible.+ Well-organized with strong planning skills.+ A team player who thrives in a multilingual, collaborative environment.+ Comfortable working on shifts in a 24/7 environment.What We Offer:- Competitive salary &amp; attractive benefits package.- Dynamic international working environment with real growth opportunities.- Business mobile and laptop to support your work.- Hybrid work model – ability to work from home part of the time.- Friendly, informal, and knowledge-sharing work atmosphere.- A chance to build your career in one of the fastest-growing tech companies in the industry.Ready to take the next step in your cloud computing career? Apply now and grow with CloudSigma!</v>
+      </c>
+      <c r="F63" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-juniormid-system-administrator-full-time-hybrid-english-en-guadalajara-21BC17C91B4B27CF61373E686DCF3405#lc=ListOffers-Score3-1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>U.S. Hospitality Internship Program - Iintern/Trainee</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Kettelsen Consulting (TN Visa Advisors)</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Tlalnepantla de Baz, Estado de México</v>
+      </c>
+      <c r="D64" t="str">
+        <v>$ 60,000.00</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Unlock Your Potential with Our U.S. Hospitality Internship Program!We offer a broad portfolio of properties in the United States, including resorts, country clubs, and castles from the most recognized hotel brands in the industry. All our internships are paid, and you’ll have the opportunity to experience the culture and gain valuable experience in the hospitality industry. We’ll assist you throughout the J-1 visa process!Our program focuses on the Hospitality, Tourism, and Culinary sectors, offering operational and entry-level roles. Salaries are determined by the host company and will be specified in your internship offer.• Comprehensive Assessment and Guidance: Receive expert review of your resume, tailored interview coaching, and personalized job placement assistance to ensure a smooth entry into your internship role.• Pre-Departure and Immigration Support: Benefit from thorough pre-departure briefings and hassle-free immigration assistance, including visa applications and essential documentation.• Insurance and Ongoing Support: Enjoy insurance coverage throughout your internship and continuous support with regular online check-ins to monitor your progress and address any issues.• Online Orientation and Resources: Access an extensive online orientation program and resources to help you adapt quickly and effectively to life in the U.S.• Professional Networking: Connect with over 200 prestigious employers offering internships and trainee positions through our exclusive online portal.Placement Guaranteed for Qualified Candidates!Requirements• Educational Background: Open to current university students, recent graduates, or experienced professionals.• Field of Study or Experience: Relevant academic background or professional experience in hospitality, tourism, or culinary arts.• Language Proficiency: Conversational English proficiency required.• Age: Applicants must be between 18 and 30 years old.• Educational Institution: Must be enrolled in or have graduated from a university outside the United States.• Valid Passport: A valid, unexpired passport is required.• Professional Experience: For those graduated over 12 months ago, a certificate of employment in a relevant role is necessary. Professionals without a degree must show relevant full-time work experience.BenefitsWhy Choose Our Program?• Global and Cultural Enrichment: Enhance your personal and professional growth with a rich international and cultural experience.• Personalized Support: Receive dedicated assistance throughout your internship to ensure a successful and rewarding experience.• Career Opportunities: Potential for post-graduation employment under a professional work visa, such as the TN Visa.• Skill Development: Acquire valuable hands-on experience and improve your English skills, boosting your employability in the U.S. job market.Lifetime Network Access: Enjoy lifetime access to our expansive network of employers offering internships and trainee positions.Ready to take the next step in your career? Apply now and unlock a world of opportunities!</v>
+      </c>
+      <c r="F64" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-us-hospitality-internship-program-iinterntrainee-en-tlalnepantla-de-baz-46BD4B3BBBDAC70461373E686DCF3405#lc=ListOffers-Score3-2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Hyatt ServiceNow Engineer – React development and Custom Applications - Remote Opportunity – Valid U.S. visa requires</v>
+      </c>
+      <c r="B65" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D65" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E65" t="str">
+        <v>The OpportunityHyatt Hotels Corporation seeks an enthusiastic ServiceNow Engineer who is a passionate problem solver and delivers solutions to join our ServiceNow Department where you’ll join a team of seven ServiceNow professionals who love what they do. In this role, you will be collaborating closely with the broader Hyatt Financial Shared Services, IT teams, and non-IT teams where you’ll be instrumental in continuing to make Hyatt a leading hospitality company. With your abilities to research and understand new process and procedures along with your strong desire to learn, you’ll be developing, implementing, and migrating on a mature ServiceNow instance. You’ll use your deep understanding of ITSM core configurations, JavaScript, HTML while accurately breaking down tasks, unit testing, and delivering on time and in scope. You’ll be part of a team that is passionate about diversity, equity, and inclusion, is committed to nurturing curiosity and new skills with the ability to use feedback critical for growth, and building connections across the organization with stakeholders, colleagues, and guests.Who You AreAs our ideal candidate, you understand the power and purpose of our Culture of Care and embody our core values of Empathy, Inclusion, Integrity, Experimentation, Respect and Wellbeing. You enjoy working with a close fun team, are results driven, and want a variety of opportunities to develop personally and professionally.At Hyatt Hotels, ServiceNow is a major productivity solution and is a very important part of our mission to take care of people so they can be their best. ServiceNow Engineers serve on a professional deployment team to architect and deploy solutions within the ServiceNow platform for our Hyatt customers. Engineers provide administrative ServiceNow support, including troubleshooting, implementing bug fixes, and root cause analysis while using their ability to develop, configure, integrate, and/or implement with knowledge of the platform helping Hyatt keep up to date and enabling the best ServiceNow platform experience possible.Responsibilities:• Interact with customer team members to capture business requirements and translate them into appropriate technical solutions.• Commit to the continuous improvement and learning of development and ServiceNow best practices, tools, and technology• Support and develop in Hyatt’s custom Financial and Customer Service modules in ServiceNow• Responsible for providing accurate and up to date documentation on current ITSM processes or Custom Applications, using understandable business language• Monitors health, usage, and overall compliance of the ServiceNow platform• Works directly with ServiceNow Architect- IT and ServiceNow Manager to align the ServiceNow application with IT organization strategy• Works with key Financial Process Owners and leadership on priorities and being the main contact on the custom applications• The position responsibilities outlined above are in no way to be construed as all encompassing. Other duties, responsibilities and qualifications may be required and/or assigned as necessary• Occasions to create and lead Hyatt engineered Citizen Developer program• Opportunities to participate in Hyatt’s Diversity &amp; Inclusion activitiesQualificationsExperience Required:• 2-4+ years of work experience in ServiceNowExperience Preferred:• Bachelor’s degree in a related field however any combination of education, experience, and certification that demonstrates the candidate can be successful in the position is acceptable• Hands-on development experience with ServiceNow• Experience building ServiceNow solutions in non-IT contexts a plus• Strong working knowledge of ITIL practices• Web development experience using HTML5, CSS, JavaScript, Angular or React, and related technologies preferred• Knowledge of web services (SOAP, REST or JSON)• Exposure to integrating ServiceNow with other applications or databases.• Experience with ServiceNow’s Service Portal and CSM modules• Exposure to Configurable Workspaces and UI Builder• An interest in leveraging new features / technologies is critical• Ability to learn new technologies as they relate to the ongoing improvement of the ServiceNow platform• System analysis &amp; design skills, technical writing skills• Critical thinking and a desire to provide user friendly and professional platform to Hyatt internal customers is required• Experience with Agile (or Scale Agile Framework) project management processes a plus• Adaptable to change and able to work independently and as part of a team• Effectively manage multiple projects concurrently while maintaining a high level of attention to detail on each project• Strong communication skills (oral and written)• Ability to work with individuals across multiple functions• Ability to communicate with several senior leaders within the companyAdditional Comments and Requirements:• Valid USA Visa and Ability to travel worldwide on as as-needed basis for meetings and conventions is required (up to 10% of total work hours)• Provide ServiceNow support on-call outside normal working hours during ServiceNow upgrades, major platform incidents or events</v>
+      </c>
+      <c r="F65" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-hyatt-servicenow-engineer-react-development-and-custom-applications-remote-opportunity-valid-us-visa-requires-en-benito-juarez-6F05B66AA188529261373E686DCF3405#lc=ListOffers-Score0-3</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Junior Financial Data Analyst – Shared Services - Datamaster</v>
+      </c>
+      <c r="B66" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D66" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Vacante: Datamaster – Centro de Servicios Compartidos (SSC)Ubicación: Cancún Uno Office, Cancún, Quintana RooÁrea: Servicios Compartidos / Finanzas / DatosTipo de puesto: Tiempo completo | Nivel de entradaDescripción del puesto:Hyatt Hotels Corporation busca un/a Datamaster para unirse a nuestro Centro de Servicios Compartidos (SSC) en Cancún. Esta posición forma parte de un equipo dinámico que colabora con áreas como Contabilidad, Sistemas Corporativos y Operaciones Regionales, asegurando la integridad de los datos financieros y el cumplimiento de procesos clave.Responsabilidades principales:- Mantener y actualizar la estructura contable (Chart of Accounts) conforme a los estándares USALI.- Validar la consistencia de datos entre Oracle EBS y aplicaciones como Hyperion.- Procesar entradas contables automáticas y masivas.- Supervisar y validar datos maestros de proveedores y clientes.- Participar en iniciativas de mejora continua, calidad de datos y automatización.- Apoyar en reportes de desempeño relacionados con indicadores de nivel de servicio (SLA y KPIs).Requisitos:- Alta atención al detalle y habilidades organizativas.- Conocimiento de Excel y manejo de sistemas de datos.- Estudios en Contabilidad, Finanzas, Administración o carreras afines (deseable).- Deseable experiencia previa con Oracle EBS, Hyperion u otros sistemas ERP.- Deseable experiencia en hotelería o centros de servicios compartidos.Acerca de Hyatt:En Hyatt, nuestro propósito es cuidar a las personas para que puedan dar lo mejor de sí. Somos una compañía global en expansión que ofrece oportunidades reales de crecimiento. Formarás parte de una cultura que valora la inclusión, la integridad y la mejora continua.Postúlate hoy y sé parte de una organización reconocida como uno de los mejores lugares para trabajar.</v>
+      </c>
+      <c r="F66" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-junior-financial-data-analyst-shared-services-datamaster-en-benito-juarez-226C14A203EFF2BB61373E686DCF3405#lc=ListOffers-Score0-4</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Operador de Van de Turismo - Playa del Carmen</v>
+      </c>
+      <c r="B67" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Solidaridad, Quintana Roo</v>
+      </c>
+      <c r="D67" t="str">
+        <v>$ 13,200.00</v>
+      </c>
+      <c r="E67" t="str">
+        <v>En Amstar DMC buscamos tu talento como:Operador de Van de Turismo (Driver)Tu perfil:- Al menos 1 año de experiencia como operador de van.- Licencia federal AF.- Examen psicofísico vigente.- Preparatoria terminada.- Inglés básico - intermedio.- Disponibilidad de horario.- Sexo indistinto.- Folio de baja de la TIA.Ofrecemos:- Sueldo de $13,200 MXN brutos + propinas.- IMSS- 12 días de vacaciones.- 15 días de aguinaldo.- 25% de prima vacacional.- Vales.- Seguro de Vida.Tenemos vacantes en Playa del Carmen.</v>
+      </c>
+      <c r="F67" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-operador-de-van-de-turismo-playa-del-carmen-en-solidaridad-8731AD62FC18DDEC61373E686DCF3405#lc=ListOffers-Score0-5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Coordinador de Transporte para DMC - Playa del Carmen</v>
+      </c>
+      <c r="B68" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C68" t="str">
+        <v>Solidaridad, Quintana Roo</v>
+      </c>
+      <c r="D68" t="str">
+        <v>$ 18,000.00</v>
+      </c>
+      <c r="E68" t="str">
+        <v>En AMSTAR DMC !te estamos buscando¡ como Coordinador de Transporte para DMC que cumpla con el siguiente perfil:Objetivo:Asegurar que los conductores lleven a cabo los procedimientos establecidos para minimizar los riesgos de accidentes y brindar un excelente servicio a los clientes.Responsabilidades:• Realizar el horario de los operadores• Controlar la puntualidad y asistencia• Supervisar la presentación los operadores• Programar y supervisar la realización de diferentes cursos• Seguimiento al rendimiento de los controladores a través de Samsara• Coaching para operadores (reuniones uno a uno)• Evaluación del desempeño de los operadores• Seguimiento de las quejas que puedan realizar los clientes• Participar en reuniones semanales y/o mensuales tanto con el Supervisor de Conductores como con el Gerente de Transporte• Mantener reuniones con los conductores a su cargo• Realizar visitas de campo (Aeropuerto, Hoteles y Parking) para asegurar que los conductores realizan el procedimiento establecido.Perfil:• Experiencia en agencias de viajes o transportadoras, facilidad de palabra y manejo de personal, excelente actitud de servicio, conocimiento en tecnología (Computadora, Software y Smartphone, sistemas operativos), trabajo en equipo.• Conocimiento del destino, manejo de solución de situaciones con clientes no satisfechos, conocimiento de las ubicaciones y distancias entre Cancún y Riviera Maya, técnicas de gestión de conflictos para la atención al cliente.• Habilidades: Facilidad de comunicación, Efectividad en relaciones interpersonales, Facilidad de aprendizaje en uso de herramientas tecnológicas, supervisión de personal, realización de reportes.• Inglés intermedio deseable• Preparación académica: Bachillerato o Licenciatura.Ofrecemos prestaciones superiores a las de Ley, Seguro de Vida, GMM, buen ambiente de trabajo, facilidad de crecimiento.Sueldo mensual $18,000 brutosInteresados postularse por este medio con CV adjunto.</v>
+      </c>
+      <c r="F68" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-coordinador-de-transporte-para-dmc-playa-del-carmen-en-solidaridad-9B083E8567FDE50861373E686DCF3405#lc=ListOffers-Score0-6</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Process Compliance Supervisor - Hyatt Corporate Cancun</v>
+      </c>
+      <c r="B69" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D69" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E69" t="str">
+        <v>We're hiring!Join the Hyatt Inclusive Collection as a Process Compliance Supervisor and help shape the future of our Financial Shared Services operations.As a Process Compliance Supervisor, you will support the successful deployment, governance, and continuous improvement of our shared services model. Reporting to the Process Compliance Manager, this role is key to ensuring smooth transitions, optimizing processes, and driving operational excellence across the region.What you’ll do:• Supervise transitions to the Shared Services model with minimal disruption• Identify customer needs and recommend system/process adaptations• Monitor performance and suggest process enhancements• Support project resource selection and process documentation• Collaborate with SSC managers, peers, and process owners• Help develop and implement training programs• Coordinate strategy execution and maintain cross-functional alignment• Travel to SSC centers and hotel properties when neededWho you are:• 2+ years of experience in hotel finance or shared services• Bachelor’s degree in Accounting or Business• Proficient in English (B1 or higher)• Experienced with tools like Oracle EBS, Blackline, Opera, Excel, and Microsoft Office• Familiar with hotel month-end processes• Strong communicator with empathy, integrity, and a proactive mindset• Collaborative team player with leadership potential• Passionate about technology and process improvementLocation: Based in Mexico with occasional travelJoin a global brand that values innovation, collaboration, and growth.Apply now and be part of the transformation!</v>
+      </c>
+      <c r="F69" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-process-compliance-supervisor-hyatt-corporate-cancun-en-benito-juarez-8B4DC4D2CAFFFB6561373E686DCF3405#lc=ListOffers-Score0-7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Agentes Comerciales, Contratación y Gestión de Productos Turísticos (Esquema híbrido) - para cubrir incapacidad por maternidad de 3 meses</v>
+      </c>
+      <c r="B70" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D70" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E70" t="str">
+        <v>¿Te apasiona el turismo y cuentas con habilidades de organización, negociación y análisis?Esta oportunidad es para ti!Estamos en búsqueda de tres Commercial Agent B, responsables de negociar, ingresar y actualizar información de productos turísticos (excursiones, traslados, hoteles y suplementos) en nuestras plataformas. Tu trabajo impactará directamente en la expansión de nuestro portafolio y en la mejora de la experiencia de nuestros clientes internos.Modalidad híbrida – combinamos trabajo presencial y remoto para mayor flexibilidad y eficiencia.Funciones clave:- Negociación y contratación con proveedores de servicios turísticos.- Ingreso, actualización y estandarización de productos en plataformas digitales.- Seguimiento a cotizaciones y solicitudes de personalización.- Comunicación efectiva con áreas internas y proveedores.- Control y cumplimiento de KPIs de carga, calidad y tiempos.Lo que buscamos:- Licenciatura concluida.- Inglés intermedio.- Habilidad para análisis de información, planeación y captura de datos.- Experiencia en turismo (deseable) y manejo de plataformas (Zoho, iData, ResRap, ALMA).- Capacidad para trabajar bajo presión y en equipo.Ofrecemos:- Sueldo mensual y prestaciones superiores a la ley- Modalidad híbrida de trabajo.- Participar en un equipo dinámico y con visión de crecimiento.- Aportar directamente al éxito comercial de la empresa.- Oportunidades de aprendizaje en el sector turístico.Aplica aqui con tu CV actualizado. Te desemoa exito en tu busqueda de empleo.Our Destination is You!</v>
+      </c>
+      <c r="F70" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-agentes-comerciales-contratacion-y-gestion-de-productos-turisticos-esquema-hibrido-para-cubrir-incapacidad-por-maternidad-de-3-meses-en-benito-juarez-3016FF45ED5C000761373E686DCF3405#lc=ListOffers-Score0-8</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Hyatt ServiceNow Engineer – React development and Custom Applications - Remote Opportunity – Valid U.S. visa requires</v>
+      </c>
+      <c r="B71" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C71" t="str">
+        <v>Cuauhtémoc, Ciudad de México DF</v>
+      </c>
+      <c r="D71" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E71" t="str">
+        <v>The OpportunityHyatt Hotels Corporation seeks an enthusiastic ServiceNow Engineer who is a passionate problem solver and delivers solutions to join our ServiceNow Department where you’ll join a team of seven ServiceNow professionals who love what they do. In this role, you will be collaborating closely with the broader Hyatt Financial Shared Services, IT teams, and non-IT teams where you’ll be instrumental in continuing to make Hyatt a leading hospitality company. With your abilities to research and understand new process and procedures along with your strong desire to learn, you’ll be developing, implementing, and migrating on a mature ServiceNow instance. You’ll use your deep understanding of ITSM core configurations, JavaScript, HTML while accurately breaking down tasks, unit testing, and delivering on time and in scope. You’ll be part of a team that is passionate about diversity, equity, and inclusion, is committed to nurturing curiosity and new skills with the ability to use feedback critical for growth, and building connections across the organization with stakeholders, colleagues, and guests.Who You AreAs our ideal candidate, you understand the power and purpose of our Culture of Care and embody our core values of Empathy, Inclusion, Integrity, Experimentation, Respect and Wellbeing. You enjoy working with a close fun team, are results driven, and want a variety of opportunities to develop personally and professionally.At Hyatt Hotels, ServiceNow is a major productivity solution and is a very important part of our mission to take care of people so they can be their best. ServiceNow Engineers serve on a professional deployment team to architect and deploy solutions within the ServiceNow platform for our Hyatt customers. Engineers provide administrative ServiceNow support, including troubleshooting, implementing bug fixes, and root cause analysis while using their ability to develop, configure, integrate, and/or implement with knowledge of the platform helping Hyatt keep up to date and enabling the best ServiceNow platform experience possible.Responsibilities:• Interact with customer team members to capture business requirements and translate them into appropriate technical solutions.• Commit to the continuous improvement and learning of development and ServiceNow best practices, tools, and technology• Support and develop in Hyatt’s custom Financial and Customer Service modules in ServiceNow• Responsible for providing accurate and up to date documentation on current ITSM processes or Custom Applications, using understandable business language• Monitors health, usage, and overall compliance of the ServiceNow platform• Works directly with ServiceNow Architect- IT and ServiceNow Manager to align the ServiceNow application with IT organization strategy• Works with key Financial Process Owners and leadership on priorities and being the main contact on the custom applications• The position responsibilities outlined above are in no way to be construed as all encompassing. Other duties, responsibilities and qualifications may be required and/or assigned as necessary• Occasions to create and lead Hyatt engineered Citizen Developer program• Opportunities to participate in Hyatt’s Diversity &amp; Inclusion activitiesQualificationsExperience Required:• 2-4+ years of work experience in ServiceNowExperience Preferred:• Bachelor’s degree in a related field however any combination of education, experience, and certification that demonstrates the candidate can be successful in the position is acceptable• Hands-on development experience with ServiceNow• Experience building ServiceNow solutions in non-IT contexts a plus• Strong working knowledge of ITIL practices• Web development experience using HTML5, CSS, JavaScript, Angular or React, and related technologies preferred• Knowledge of web services (SOAP, REST or JSON)• Exposure to integrating ServiceNow with other applications or databases.• Experience with ServiceNow’s Service Portal and CSM modules• Exposure to Configurable Workspaces and UI Builder• An interest in leveraging new features / technologies is critical• Ability to learn new technologies as they relate to the ongoing improvement of the ServiceNow platform• System analysis &amp; design skills, technical writing skills• Critical thinking and a desire to provide user friendly and professional platform to Hyatt internal customers is required• Experience with Agile (or Scale Agile Framework) project management processes a plus• Adaptable to change and able to work independently and as part of a team• Effectively manage multiple projects concurrently while maintaining a high level of attention to detail on each project• Strong communication skills (oral and written)• Ability to work with individuals across multiple functions• Ability to communicate with several senior leaders within the companyAdditional Comments and Requirements:• Valid USA Visa and Ability to travel worldwide on as as-needed basis for meetings and conventions is required (up to 10% of total work hours)• Provide ServiceNow support on-call outside normal working hours during ServiceNow upgrades, major platform incidents or events</v>
+      </c>
+      <c r="F71" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-hyatt-servicenow-engineer-react-development-and-custom-applications-remote-opportunity-valid-us-visa-requires-en-cuauhtemoc-E28B3997C060D78C61373E686DCF3405#lc=ListOffers-Score0-9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>General Ledger and Income Journal Manager - Hyatt Corporate Cancun</v>
+      </c>
+      <c r="B72" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C72" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D72" t="str">
+        <v>$ 15,607</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Lead Financial Transformation at Hyatt – General Ledger &amp; Income Journal Manager (Shared Services) | CancunHyatt Inclusive Collection is seeking a results-driven finance leader to join our Shared Services Center in Cancun. This role offers a unique opportunity to lead the General Ledger and Income Journal functions, playing a key part in the transformation and optimization of financial operations across our hotel portfolio.Location: Cancun, MexicoIndustry: Hospitality / Hotels – Shared ServicesThe OpportunityAs the GL &amp; Income Journal Manager, you will lead a team responsible for delivering accurate and timely financial reporting by overseeing both daily revenue audit activities and General Ledger operations. You will be involved throughout the transformation lifecycle—from process design and implementation to stabilization and continuous improvement—while fostering collaboration with property finance teams and global stakeholders.Key ResponsibilitiesGeneral Ledger (GL)Lead the deployment and enhancement of GL processes under the Shared Services framework, ensuring minimal disruption to hotel operationsSupervise journal entries, account reconciliations, month-end closings, and internal reportingEnsure compliance with internal controls, corporate policies, and applicable regulationsManage a team responsible for financial transaction processing and general ledger accuracyAct as the main point of contact with hotel finance leaders to resolve escalations and strengthen service deliveryMonitor KPIs and implement initiatives for automation and operational efficiencyIncome Journal (Revenue Audit)Ensure daily hotel revenue transactions are accurately captured and reconciled with systems such as PMS and POSOversee the daily income audit process, including cash, credit card, and folio reconciliationValidate reports from Opera and other sources, ensuring alignment and identifying discrepanciesCollaborate with hotel teams to address issues and uphold revenue recognition standardsDeliver training and maintain SOPs to ensure consistency and high-quality outputTransformation &amp; LeadershipLead change management initiatives, including communication, training, and stakeholder engagementCollaborate with global Shared Services teams, including Hyatt’s corporate offices in Chicago, to ensure strategic alignmentTravel to hotel properties and delivery centers as needed to support transitions and strengthen relationshipsYour Background4+ years of experience in finance or accounting, with a strong focus on General Ledger and Income Journal functionsDemonstrated leadership experience in Shared Services or hotel finance environmentsBachelor’s degree in Accounting, Finance, or related fieldFluent in English and SpanishProficiency in ERP and hotel systems such as Oracle EBS, Opera, Blackline, or SAPStrong analytical mindset, process discipline, and leadership skillsWhy HyattLead a key function in a high-impact transformation across the Hyatt Inclusive CollectionJoin a globally recognized hospitality brand with a commitment to excellence and innovationCollaborate in a culture of integrity, care, and continuous improvementAccess to competitive compensation, international exposure, and professional development opportunitiesReady to shape the future of finance at Hyatt?Apply now with your updated resume.Care Connects Us!</v>
+      </c>
+      <c r="F72" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-general-ledger-and-income-journal-manager-hyatt-corporate-cancun-en-benito-juarez-3E6E6C390AA1EE0461373E686DCF3405#lc=ListOffers-Score0-10</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Encargado de Logística de Transportes Turisticos - Playa del Carmen</v>
+      </c>
+      <c r="B73" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Solidaridad, Quintana Roo</v>
+      </c>
+      <c r="D73" t="str">
+        <v>$ 18,000.00</v>
+      </c>
+      <c r="E73" t="str">
+        <v>En AMSTAR DMC !te estamos buscando¡ como Coordinador de Transporte para DMC que cumpla con el siguiente perfil:Objetivo:Asegurar que los conductores lleven a cabo los procedimientos establecidos para minimizar los riesgos de accidentes y brindar un excelente servicio a los clientes.Responsabilidades:• Realizar el horario de los operadores• Controlar la puntualidad y asistencia• Supervisar la presentación los operadores• Programar y supervisar la realización de diferentes cursos• Seguimiento al rendimiento de los controladores a través de Samsara• Coaching para operadores (reuniones uno a uno)• Evaluación del desempeño de los operadores• Seguimiento de las quejas que puedan realizar los clientes• Participar en reuniones semanales y/o mensuales tanto con el Supervisor de Conductores como con el Gerente de Transporte• Mantener reuniones con los conductores a su cargo• Realizar visitas de campo (Aeropuerto, Hoteles y Parking) para asegurar que los conductores realizan el procedimiento establecido.Perfil:• Experiencia en agencias de viajes o transportadoras, facilidad de palabra y manejo de personal, excelente actitud de servicio, conocimiento en tecnología (Computadora, Software y Smartphone, sistemas operativos), trabajo en equipo.• Conocimiento del destino, manejo de solución de situaciones con clientes no satisfechos, conocimiento de las ubicaciones y distancias entre Cancún y Riviera Maya, técnicas de gestión de conflictos para la atención al cliente.• Habilidades: Facilidad de comunicación, Efectividad en relaciones interpersonales, Facilidad de aprendizaje en uso de herramientas tecnológicas, supervisión de personal, realización de reportes.• Inglés intermedio deseable• Preparación académica: Bachillerato o Licenciatura.Ofrecemos prestaciones superiores a las de Ley, Seguro de Vida, GMM, buen ambiente de trabajo, facilidad de crecimiento.Sueldo mensual $18,000 brutosInteresados postularse por este medio con CV adjunto.</v>
+      </c>
+      <c r="F73" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-encargado-de-logistica-de-transportes-turisticos-playa-del-carmen-en-solidaridad-E56206E910028E8261373E686DCF3405#lc=ListOffers-Score0-11</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Representante de ventas en mesas de hospitalidad - En Cancún</v>
+      </c>
+      <c r="B74" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D74" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E74" t="str">
+        <v>Únete a nuestro equipo como Representante de Ventas en mesas de Hospitalidad en Cancún¡Estamos en expansión y buscamos talento como el tuyo! Si tienes habilidades en ventas, disfrutas el trato con clientes y quieres formar parte de una empresa en crecimiento, esta es tu oportunidad.Tu misión:Brindar un servicio de clase mundial a nuestros clientes y alcanzar altos volúmenes de venta, siempre reflejando nuestros valores y manteniendo una excelente imagen profesional.¿Qué harás?• Ofrecer una cálida bienvenida a los huéspedes en sus primeras 24 horas y establecer un contacto profesional.• Proporcionar información sobre nuestros productos y servicios, así como sobre las opciones disponibles en los hoteles.• Identificar y coordinar soluciones para situaciones que puedan afectar la experiencia del huésped.• Cumplir con las metas de ventas y procedimientos de reservación, cancelación y manejo de dinero.• Participar en viajes de familiarización, entrenamientos y actividades para fortalecer tu conocimiento del destino.• Mantener relaciones positivas con clientes, socios y colegas.• Elaborar reportes claros y precisos sobre las operaciones diarias.¿A quién buscamos?• Personas extrovertidas, con facilidad de palabra y pasión por el servicio al cliente.• Experiencia mínima de 1 año en ventas, servicio al cliente, mercadotecnia o relaciones públicas.• Habilidades en cierre de ventas, comunicación efectiva y uso de tecnología (terminales bancarias, software, smartphones).• Disponibilidad para turnos rotativos semanales según la zona asignada, con descanso entre semana.• Dominio del inglés en un 90%.• Bachillerato concluido o licenciatura.Lo que ofrecemos:Esquema de comisiones atractivo.Prestaciones superiores a la ley.Seguro de vida y gastos médicos mayores.Excelente ambiente de trabajo y oportunidades de crecimiento.Si cumples con el perfil, ¡postúlate enviando tu CV por este medio y forma parte de nuestro equipo!</v>
+      </c>
+      <c r="F74" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-representante-de-ventas-en-mesas-de-hospitalidad-en-cancun-en-benito-juarez-AD69CAE71123268A61373E686DCF3405#lc=ListOffers-Score0-12</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Representante de ventas en hoteles - En Playa del Carmen</v>
+      </c>
+      <c r="B75" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Solidaridad, Quintana Roo</v>
+      </c>
+      <c r="D75" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Por expansión, nos enconntramos en búsqueda de tu talento comoREPRESENTANTES DE VENTAS EN HOTELES en la Ciudad de PLAYA DEL CARMEN,Tu objetivo será:Prestar un excelente servicio de clase mundial a todos nuestros clientes, así como generar altos volúmenes de venta de acuerdo a las metas establecidas, cuidando la imagen y valores empresariales en todo momento.Tus responsabilidades serán:• Brindar un servicio de clase mundial (WCCS) a todos nuestros clientes de las diferentes cuentas que sirve la empresa.• Dar una presentación de bienvenida a la llegada de los huéspedes en sus hoteles estableciendo un contacto profesional con todos ellos en las primeras 24 horas de su llegada.• Proporcionar a los huéspedes en los hoteles información sobre los productos y servicios que nuestra empresa ofrece, así como también sobre servicios ofrecidos por los hoteles en donde estemos trabajando, sus políticas y procedimientos.• Reconocer situaciones que estuvieran afectando las vacaciones de los huéspedes, coordinando la implementación de soluciones efectivas con el personal del hotel si es posible o y reportando a la gerencia de la empresa y del hotel.• Lograr los objetivos y metas de ventas establecidas.• Cumplir con los lineamientos establecidos por la empresa sobre la reservación, venta, cancelación, reembolso, reportes de excursiones, y manejo del dinero.• Elaborar reportes exactos y precisos de acuerdo con las políticas y procedimientos establecidos.• Participar a todos los viajes de familiarización, excursiones y hoteles requeridos por la empresa.• Participar a todos los cursos de formación y entrenamiento requeridos.• Establecer y mantener excelentes relaciones con todos nuestros socios, colegas y clientes de acuerdo con las políticas establecidas.• Escribir reportes sobre asuntos que haya o pudieran impactar directa o indirectamente la vacación de los huéspedes en el hotel.Tu Perfil:• Extrovertido, facilidad de palabra y manejo de servicio a clientes, excelente actitud de servicio, conocimiento en tecnología (terminales bancarias, computadora, Software y Smartphone), buena presentación, trabajo en equipo.• Conocimiento del destino, experiencia mínima de 1 año en las áreas de servicio a clientes, ventas, mercadotecnia y/o relaciones públicas, Manejo de solución de situaciones con clientes no satisfechos.• Habilidades: Cierre de ventas, Facilidad de comunicación, Efectividad en relaciones interpersonales, Facilidad de aprendizaje en uso de herramientas tecnológicas (terminales bancarias, computadora, software y Smart phones)• Dominio del idioma inglés 90%.• Preparación académica: Bachillerato o Licenciatura.SUELDO BASADO EN COMISIONESOfrecemos prestaciones superiores a las de Ley, Seguro de Vida, GMM, buen ambiente de trabajo, facilidad de crecimiento.Interesados postularse por este medio con CV adjunto.</v>
+      </c>
+      <c r="F75" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-representante-de-ventas-en-hoteles-en-playa-del-carmen-en-solidaridad-9E74627D5CD2A96F61373E686DCF3405#lc=ListOffers-Score0-13</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Representante de ventas en hoteles - En Cancún</v>
+      </c>
+      <c r="B76" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C76" t="str">
+        <v>Benito Juárez, Quintana Roo</v>
+      </c>
+      <c r="D76" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Únete a nuestro equipo como Representante de Ventas en Hoteles en Cancún¡Estamos en expansión y buscamos talento como el tuyo! Si tienes habilidades en ventas, disfrutas el trato con clientes y quieres formar parte de una empresa en crecimiento, esta es tu oportunidad.Tu misión:Brindar un servicio de clase mundial a nuestros clientes y alcanzar altos volúmenes de venta, siempre reflejando nuestros valores y manteniendo una excelente imagen profesional.¿Qué harás?• Ofrecer una cálida bienvenida a los huéspedes en sus primeras 24 horas y establecer un contacto profesional.• Proporcionar información sobre nuestros productos y servicios, así como sobre las opciones disponibles en los hoteles.• Identificar y coordinar soluciones para situaciones que puedan afectar la experiencia del huésped.• Cumplir con las metas de ventas y procedimientos de reservación, cancelación y manejo de dinero.• Participar en viajes de familiarización, entrenamientos y actividades para fortalecer tu conocimiento del destino.• Mantener relaciones positivas con clientes, socios y colegas.• Elaborar reportes claros y precisos sobre las operaciones diarias.¿A quién buscamos?• Personas extrovertidas, con facilidad de palabra y pasión por el servicio al cliente.• Experiencia mínima de 1 año en ventas, servicio al cliente, mercadotecnia o relaciones públicas.• Habilidades en cierre de ventas, comunicación efectiva y uso de tecnología (terminales bancarias, software, smartphones).• Disponibilidad para turnos rotativos semanales según la zona asignada, con descanso entre semana.• Dominio del inglés en un 90%.• Bachillerato concluido o licenciatura.Lo que ofrecemos:Esquema de comisiones atractivo.Prestaciones superiores a la ley.Seguro de vida y gastos médicos mayores.Excelente ambiente de trabajo y oportunidades de crecimiento.Si cumples con el perfil, ¡postúlate enviando tu CV por este medio y forma parte de nuestro equipo!</v>
+      </c>
+      <c r="F76" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-representante-de-ventas-en-hoteles-en-cancun-en-benito-juarez-8B15C400AF70469E61373E686DCF3405#lc=ListOffers-Score0-14</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Representante de ventas en hoteles - En Cozumel</v>
+      </c>
+      <c r="B77" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C77" t="str">
+        <v>Cozumel, Quintana Roo</v>
+      </c>
+      <c r="D77" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E77" t="str">
+        <v>¡Da el siguiente paso en tu carrera! En Amstar estamos en búsqueda de tu talento como REPRESENTANTES DE VENTAS EN HOTELES en la Ciudad de Cozumel.Tu objetivo será:Prestar un excelente servicio de clase mundial a todos nuestros clientes, así como generar altos volúmenes de venta de acuerdo a las metas establecidas, cuidando la imagen y valores empresariales en todo momento.Tus principales funciones serán:• Brindar un servicio de clase mundial (WCCS) a todos nuestros clientes de las diferentes cuentas que sirve la empresa.• Dar una presentación de bienvenida a la llegada de los huéspedes en sus hoteles estableciendo un contacto profesional con todos ellos en las primeras 24 horas de su llegada.• Proporcionar a los huéspedes en los hoteles información sobre los productos y servicios que nuestra empresa ofrece, así como también sobre servicios ofrecidos por los hoteles en donde estemos trabajando, sus políticas y procedimientos.• Reconocer situaciones que estuvieran afectando las vacaciones de los huéspedes, coordinando la implementación de soluciones efectivas con el personal del hotel si es posible o y reportando a la gerencia de la empresa y del hotel.• Lograr los objetivos y metas de ventas establecidas.• Cumplir con los lineamientos establecidos por la empresa sobre la reservación, venta, cancelación, reembolso, reportes de excursiones, y manejo del dinero.• Elaborar reportes exactos y precisos de acuerdo con las políticas y procedimientos establecidos.• Participar a todos los viajes de familiarización, excursiones y hoteles requeridos por la empresa.• Participar a todos los cursos de formación y entrenamiento requeridos.• Establecer y mantener excelentes relaciones con todos nuestros socios, colegas y clientes de acuerdo con las políticas establecidas.• Escribir reportes sobre asuntos que haya o pudieran impactar directa o indirectamente la vacación de los huéspedes en el hotel.Perfil:• Extrovertido, facilidad de palabra y manejo de servicio a clientes, excelente actitud de servicio, conocimiento en tecnología (terminales bancarias, computadora, Software y Smartphone), buena presentación, trabajo en equipo.• Conocimiento del destino, experiencia mínima de 1 año en las áreas de servicio a clientes, ventas, mercadotecnia y/o relaciones públicas, Manejo de solución de situaciones con clientes no satisfechos.• Habilidades: Cierre de ventas, Facilidad de comunicación, Efectividad en relaciones interpersonales, Facilidad de aprendizaje en uso de herramientas tecnológicas (terminales bancarias, computadora, software y Smart phones)• Dominio del idioma inglés 90%.• Preparación académica: Bachillerato o Licenciatura.SUELDO BASADO EN COMISIONESOfrecemos prestaciones superiores a las de Ley, Seguro de Vida, GMM, buen ambiente de trabajo, facilidad de crecimiento.Interesados postularse por este medio con CV adjunto."Cuidamos de las personas para que puedan alcanzar su mejor versión."</v>
+      </c>
+      <c r="F77" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-representante-de-ventas-en-hoteles-en-cozumel-en-cozumel-796CCF50654F84C061373E686DCF3405#lc=ListOffers-Score0-15</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Representante de ventas en hoteles - En Huatulco</v>
+      </c>
+      <c r="B78" t="str">
+        <v>AMSTAR OPERACIONES DMC MX</v>
+      </c>
+      <c r="C78" t="str">
+        <v>Santa Cruz Huatulco, Oaxaca</v>
+      </c>
+      <c r="D78" t="str">
+        <v>$ 16,521</v>
+      </c>
+      <c r="E78" t="str">
+        <v>¡Da el siguiente paso en tu carrera! En Amstar estamos en búsqueda de tu talento como REPRESENTANTES DE VENTAS EN HOTELES en la Ciudad de Huatulco.Tu objetivo será:Prestar un excelente servicio de clase mundial a todos nuestros clientes, así como generar altos volúmenes de venta de acuerdo a las metas establecidas, cuidando la imagen y valores empresariales en todo momento.Tus principales funciones serán:• Brindar un servicio de clase mundial (WCCS) a todos nuestros clientes de las diferentes cuentas que sirve la empresa.• Dar una presentación de bienvenida a la llegada de los huéspedes en sus hoteles estableciendo un contacto profesional con todos ellos en las primeras 24 horas de su llegada.• Proporcionar a los huéspedes en los hoteles información sobre los productos y servicios que nuestra empresa ofrece, así como también sobre servicios ofrecidos por los hoteles en donde estemos trabajando, sus políticas y procedimientos.• Reconocer situaciones que estuvieran afectando las vacaciones de los huéspedes, coordinando la implementación de soluciones efectivas con el personal del hotel si es posible o y reportando a la gerencia de la empresa y del hotel.• Lograr los objetivos y metas de ventas establecidas.• Cumplir con los lineamientos establecidos por la empresa sobre la reservación, venta, cancelación, reembolso, reportes de excursiones, y manejo del dinero.• Elaborar reportes exactos y precisos de acuerdo con las políticas y procedimientos establecidos.• Participar a todos los viajes de familiarización, excursiones y hoteles requeridos por la empresa.• Participar a todos los cursos de formación y entrenamiento requeridos.• Establecer y mantener excelentes relaciones con todos nuestros socios, colegas y clientes de acuerdo con las políticas establecidas.• Escribir reportes sobre asuntos que haya o pudieran impactar directa o indirectamente la vacación de los huéspedes en el hotel.Perfil:• Extrovertido, facilidad de palabra y manejo de servicio a clientes, excelente actitud de servicio, conocimiento en tecnología (terminales bancarias, computadora, Software y Smartphone), buena presentación, trabajo en equipo.• Conocimiento del destino, experiencia mínima de 1 año en las áreas de servicio a clientes, ventas, mercadotecnia y/o relaciones públicas, Manejo de solución de situaciones con clientes no satisfechos.• Habilidades: Cierre de ventas, Facilidad de comunicación, Efectividad en relaciones interpersonales, Facilidad de aprendizaje en uso de herramientas tecnológicas (terminales bancarias, computadora, software y Smart phones)• Dominio del idioma inglés 90%.• Preparación académica: Bachillerato o Licenciatura.SUELDO BASADO EN COMISIONESOfrecemos prestaciones superiores a las de Ley, Seguro de Vida, GMM, buen ambiente de trabajo, facilidad de crecimiento.Interesados postularse por este medio con CV adjunto."Cuidamos de las personas para que puedan alcanzar su mejor versión."</v>
+      </c>
+      <c r="F78" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-representante-de-ventas-en-hoteles-en-huatulco-en-santa-cruz-huatulco-4BC996EBB84FC1DE61373E686DCF3405#lc=ListOffers-Score0-16</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Customer service agent - customer service agent</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Smart Pro Connect</v>
+      </c>
+      <c r="C79" t="str">
+        <v>Cuauhtémoc, Ciudad de México DF</v>
+      </c>
+      <c r="D79" t="str">
+        <v>$ 16,500.00</v>
+      </c>
+      <c r="E79" t="str">
+        <v>Job Overview We are seeking a Customer Service Representative (CSR) / Back Office to join our dynamic team. In this role, you will provide administrative support, manage communications, and ensure an efficient workflow between teams in Mexico and the United States. This position requires a highly organized, detail-oriented individual with near-native English proficiency.</v>
+      </c>
+      <c r="F79" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-customer-service-agent-customer-service-agent-en-cuauhtemoc-2B5413B12E3F606E61373E686DCF3405#lc=ListOffers-Score0-17</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>back office bilingual - back office bilingual</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Smart Pro Connect</v>
+      </c>
+      <c r="C80" t="str">
+        <v>Cuauhtémoc, Ciudad de México DF</v>
+      </c>
+      <c r="D80" t="str">
+        <v>$ 16,500.00</v>
+      </c>
+      <c r="E80" t="str">
+        <v>Job Overview We are seeking a Customer Service Representative (CSR) / Back Office to join our dynamic team. In this role, you will provide administrative support, manage communications, and ensure an efficient workflow between teams in Mexico and the United States. This position requires a highly organized, detail-oriented individual with near-native English proficiency.</v>
+      </c>
+      <c r="F80" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-back-office-bilingual-back-office-bilingual-en-cuauhtemoc-1989D061C8F914FC61373E686DCF3405#lc=ListOffers-Score0-18</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Asistencia Conectividad WiFi - WiFi Concierge</v>
+      </c>
+      <c r="B81" t="str">
+        <v>SINGLE DIGITS MEXICO</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Los Cabos, Baja California Sur</v>
+      </c>
+      <c r="D81" t="str">
+        <v>$ 20,000.00</v>
+      </c>
+      <c r="E81" t="str">
+        <v>NOTA IMPORTANTE: SE CONSIDERARÁN PARA EL PROCESO EXCLUSIVAMENTE AQUELLOS CANDIDATOS RADICANDO EN CABO SAN LUCAS, B.C.SQuiénes somos:Brindamos a los usuarios finales THE CONNECTED LIFE EXPERIENCE: la EXPERIENCIA DE CONECTIVIDAD FLUIDA, SIN ESFUERZO Y ROBUSTA que los clientes esperan, y mostramos a los propietarios cómo ROMPER LOS LÍMITES DE LA CONECTIVIDAD POCO INSPIRADA para aumentar los ingresos, mejorar la satisfacción del cliente/residente y, en última instancia, aumentar el valor de su propiedad.Ofrecemos soluciones completas de Internet y conectividad para huéspedes, residentes y clientes, que incluyen software de clase empresarial, diseño de red, ingeniería, servicios profesionales, mantenimiento continuo, monitoreo de red, soporte multilingüe, informes de ingresos y seguimiento de autenticación.Actividades:Apoyar a los huéspedes del hotel (con sede en los Cabos BC) con sus conexiones cableadas e inalámbricas y el uso de la red SD HSIA.Proporcionar conectividad de red al personal del hotel y soporte de resolución de problemas a pedido.Proporcionar asistencia de configuración y desmontaje con cualquier reunión o conferencia en el lugar.Trabajando con el equipo de soporte de SD, monitoree el rendimiento del sistema y las quejas de los clientes. Interactúe con los huéspedes del hotel y de la conferencia para identificar cualquier necesidad potencial a su llegada. Comunicarse con los invitados, el personal y el equipo de apoyo de SDI con fluidez en español o inglés.Propósito / Resumen del trabajo:El Representante de Servicios al Huésped atiende las necesidades de soporte tecnológico y de sistemas de los huéspedes y el personal del hotel, ayudándolos con la configuración de la conectividad a Internet, así como con la resolución de cualquier desafío relacionado con el funcionamiento o la funcionalidad de la red deAcceso a Internet de Alta Velocidad (HSIA) de un solo dígito (SD).El puesto está ubicado en un sitio específico del hotel, y es de lunes a sábado, de 9:00 a 18:30 hrs.Los solicitantes deben tener la capacidad de leer/escribir/hablar español e inglés.Deberes /Responsabilidades:Apoye a los huéspedes del hotel con sus conexiones cableadas e inalámbricas y el uso de la red SD HSIA Proporcionar conectividad de red al personal del hotel y soporte de resolución de problemas bajo demanda Proporcionar asistencia de configuración y desmontaje con cualquier reunión o conferencia en el lugarTrabajando con el equipo de soporte de SD, monitoree el rendimiento del sistema y las quejas de los clientes Interactúe con los huéspedes del hotel y de la conferencia para identificar cualquier necesidad potencial a su llegada Proporcionar una excelente experiencia al cliente mientras se mantiene un entorno de trabajo seguro Multitarea y prioriza según sea necesario para satisfacer las necesidades del cliente Garantizar que se brinde la más alta calidad de servicio para promover la satisfacción superior del cliente Cumplir con las pautas y requisitos de seguridad de la empresa Comunicarse con los invitados, el personal y elequipo de apoyo de SDI con fluidez en español o inglés Requisitos y calificaciones del trabajoEducación: Diploma técnico o equivalente.Bilingüe 70% Experiencia:Experiencia previa trabajando en la industria hotelera (preferiblemente). Experiencia conectando computadoras, teléfonos, tabletas y dispositivos de juego a redes wifi e internetExperiencia en Servicio al Cliente trabajando con el público.Experiencia en un rol/entorno de soporte de escritorio o red.Recomendable aquellos con experiencia trabajando como técnico/ingenierode campo Conocimiento:Conocimiento de los conceptos de redes de Internet y lasherramientas relacionadas, conocimientos LAN/WAN/WLAN es un plus. Conocimiento de los sistemas operativos y uso básico de Windows / MAC / IOS / Android / Consola de juegosRecomendable conocimiento de los sistemas, equipos, fabricantes y componentes de wifi y redes (ej. cisco)Conocimientos básicos de sistemas de cableado estructurado, deseable compresión de fibra óptica.Microsoft Office, Teams, Zoom, Visio, etc.</v>
+      </c>
+      <c r="F81" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-asistencia-conectividad-wifi-wifi-concierge-en-los-cabos-A5F02E8DB58AE49261373E686DCF3405#lc=ListOffers-Score0-19</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>data entry bilingual agent - data entry bilingual agent</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Smart Pro Connect</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Cuauhtémoc, Ciudad de México DF</v>
+      </c>
+      <c r="D82" t="str">
+        <v>$ 16,500.00</v>
+      </c>
+      <c r="E82" t="str">
+        <v>Job Overview We are seeking a Customer Service Representative (CSR) / Back Office to join our dynamic team. In this role, you will provide administrative support, manage communications, and ensure an efficient workflow between teams in Mexico and the United States. This position requires a highly organized, detail-oriented individual with near-native English proficiency.</v>
+      </c>
+      <c r="F82" t="str">
+        <v>https://mx.computrabajo.com/ofertas-de-trabajo/oferta-de-trabajo-de-data-entry-bilingual-agent-data-entry-bilingual-agent-en-cuauhtemoc-4D2D0B4D51E2D58561373E686DCF3405#lc=ListOffers-Score0-0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F82"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>